<commit_message>
Misc Updates to Reach Ranks and other scripts
-found some misc errors in the Limiting Factor code (one was reading in spring chinook index values for steelhead)
-updated barriers to exclude in Okanogan based on John A.'s input
</commit_message>
<xml_diff>
--- a/Data/Criteria_and_Scoring/Habitat_Limiting_Factor_Rating_Criteria.xlsx
+++ b/Data/Criteria_and_Scoring/Habitat_Limiting_Factor_Rating_Criteria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14A4DE8-C220-4F17-8908-51AAF6FD5E07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03512EB5-79EA-4326-850C-C0195187C929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="492" windowWidth="22188" windowHeight="11508" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
+    <workbookView xWindow="300" yWindow="384" windowWidth="22740" windowHeight="11676" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="209">
   <si>
     <t>Habitat Limiting Factor Scoring Rules</t>
   </si>
@@ -656,6 +656,33 @@
   </si>
   <si>
     <t>Based on Floodplain analysis by Aspect Consulting and UCSRB (Greer)</t>
+  </si>
+  <si>
+    <t>ATLAS_FlowBin</t>
+  </si>
+  <si>
+    <t>ATLAS_Flow</t>
+  </si>
+  <si>
+    <t>ATLAS flow class 3</t>
+  </si>
+  <si>
+    <t>ATLAS flow class 2</t>
+  </si>
+  <si>
+    <t>ATLAS flow class 1</t>
+  </si>
+  <si>
+    <t>no data present</t>
+  </si>
+  <si>
+    <t>Canopy_Cover_NORWEST</t>
+  </si>
+  <si>
+    <t>Riparian- Canopy Cover</t>
+  </si>
+  <si>
+    <t>NorWEST Canopy Cover</t>
   </si>
 </sst>
 </file>
@@ -927,9 +954,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="1" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -940,6 +964,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="4" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3756,12 +3781,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FD6E8C-F414-4D9F-82CB-33D09B6D4DCD}">
-  <dimension ref="A1:O104"/>
+  <dimension ref="A1:O108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="D103" sqref="D103"/>
+      <selection pane="bottomLeft" activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3776,49 +3801,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="38" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3857,7 +3882,7 @@
       <c r="K2" s="2">
         <v>1.4</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="34">
         <v>1</v>
       </c>
       <c r="M2" s="4" t="s">
@@ -3905,7 +3930,7 @@
       <c r="K3" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="34">
         <v>3</v>
       </c>
       <c r="M3" s="4" t="s">
@@ -3953,7 +3978,7 @@
       <c r="K4" s="2">
         <v>100000</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="34">
         <v>5</v>
       </c>
       <c r="M4" s="4" t="s">
@@ -4090,7 +4115,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="2">
-        <f>I7</f>
+        <f t="shared" ref="J7:J14" si="0">I7</f>
         <v>20</v>
       </c>
       <c r="K7" s="2">
@@ -4138,7 +4163,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="2">
-        <f>I8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K8" s="2">
@@ -4186,7 +4211,7 @@
         <v>17</v>
       </c>
       <c r="J9" s="2">
-        <f>I9</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="K9" s="2">
@@ -4234,7 +4259,7 @@
         <v>70</v>
       </c>
       <c r="J10" s="2">
-        <f>I10</f>
+        <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="K10" s="2">
@@ -4282,13 +4307,13 @@
         <v>0</v>
       </c>
       <c r="J11" s="2">
-        <f>I11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K11" s="2">
         <v>2</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="34">
         <v>1</v>
       </c>
       <c r="M11" s="4" t="s">
@@ -4330,13 +4355,13 @@
         <v>2</v>
       </c>
       <c r="J12" s="2">
-        <f>I12</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K12" s="2">
         <v>5</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="34">
         <v>3</v>
       </c>
       <c r="M12" s="4" t="s">
@@ -4378,13 +4403,13 @@
         <v>5</v>
       </c>
       <c r="J13" s="2">
-        <f>I13</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="K13" s="2">
         <v>101</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="34">
         <v>5</v>
       </c>
       <c r="M13" s="4" t="s">
@@ -4426,13 +4451,13 @@
         <v>0</v>
       </c>
       <c r="J14" s="2">
-        <f>I14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K14" s="2">
         <v>1</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="34">
         <v>1</v>
       </c>
       <c r="M14" s="4" t="s">
@@ -4479,7 +4504,7 @@
       <c r="K15" s="2">
         <v>20</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="34">
         <v>3</v>
       </c>
       <c r="M15" s="4" t="s">
@@ -4521,13 +4546,13 @@
         <v>20</v>
       </c>
       <c r="J16" s="2">
-        <f>I16</f>
+        <f t="shared" ref="J16:J55" si="1">I16</f>
         <v>20</v>
       </c>
       <c r="K16" s="2">
         <v>101</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="34">
         <v>5</v>
       </c>
       <c r="M16" s="4" t="s">
@@ -4569,13 +4594,13 @@
         <v>0</v>
       </c>
       <c r="J17" s="2">
-        <f>I17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K17" s="2">
         <v>0.1</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="34">
         <v>1</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -4617,13 +4642,13 @@
         <v>0.1</v>
       </c>
       <c r="J18" s="2">
-        <f>I18</f>
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
       <c r="K18" s="2">
         <v>5</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="34">
         <v>3</v>
       </c>
       <c r="M18" s="2" t="s">
@@ -4665,13 +4690,13 @@
         <v>5</v>
       </c>
       <c r="J19" s="2">
-        <f>I19</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="K19" s="2">
         <v>100000</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19" s="34">
         <v>5</v>
       </c>
       <c r="M19" s="2" t="s">
@@ -4705,13 +4730,13 @@
         <v>0</v>
       </c>
       <c r="J20" s="37">
-        <f>I20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K20" s="37">
         <v>5</v>
       </c>
-      <c r="L20" s="37">
+      <c r="L20" s="46">
         <v>1</v>
       </c>
       <c r="M20" s="37" t="str">
@@ -4746,13 +4771,13 @@
         <v>5</v>
       </c>
       <c r="J21" s="37">
-        <f>I21</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="K21" s="37">
         <v>20</v>
       </c>
-      <c r="L21" s="37">
+      <c r="L21" s="46">
         <v>3</v>
       </c>
       <c r="M21" s="37" t="str">
@@ -4787,13 +4812,13 @@
         <v>20</v>
       </c>
       <c r="J22" s="37">
-        <f>I22</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K22" s="37">
         <v>10000</v>
       </c>
-      <c r="L22" s="37">
+      <c r="L22" s="46">
         <v>5</v>
       </c>
       <c r="M22" s="37" t="str">
@@ -4836,13 +4861,13 @@
         <v>0</v>
       </c>
       <c r="J23" s="2">
-        <f>I23</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K23" s="2">
         <v>10</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L23" s="34">
         <v>1</v>
       </c>
       <c r="M23" s="2" t="s">
@@ -4884,13 +4909,13 @@
         <v>10</v>
       </c>
       <c r="J24" s="2">
-        <f>I24</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="K24" s="2">
         <v>20</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L24" s="34">
         <v>3</v>
       </c>
       <c r="M24" s="2" t="s">
@@ -4932,13 +4957,13 @@
         <v>20</v>
       </c>
       <c r="J25" s="2">
-        <f>I25</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K25" s="2">
         <v>101</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25" s="34">
         <v>5</v>
       </c>
       <c r="M25" s="2" t="s">
@@ -4981,13 +5006,13 @@
         <v>0</v>
       </c>
       <c r="J26" s="2">
-        <f>I26</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K26" s="2">
         <v>184</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L26" s="34">
         <v>1</v>
       </c>
       <c r="M26" s="2" t="s">
@@ -5030,13 +5055,13 @@
         <v>184</v>
       </c>
       <c r="J27" s="2">
-        <f>I27</f>
+        <f t="shared" si="1"/>
         <v>184</v>
       </c>
       <c r="K27" s="2">
         <v>10000</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L27" s="34">
         <v>5</v>
       </c>
       <c r="M27" s="2" t="s">
@@ -5079,13 +5104,13 @@
         <v>32</v>
       </c>
       <c r="J28" s="2" t="str">
-        <f>I28</f>
+        <f t="shared" si="1"/>
         <v>NA</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L28" s="2" t="s">
+      <c r="L28" s="34" t="s">
         <v>32</v>
       </c>
       <c r="M28" s="2" t="s">
@@ -5129,13 +5154,13 @@
         <v>0</v>
       </c>
       <c r="J29" s="2">
-        <f>I29</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K29" s="2">
         <v>95</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L29" s="34">
         <v>1</v>
       </c>
       <c r="M29" s="2" t="s">
@@ -5179,13 +5204,13 @@
         <v>95</v>
       </c>
       <c r="J30" s="2">
-        <f>I30</f>
+        <f t="shared" si="1"/>
         <v>95</v>
       </c>
       <c r="K30" s="2">
         <v>100000</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L30" s="34">
         <v>5</v>
       </c>
       <c r="M30" s="2" t="s">
@@ -5229,11 +5254,11 @@
         <v>32</v>
       </c>
       <c r="J31" s="2" t="str">
-        <f>I31</f>
+        <f t="shared" si="1"/>
         <v>NA</v>
       </c>
       <c r="K31" s="2"/>
-      <c r="L31" s="2" t="s">
+      <c r="L31" s="34" t="s">
         <v>32</v>
       </c>
       <c r="M31" s="2" t="s">
@@ -5277,13 +5302,13 @@
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <f>I32</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K32" s="2">
         <v>70</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L32" s="34">
         <v>1</v>
       </c>
       <c r="M32" s="2" t="s">
@@ -5327,13 +5352,13 @@
         <v>70</v>
       </c>
       <c r="J33" s="2">
-        <f>I33</f>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="K33" s="2">
         <v>100000</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L33" s="34">
         <v>5</v>
       </c>
       <c r="M33" s="2" t="s">
@@ -5377,13 +5402,13 @@
         <v>32</v>
       </c>
       <c r="J34" s="2" t="str">
-        <f>I34</f>
+        <f t="shared" si="1"/>
         <v>NA</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L34" s="2" t="s">
+      <c r="L34" s="34" t="s">
         <v>32</v>
       </c>
       <c r="M34" s="2" t="s">
@@ -5427,13 +5452,13 @@
         <v>0</v>
       </c>
       <c r="J35" s="2">
-        <f>I35</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K35" s="2">
         <v>55</v>
       </c>
-      <c r="L35" s="2">
+      <c r="L35" s="34">
         <v>1</v>
       </c>
       <c r="M35" s="2" t="s">
@@ -5477,13 +5502,13 @@
         <v>55</v>
       </c>
       <c r="J36" s="2">
-        <f>I36</f>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="K36" s="2">
         <v>10000</v>
       </c>
-      <c r="L36" s="2">
+      <c r="L36" s="34">
         <v>5</v>
       </c>
       <c r="M36" s="2" t="s">
@@ -5527,13 +5552,13 @@
         <v>32</v>
       </c>
       <c r="J37" s="2" t="str">
-        <f>I37</f>
+        <f t="shared" si="1"/>
         <v>NA</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L37" s="2" t="s">
+      <c r="L37" s="34" t="s">
         <v>32</v>
       </c>
       <c r="M37" s="2" t="s">
@@ -5577,13 +5602,13 @@
         <v>0</v>
       </c>
       <c r="J38" s="2">
-        <f>I38</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K38" s="2">
         <v>47</v>
       </c>
-      <c r="L38" s="2">
+      <c r="L38" s="34">
         <v>1</v>
       </c>
       <c r="M38" s="2" t="s">
@@ -5627,13 +5652,13 @@
         <v>47</v>
       </c>
       <c r="J39" s="2">
-        <f>I39</f>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="K39" s="2">
         <v>10000</v>
       </c>
-      <c r="L39" s="2">
+      <c r="L39" s="34">
         <v>5</v>
       </c>
       <c r="M39" s="2" t="s">
@@ -5677,13 +5702,13 @@
         <v>32</v>
       </c>
       <c r="J40" s="2" t="str">
-        <f>I40</f>
+        <f t="shared" si="1"/>
         <v>NA</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L40" s="2" t="s">
+      <c r="L40" s="34" t="s">
         <v>32</v>
       </c>
       <c r="M40" s="2" t="s">
@@ -5727,13 +5752,13 @@
         <v>0</v>
       </c>
       <c r="J41" s="2">
-        <f>I41</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K41" s="2">
         <v>25</v>
       </c>
-      <c r="L41" s="2">
+      <c r="L41" s="34">
         <v>1</v>
       </c>
       <c r="M41" s="2" t="s">
@@ -5777,13 +5802,13 @@
         <v>25</v>
       </c>
       <c r="J42" s="2">
-        <f>I42</f>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="K42" s="2">
         <v>100000</v>
       </c>
-      <c r="L42" s="2">
+      <c r="L42" s="34">
         <v>5</v>
       </c>
       <c r="M42" s="2" t="s">
@@ -5827,13 +5852,13 @@
         <v>32</v>
       </c>
       <c r="J43" s="2" t="str">
-        <f>I43</f>
+        <f t="shared" si="1"/>
         <v>NA</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L43" s="2" t="s">
+      <c r="L43" s="34" t="s">
         <v>32</v>
       </c>
       <c r="M43" s="2" t="s">
@@ -5877,13 +5902,13 @@
         <v>0</v>
       </c>
       <c r="J44" s="2">
-        <f>I44</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K44" s="2">
         <v>23</v>
       </c>
-      <c r="L44" s="2">
+      <c r="L44" s="34">
         <v>1</v>
       </c>
       <c r="M44" s="2" t="s">
@@ -5927,13 +5952,13 @@
         <v>23</v>
       </c>
       <c r="J45" s="2">
-        <f>I45</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="K45" s="2">
         <v>100000</v>
       </c>
-      <c r="L45" s="2">
+      <c r="L45" s="34">
         <v>5</v>
       </c>
       <c r="M45" s="2" t="s">
@@ -5977,13 +6002,13 @@
         <v>32</v>
       </c>
       <c r="J46" s="2" t="str">
-        <f>I46</f>
+        <f t="shared" si="1"/>
         <v>NA</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L46" s="2" t="s">
+      <c r="L46" s="34" t="s">
         <v>32</v>
       </c>
       <c r="M46" s="2" t="s">
@@ -6026,13 +6051,13 @@
         <v>0</v>
       </c>
       <c r="J47" s="2">
-        <f>I47</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K47" s="2">
         <v>18</v>
       </c>
-      <c r="L47" s="2">
+      <c r="L47" s="34">
         <v>1</v>
       </c>
       <c r="M47" s="2" t="s">
@@ -6075,13 +6100,13 @@
         <v>18</v>
       </c>
       <c r="J48" s="2">
-        <f>I48</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="K48" s="2">
         <v>100000</v>
       </c>
-      <c r="L48" s="2">
+      <c r="L48" s="34">
         <v>5</v>
       </c>
       <c r="M48" s="2" t="s">
@@ -6124,13 +6149,13 @@
         <v>32</v>
       </c>
       <c r="J49" s="2" t="str">
-        <f>I49</f>
+        <f t="shared" si="1"/>
         <v>NA</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L49" s="2" t="s">
+      <c r="L49" s="34" t="s">
         <v>32</v>
       </c>
       <c r="M49" s="2" t="s">
@@ -6143,120 +6168,130 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B50" s="36" t="s">
+    <row r="50" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="B50" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="E50" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="H50" s="36" t="s">
+      <c r="C50" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="D50" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="E50" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H50" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I50" s="37">
+      <c r="I50" s="41">
         <v>0</v>
       </c>
-      <c r="J50" s="37">
-        <f>I50</f>
+      <c r="J50" s="41">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K50" s="37">
+      <c r="K50" s="41">
         <f>50</f>
         <v>50</v>
       </c>
-      <c r="L50" s="37">
+      <c r="L50" s="42">
         <v>1</v>
       </c>
-      <c r="M50" s="38" t="s">
+      <c r="M50" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="N50" s="37" t="s">
+      <c r="N50" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="O50" s="36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A51" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B51" s="36" t="s">
+      <c r="O50" s="40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="B51" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36" t="s">
+      <c r="C51" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="D51" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="E51" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H51" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I51" s="37">
+      <c r="I51" s="41">
         <v>50</v>
       </c>
-      <c r="J51" s="37">
-        <f>I51</f>
+      <c r="J51" s="41">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="K51" s="37">
+      <c r="K51" s="41">
         <v>80</v>
       </c>
-      <c r="L51" s="37">
+      <c r="L51" s="42">
         <v>3</v>
       </c>
-      <c r="M51" s="38" t="s">
+      <c r="M51" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="N51" s="37" t="s">
+      <c r="N51" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="O51" s="36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A52" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="B52" s="36" t="s">
+      <c r="O51" s="40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="B52" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36" t="s">
+      <c r="C52" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="D52" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="E52" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H52" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I52" s="37">
+      <c r="I52" s="41">
         <v>80</v>
       </c>
-      <c r="J52" s="37">
-        <f>I52</f>
+      <c r="J52" s="41">
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="K52" s="37">
+      <c r="K52" s="41">
         <v>101</v>
       </c>
-      <c r="L52" s="37">
+      <c r="L52" s="42">
         <v>5</v>
       </c>
-      <c r="M52" s="38" t="s">
+      <c r="M52" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="N52" s="37" t="s">
+      <c r="N52" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="O52" s="36" t="s">
+      <c r="O52" s="40" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6289,13 +6324,13 @@
         <v>0</v>
       </c>
       <c r="J53" s="2">
-        <f>I53</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K53" s="2">
         <v>2</v>
       </c>
-      <c r="L53" s="2">
+      <c r="L53" s="34">
         <v>1</v>
       </c>
       <c r="M53" s="4" t="s">
@@ -6337,13 +6372,13 @@
         <v>2</v>
       </c>
       <c r="J54" s="2">
-        <f>I54</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="K54" s="2">
         <v>5</v>
       </c>
-      <c r="L54" s="2">
+      <c r="L54" s="34">
         <v>3</v>
       </c>
       <c r="M54" s="4" t="s">
@@ -6385,13 +6420,13 @@
         <v>5</v>
       </c>
       <c r="J55" s="2">
-        <f>I55</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="K55" s="2">
         <v>101</v>
       </c>
-      <c r="L55" s="2">
+      <c r="L55" s="34">
         <v>5</v>
       </c>
       <c r="M55" s="4" t="s">
@@ -6438,7 +6473,7 @@
       <c r="K56" s="2">
         <v>1</v>
       </c>
-      <c r="L56" s="2">
+      <c r="L56" s="34">
         <v>1</v>
       </c>
       <c r="M56" s="4" t="s">
@@ -6485,7 +6520,7 @@
       <c r="K57" s="2">
         <v>4</v>
       </c>
-      <c r="L57" s="2">
+      <c r="L57" s="34">
         <v>3</v>
       </c>
       <c r="M57" s="4" t="s">
@@ -6532,7 +6567,7 @@
       <c r="K58" s="2">
         <v>5.0999999999999996</v>
       </c>
-      <c r="L58" s="2">
+      <c r="L58" s="34">
         <v>5</v>
       </c>
       <c r="M58" s="4" t="s">
@@ -6574,7 +6609,7 @@
         <v>0</v>
       </c>
       <c r="J59" s="2">
-        <f>I59</f>
+        <f t="shared" ref="J59:J82" si="2">I59</f>
         <v>0</v>
       </c>
       <c r="K59" s="2">
@@ -6622,7 +6657,7 @@
         <v>2</v>
       </c>
       <c r="J60" s="2">
-        <f>I60</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K60" s="2">
@@ -6670,7 +6705,7 @@
         <v>5</v>
       </c>
       <c r="J61" s="2">
-        <f>I61</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="K61" s="2">
@@ -6718,7 +6753,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="2">
-        <f>I62</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K62" s="2">
@@ -6766,7 +6801,7 @@
         <v>1</v>
       </c>
       <c r="J63" s="2">
-        <f>I63</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K63" s="2">
@@ -6814,7 +6849,7 @@
         <v>50</v>
       </c>
       <c r="J64" s="2">
-        <f>I64</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="K64" s="2">
@@ -6862,7 +6897,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="2">
-        <f>I65</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K65" s="2">
@@ -6910,7 +6945,7 @@
         <v>12</v>
       </c>
       <c r="J66" s="2">
-        <f>I66</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="K66" s="2">
@@ -6958,7 +6993,7 @@
         <v>20</v>
       </c>
       <c r="J67" s="2">
-        <f>I67</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="K67" s="2">
@@ -6978,880 +7013,880 @@
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A68" s="41" t="s">
+      <c r="A68" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B68" s="41" t="s">
+      <c r="B68" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="C68" s="42" t="s">
+      <c r="C68" s="41" t="s">
         <v>146</v>
       </c>
-      <c r="D68" s="41" t="s">
+      <c r="D68" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="E68" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F68" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G68" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H68" s="41" t="s">
+      <c r="E68" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F68" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G68" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H68" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I68" s="42">
+      <c r="I68" s="41">
         <v>0</v>
       </c>
-      <c r="J68" s="42">
-        <f>I68</f>
+      <c r="J68" s="41">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K68" s="42">
+      <c r="K68" s="41">
         <v>10</v>
       </c>
-      <c r="L68" s="43">
+      <c r="L68" s="42">
         <v>1</v>
       </c>
-      <c r="M68" s="42" t="s">
+      <c r="M68" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="N68" s="42" t="s">
+      <c r="N68" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="O68" s="41" t="s">
+      <c r="O68" s="40" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A69" s="41" t="s">
+      <c r="A69" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B69" s="41" t="s">
+      <c r="B69" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="C69" s="42" t="s">
+      <c r="C69" s="41" t="s">
         <v>146</v>
       </c>
-      <c r="D69" s="41" t="s">
+      <c r="D69" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="E69" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F69" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G69" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H69" s="41" t="s">
+      <c r="E69" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F69" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G69" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H69" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I69" s="42">
+      <c r="I69" s="41">
         <v>10</v>
       </c>
-      <c r="J69" s="42">
-        <f>I69</f>
+      <c r="J69" s="41">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="K69" s="42">
+      <c r="K69" s="41">
         <v>20</v>
       </c>
-      <c r="L69" s="43">
+      <c r="L69" s="42">
         <v>3</v>
       </c>
-      <c r="M69" s="42" t="s">
+      <c r="M69" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="N69" s="42" t="s">
+      <c r="N69" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="O69" s="41" t="s">
+      <c r="O69" s="40" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A70" s="41" t="s">
+      <c r="A70" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="41" t="s">
+      <c r="B70" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="C70" s="42" t="s">
+      <c r="C70" s="41" t="s">
         <v>146</v>
       </c>
-      <c r="D70" s="41" t="s">
+      <c r="D70" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="E70" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F70" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G70" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H70" s="41" t="s">
+      <c r="E70" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F70" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G70" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H70" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I70" s="42">
+      <c r="I70" s="41">
         <v>20</v>
       </c>
-      <c r="J70" s="42">
-        <f>I70</f>
+      <c r="J70" s="41">
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="K70" s="42">
+      <c r="K70" s="41">
         <v>100000</v>
       </c>
-      <c r="L70" s="43">
+      <c r="L70" s="42">
         <v>5</v>
       </c>
-      <c r="M70" s="42" t="s">
+      <c r="M70" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="N70" s="42" t="s">
+      <c r="N70" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="O70" s="41" t="s">
+      <c r="O70" s="40" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A71" s="41" t="s">
+      <c r="A71" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B71" s="41" t="s">
+      <c r="B71" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="C71" s="41" t="s">
+      <c r="C71" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D71" s="41" t="s">
+      <c r="D71" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="E71" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F71" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G71" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H71" s="41" t="s">
+      <c r="E71" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F71" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G71" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H71" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I71" s="42">
+      <c r="I71" s="41">
         <v>0</v>
       </c>
-      <c r="J71" s="42">
-        <f>I71</f>
+      <c r="J71" s="41">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K71" s="42">
+      <c r="K71" s="41">
         <v>15</v>
       </c>
-      <c r="L71" s="43">
+      <c r="L71" s="42">
         <v>5</v>
       </c>
-      <c r="M71" s="44" t="s">
+      <c r="M71" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="N71" s="42" t="s">
+      <c r="N71" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="O71" s="41" t="s">
+      <c r="O71" s="40" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A72" s="41" t="s">
+      <c r="A72" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B72" s="41" t="s">
+      <c r="B72" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="C72" s="41" t="s">
+      <c r="C72" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D72" s="41" t="s">
+      <c r="D72" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="E72" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F72" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G72" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H72" s="41" t="s">
+      <c r="E72" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F72" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G72" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H72" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I72" s="42">
+      <c r="I72" s="41">
         <v>15</v>
       </c>
-      <c r="J72" s="42">
-        <f>I72</f>
+      <c r="J72" s="41">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="K72" s="42">
+      <c r="K72" s="41">
         <v>30</v>
       </c>
-      <c r="L72" s="43">
+      <c r="L72" s="42">
         <v>3</v>
       </c>
-      <c r="M72" s="44" t="s">
+      <c r="M72" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="N72" s="42" t="s">
+      <c r="N72" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="O72" s="41" t="s">
+      <c r="O72" s="40" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A73" s="41" t="s">
+      <c r="A73" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B73" s="41" t="s">
+      <c r="B73" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="C73" s="41" t="s">
+      <c r="C73" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D73" s="41" t="s">
+      <c r="D73" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="E73" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F73" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G73" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H73" s="41" t="s">
+      <c r="E73" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F73" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G73" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H73" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I73" s="42">
+      <c r="I73" s="41">
         <v>30</v>
       </c>
-      <c r="J73" s="42">
-        <f>I73</f>
+      <c r="J73" s="41">
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="K73" s="42">
+      <c r="K73" s="41">
         <v>101</v>
       </c>
-      <c r="L73" s="43">
+      <c r="L73" s="42">
         <v>1</v>
       </c>
-      <c r="M73" s="44" t="s">
+      <c r="M73" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="N73" s="42" t="s">
+      <c r="N73" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="O73" s="41" t="s">
+      <c r="O73" s="40" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A74" s="41" t="s">
+      <c r="A74" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B74" s="41" t="s">
+      <c r="B74" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C74" s="41" t="s">
+      <c r="C74" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="D74" s="41" t="s">
+      <c r="D74" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="E74" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F74" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G74" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H74" s="41" t="s">
+      <c r="E74" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F74" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G74" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H74" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I74" s="42">
+      <c r="I74" s="41">
         <v>0</v>
       </c>
-      <c r="J74" s="42">
-        <f>I74</f>
+      <c r="J74" s="41">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K74" s="42">
+      <c r="K74" s="41">
         <v>12</v>
       </c>
       <c r="L74" s="42">
         <v>5</v>
       </c>
-      <c r="M74" s="42" t="str">
+      <c r="M74" s="41" t="str">
         <f>"&lt;" &amp;I75 &amp;" deg"</f>
         <v>&lt;12 deg</v>
       </c>
-      <c r="N74" s="42" t="s">
+      <c r="N74" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="O74" s="45" t="s">
+      <c r="O74" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A75" s="41" t="s">
+      <c r="A75" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B75" s="41" t="s">
+      <c r="B75" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C75" s="41" t="s">
+      <c r="C75" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="D75" s="41" t="s">
+      <c r="D75" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="E75" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F75" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G75" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H75" s="41" t="s">
+      <c r="E75" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F75" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G75" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H75" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I75" s="42">
+      <c r="I75" s="41">
         <v>12</v>
       </c>
-      <c r="J75" s="42">
-        <f>I75</f>
+      <c r="J75" s="41">
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="K75" s="42">
+      <c r="K75" s="41">
         <v>14</v>
       </c>
       <c r="L75" s="42">
         <v>3</v>
       </c>
-      <c r="M75" s="42" t="str">
+      <c r="M75" s="41" t="str">
         <f>I75&amp;"-"&amp;I76&amp;" deg"</f>
         <v>12-14 deg</v>
       </c>
-      <c r="N75" s="42" t="s">
+      <c r="N75" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="O75" s="45" t="s">
+      <c r="O75" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A76" s="41" t="s">
+      <c r="A76" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B76" s="41" t="s">
+      <c r="B76" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C76" s="41" t="s">
+      <c r="C76" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="D76" s="41" t="s">
+      <c r="D76" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="E76" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F76" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G76" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H76" s="41" t="s">
+      <c r="E76" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F76" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H76" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I76" s="42">
+      <c r="I76" s="41">
         <v>14</v>
       </c>
-      <c r="J76" s="42">
-        <f>I76</f>
+      <c r="J76" s="41">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="K76" s="42">
+      <c r="K76" s="41">
         <v>1000</v>
       </c>
       <c r="L76" s="42">
         <v>1</v>
       </c>
-      <c r="M76" s="42" t="str">
+      <c r="M76" s="41" t="str">
         <f>"&gt;" &amp;I76 &amp;" deg"</f>
         <v>&gt;14 deg</v>
       </c>
-      <c r="N76" s="42" t="s">
+      <c r="N76" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="O76" s="45" t="s">
+      <c r="O76" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A77" s="41" t="s">
+      <c r="A77" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B77" s="41" t="s">
+      <c r="B77" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C77" s="41" t="s">
+      <c r="C77" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="D77" s="41" t="s">
+      <c r="D77" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="E77" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F77" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G77" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H77" s="41" t="s">
+      <c r="E77" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F77" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G77" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H77" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I77" s="42">
+      <c r="I77" s="41">
         <v>0</v>
       </c>
-      <c r="J77" s="42">
-        <f>I77</f>
+      <c r="J77" s="41">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K77" s="42">
+      <c r="K77" s="41">
         <v>10</v>
       </c>
       <c r="L77" s="42">
         <v>5</v>
       </c>
-      <c r="M77" s="42" t="s">
+      <c r="M77" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="N77" s="42" t="s">
+      <c r="N77" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="O77" s="45" t="s">
+      <c r="O77" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A78" s="41" t="s">
+      <c r="A78" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B78" s="41" t="s">
+      <c r="B78" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C78" s="41" t="s">
+      <c r="C78" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="D78" s="41" t="s">
+      <c r="D78" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="E78" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F78" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G78" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H78" s="41" t="s">
+      <c r="E78" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F78" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G78" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H78" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I78" s="42">
+      <c r="I78" s="41">
         <v>10</v>
       </c>
-      <c r="J78" s="42">
-        <f>I78</f>
+      <c r="J78" s="41">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="K78" s="42">
+      <c r="K78" s="41">
         <v>14</v>
       </c>
       <c r="L78" s="42">
         <v>3</v>
       </c>
-      <c r="M78" s="42" t="s">
+      <c r="M78" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="N78" s="42" t="s">
+      <c r="N78" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="O78" s="45" t="s">
+      <c r="O78" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A79" s="41" t="s">
+      <c r="A79" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="41" t="s">
+      <c r="B79" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C79" s="41" t="s">
+      <c r="C79" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="D79" s="41" t="s">
+      <c r="D79" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="E79" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F79" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G79" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H79" s="41" t="s">
+      <c r="E79" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F79" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G79" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H79" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I79" s="42">
+      <c r="I79" s="41">
         <v>14</v>
       </c>
-      <c r="J79" s="42">
-        <f>I79</f>
+      <c r="J79" s="41">
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="K79" s="42">
+      <c r="K79" s="41">
         <v>1000</v>
       </c>
       <c r="L79" s="42">
         <v>1</v>
       </c>
-      <c r="M79" s="42" t="s">
+      <c r="M79" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="N79" s="42" t="s">
+      <c r="N79" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="O79" s="45" t="s">
+      <c r="O79" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A80" s="41" t="s">
+      <c r="A80" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="B80" s="41" t="s">
+      <c r="B80" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C80" s="41" t="s">
+      <c r="C80" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="D80" s="41" t="s">
+      <c r="D80" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="E80" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F80" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G80" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H80" s="41" t="s">
+      <c r="E80" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F80" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H80" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I80" s="42">
+      <c r="I80" s="41">
         <v>0</v>
       </c>
-      <c r="J80" s="42">
-        <f>I80</f>
+      <c r="J80" s="41">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K80" s="42">
+      <c r="K80" s="41">
         <v>16</v>
       </c>
       <c r="L80" s="42">
         <v>5</v>
       </c>
-      <c r="M80" s="42" t="s">
+      <c r="M80" s="41" t="s">
         <v>185</v>
       </c>
-      <c r="N80" s="42" t="s">
+      <c r="N80" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="O80" s="45" t="s">
+      <c r="O80" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A81" s="41" t="s">
+      <c r="A81" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="B81" s="41" t="s">
+      <c r="B81" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C81" s="41" t="s">
+      <c r="C81" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="D81" s="41" t="s">
+      <c r="D81" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="E81" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F81" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G81" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H81" s="41" t="s">
+      <c r="E81" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F81" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G81" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H81" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I81" s="42">
+      <c r="I81" s="41">
         <v>16</v>
       </c>
-      <c r="J81" s="42">
-        <f>I81</f>
+      <c r="J81" s="41">
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="K81" s="42">
+      <c r="K81" s="41">
         <v>22</v>
       </c>
       <c r="L81" s="42">
         <v>3</v>
       </c>
-      <c r="M81" s="42" t="s">
+      <c r="M81" s="41" t="s">
         <v>186</v>
       </c>
-      <c r="N81" s="42" t="s">
+      <c r="N81" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="O81" s="45" t="s">
+      <c r="O81" s="44" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A82" s="41" t="s">
+      <c r="A82" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="B82" s="41" t="s">
+      <c r="B82" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="C82" s="41" t="s">
+      <c r="C82" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="D82" s="41" t="s">
+      <c r="D82" s="40" t="s">
         <v>170</v>
       </c>
-      <c r="E82" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F82" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G82" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H82" s="41" t="s">
+      <c r="E82" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F82" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G82" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H82" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I82" s="42">
+      <c r="I82" s="41">
         <v>22</v>
       </c>
-      <c r="J82" s="42">
-        <f>I82</f>
+      <c r="J82" s="41">
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="K82" s="42">
+      <c r="K82" s="41">
         <v>1000</v>
       </c>
       <c r="L82" s="42">
         <v>1</v>
       </c>
-      <c r="M82" s="42" t="s">
+      <c r="M82" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="N82" s="42" t="s">
+      <c r="N82" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="O82" s="45" t="s">
+      <c r="O82" s="44" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="41" t="s">
+    <row r="83" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="B83" s="41" t="s">
+      <c r="B83" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="C83" s="41" t="s">
+      <c r="C83" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D83" s="41" t="s">
+      <c r="D83" s="40" t="s">
         <v>192</v>
       </c>
-      <c r="E83" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F83" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G83" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H83" s="41" t="s">
+      <c r="E83" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F83" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G83" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H83" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I83" s="42">
+      <c r="I83" s="41">
         <v>99</v>
       </c>
-      <c r="J83" s="41">
+      <c r="J83" s="40">
         <v>99</v>
       </c>
-      <c r="K83" s="42">
+      <c r="K83" s="41">
         <v>100</v>
       </c>
-      <c r="L83" s="46">
+      <c r="L83" s="45">
         <v>1</v>
       </c>
-      <c r="M83" s="42" t="s">
+      <c r="M83" s="41" t="s">
         <v>194</v>
       </c>
-      <c r="N83" s="42" t="s">
+      <c r="N83" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="O83" s="41" t="s">
+      <c r="O83" s="40" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="84" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="41" t="s">
+    <row r="84" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="B84" s="41" t="s">
+      <c r="B84" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="C84" s="41" t="s">
+      <c r="C84" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D84" s="41" t="s">
+      <c r="D84" s="40" t="s">
         <v>192</v>
       </c>
-      <c r="E84" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F84" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G84" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H84" s="41" t="s">
+      <c r="E84" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F84" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G84" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H84" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I84" s="42">
+      <c r="I84" s="41">
         <v>50</v>
       </c>
       <c r="J84">
         <v>50</v>
       </c>
-      <c r="K84" s="42">
+      <c r="K84" s="41">
         <v>99</v>
       </c>
       <c r="L84" s="35">
         <v>3</v>
       </c>
-      <c r="M84" s="42" t="s">
+      <c r="M84" s="41" t="s">
         <v>195</v>
       </c>
-      <c r="N84" s="42" t="s">
+      <c r="N84" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="O84" s="41" t="s">
+      <c r="O84" s="40" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="85" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="41" t="s">
+    <row r="85" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="B85" s="41" t="s">
+      <c r="B85" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="C85" s="41" t="s">
+      <c r="C85" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D85" s="41" t="s">
+      <c r="D85" s="40" t="s">
         <v>192</v>
       </c>
-      <c r="E85" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="F85" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G85" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H85" s="41" t="s">
+      <c r="E85" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F85" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="G85" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H85" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="I85" s="42">
+      <c r="I85" s="41">
         <v>0</v>
       </c>
       <c r="J85">
         <v>0</v>
       </c>
-      <c r="K85" s="42">
+      <c r="K85" s="41">
         <v>50</v>
       </c>
       <c r="L85" s="35">
         <v>5</v>
       </c>
-      <c r="M85" s="42" t="s">
+      <c r="M85" s="41" t="s">
         <v>196</v>
       </c>
-      <c r="N85" s="42" t="s">
+      <c r="N85" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="O85" s="41" t="s">
+      <c r="O85" s="40" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="86" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="41" t="s">
+    <row r="86" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B86" s="41" t="s">
+      <c r="B86" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="D86" s="41" t="s">
+      <c r="D86" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="E86" s="41" t="s">
+      <c r="E86" s="40" t="s">
         <v>32</v>
       </c>
       <c r="F86" t="s">
@@ -7863,39 +7898,39 @@
       <c r="H86" t="s">
         <v>179</v>
       </c>
-      <c r="I86" s="42" t="s">
+      <c r="I86" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="J86" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="K86" s="42" t="s">
+      <c r="J86" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="K86" s="41" t="s">
         <v>32</v>
       </c>
       <c r="L86" s="42">
         <v>1</v>
       </c>
-      <c r="M86" s="42" t="s">
+      <c r="M86" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="N86" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="O86" s="41" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="41" t="s">
+      <c r="N86" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="O86" s="40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B87" s="41" t="s">
+      <c r="B87" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="D87" s="41" t="s">
+      <c r="D87" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="E87" s="41" t="s">
+      <c r="E87" s="40" t="s">
         <v>32</v>
       </c>
       <c r="F87" t="s">
@@ -7907,39 +7942,39 @@
       <c r="H87" t="s">
         <v>179</v>
       </c>
-      <c r="I87" s="42" t="s">
+      <c r="I87" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="J87" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="K87" s="42" t="s">
+      <c r="J87" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="K87" s="41" t="s">
         <v>32</v>
       </c>
       <c r="L87" s="42">
         <v>3</v>
       </c>
-      <c r="M87" s="42" t="s">
+      <c r="M87" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="N87" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="O87" s="41" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="88" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="41" t="s">
+      <c r="N87" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="O87" s="40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B88" s="41" t="s">
+      <c r="B88" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="D88" s="41" t="s">
+      <c r="D88" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="E88" s="41" t="s">
+      <c r="E88" s="40" t="s">
         <v>32</v>
       </c>
       <c r="F88" t="s">
@@ -7951,29 +7986,29 @@
       <c r="H88" t="s">
         <v>179</v>
       </c>
-      <c r="I88" s="42" t="s">
+      <c r="I88" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="J88" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="K88" s="42" t="s">
+      <c r="J88" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="K88" s="41" t="s">
         <v>32</v>
       </c>
       <c r="L88" s="42">
         <v>5</v>
       </c>
-      <c r="M88" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="N88" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="O88" s="41" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M88" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="N88" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="O88" s="40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -8001,13 +8036,13 @@
       <c r="I89" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J89" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="K89" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="L89" s="2" t="s">
+      <c r="J89" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="K89" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="L89" s="34" t="s">
         <v>32</v>
       </c>
       <c r="M89" s="2" t="s">
@@ -8020,7 +8055,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>36</v>
       </c>
@@ -8048,13 +8083,13 @@
       <c r="I90" s="3">
         <v>1</v>
       </c>
-      <c r="J90" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="K90" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="L90" s="2">
+      <c r="J90" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="K90" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="L90" s="34">
         <v>5</v>
       </c>
       <c r="M90" s="2" t="s">
@@ -8067,7 +8102,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>36</v>
       </c>
@@ -8095,13 +8130,13 @@
       <c r="I91" s="3">
         <v>2</v>
       </c>
-      <c r="J91" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="K91" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="L91" s="2">
+      <c r="J91" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="K91" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="L91" s="34">
         <v>3</v>
       </c>
       <c r="M91" s="2" t="s">
@@ -8114,7 +8149,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>36</v>
       </c>
@@ -8142,13 +8177,13 @@
       <c r="I92" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="J92" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="K92" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="L92" s="2">
+      <c r="J92" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="K92" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="L92" s="34">
         <v>1</v>
       </c>
       <c r="M92" s="2" t="s">
@@ -8161,7 +8196,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="93" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>36</v>
       </c>
@@ -8189,13 +8224,13 @@
       <c r="I93" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="J93" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="K93" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="L93" s="2">
+      <c r="J93" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="K93" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="L93" s="34">
         <v>1</v>
       </c>
       <c r="M93" s="2" t="s">
@@ -8208,7 +8243,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>36</v>
       </c>
@@ -8236,13 +8271,13 @@
       <c r="I94" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="J94" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="K94" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="L94" s="2">
+      <c r="J94" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="K94" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="L94" s="34">
         <v>1</v>
       </c>
       <c r="M94" s="2" t="s">
@@ -8255,7 +8290,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>36</v>
       </c>
@@ -8283,13 +8318,13 @@
       <c r="I95" s="3">
         <v>5</v>
       </c>
-      <c r="J95" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="K95" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="L95" s="2">
+      <c r="J95" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="K95" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="L95" s="34">
         <v>1</v>
       </c>
       <c r="M95" s="2" t="s">
@@ -8302,7 +8337,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -8349,7 +8384,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -8396,7 +8431,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -8518,10 +8553,10 @@
       <c r="I100" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J100" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="K100" s="42" t="s">
+      <c r="J100" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="K100" s="41" t="s">
         <v>32</v>
       </c>
       <c r="L100" s="35">
@@ -8723,6 +8758,194 @@
       </c>
       <c r="O104" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>200</v>
+      </c>
+      <c r="B105" t="s">
+        <v>136</v>
+      </c>
+      <c r="C105" t="s">
+        <v>144</v>
+      </c>
+      <c r="D105" t="s">
+        <v>201</v>
+      </c>
+      <c r="E105" t="s">
+        <v>32</v>
+      </c>
+      <c r="F105" t="s">
+        <v>32</v>
+      </c>
+      <c r="G105" t="s">
+        <v>32</v>
+      </c>
+      <c r="H105" t="s">
+        <v>179</v>
+      </c>
+      <c r="I105" s="2">
+        <v>3</v>
+      </c>
+      <c r="J105" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L105" s="34">
+        <v>5</v>
+      </c>
+      <c r="M105" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="N105" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O105" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>200</v>
+      </c>
+      <c r="B106" t="s">
+        <v>136</v>
+      </c>
+      <c r="C106" t="s">
+        <v>144</v>
+      </c>
+      <c r="D106" t="s">
+        <v>201</v>
+      </c>
+      <c r="E106" t="s">
+        <v>32</v>
+      </c>
+      <c r="F106" t="s">
+        <v>32</v>
+      </c>
+      <c r="G106" t="s">
+        <v>32</v>
+      </c>
+      <c r="H106" t="s">
+        <v>179</v>
+      </c>
+      <c r="I106" s="2">
+        <v>2</v>
+      </c>
+      <c r="J106" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K106" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L106" s="34">
+        <v>3</v>
+      </c>
+      <c r="M106" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="N106" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O106" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>200</v>
+      </c>
+      <c r="B107" t="s">
+        <v>136</v>
+      </c>
+      <c r="C107" t="s">
+        <v>144</v>
+      </c>
+      <c r="D107" t="s">
+        <v>201</v>
+      </c>
+      <c r="E107" t="s">
+        <v>32</v>
+      </c>
+      <c r="F107" t="s">
+        <v>32</v>
+      </c>
+      <c r="G107" t="s">
+        <v>32</v>
+      </c>
+      <c r="H107" t="s">
+        <v>179</v>
+      </c>
+      <c r="I107" s="2">
+        <v>1</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K107" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L107" s="34">
+        <v>1</v>
+      </c>
+      <c r="M107" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="N107" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O107" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>200</v>
+      </c>
+      <c r="B108" t="s">
+        <v>136</v>
+      </c>
+      <c r="C108" t="s">
+        <v>144</v>
+      </c>
+      <c r="D108" t="s">
+        <v>201</v>
+      </c>
+      <c r="E108" t="s">
+        <v>32</v>
+      </c>
+      <c r="F108" t="s">
+        <v>32</v>
+      </c>
+      <c r="G108" t="s">
+        <v>32</v>
+      </c>
+      <c r="H108" t="s">
+        <v>179</v>
+      </c>
+      <c r="I108" s="2">
+        <v>0</v>
+      </c>
+      <c r="J108" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K108" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L108" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="M108" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="N108" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O108" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -8752,8 +8975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D3CB046-13DE-47BF-9FEF-248A4A26DE1B}">
   <dimension ref="A1:AA88"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updates to Ranks, Update LF pathway, etc.
</commit_message>
<xml_diff>
--- a/Data/Criteria_and_Scoring/Habitat_Limiting_Factor_Rating_Criteria.xlsx
+++ b/Data/Criteria_and_Scoring/Habitat_Limiting_Factor_Rating_Criteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03512EB5-79EA-4326-850C-C0195187C929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439D82FA-020C-4330-88D5-B5FBA7F89504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="384" windowWidth="22740" windowHeight="11676" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17520" windowHeight="11184" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -505,9 +505,6 @@
     <t>Coarse Substrate</t>
   </si>
   <si>
-    <t>GravelCobble_UCSRB_pct</t>
-  </si>
-  <si>
     <t>Cover- Boulders</t>
   </si>
   <si>
@@ -683,6 +680,9 @@
   </si>
   <si>
     <t>NorWEST Canopy Cover</t>
+  </si>
+  <si>
+    <t>GravelCobble_UCSRB_pct,GRVL_COBL_UCSRB_CHAMP</t>
   </si>
 </sst>
 </file>
@@ -3783,10 +3783,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FD6E8C-F414-4D9F-82CB-33D09B6D4DCD}">
   <dimension ref="A1:O108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H99" sqref="H99"/>
+      <selection pane="bottomLeft" activeCell="J74" sqref="J74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3817,22 +3817,22 @@
         <v>126</v>
       </c>
       <c r="F1" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="G1" s="38" t="s">
-        <v>184</v>
-      </c>
       <c r="H1" s="38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I1" s="38" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="K1" s="38" t="s">
         <v>181</v>
-      </c>
-      <c r="K1" s="38" t="s">
-        <v>182</v>
       </c>
       <c r="L1" s="39" t="s">
         <v>10</v>
@@ -3855,11 +3855,11 @@
         <v>139</v>
       </c>
       <c r="C2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" t="s">
         <v>159</v>
       </c>
-      <c r="D2" t="s">
-        <v>160</v>
-      </c>
       <c r="E2" t="s">
         <v>32</v>
       </c>
@@ -3870,7 +3870,7 @@
         <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I2" s="2">
         <v>0</v>
@@ -3903,11 +3903,11 @@
         <v>139</v>
       </c>
       <c r="C3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" t="s">
         <v>159</v>
       </c>
-      <c r="D3" t="s">
-        <v>160</v>
-      </c>
       <c r="E3" t="s">
         <v>32</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I3" s="2">
         <v>1.4</v>
@@ -3951,11 +3951,11 @@
         <v>139</v>
       </c>
       <c r="C4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" t="s">
         <v>159</v>
       </c>
-      <c r="D4" t="s">
-        <v>160</v>
-      </c>
       <c r="E4" t="s">
         <v>32</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I4" s="2">
         <v>2.2000000000000002</v>
@@ -3999,10 +3999,10 @@
         <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E5" t="s">
         <v>127</v>
@@ -4014,7 +4014,7 @@
         <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -4047,10 +4047,10 @@
         <v>125</v>
       </c>
       <c r="C6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E6" t="s">
         <v>127</v>
@@ -4062,7 +4062,7 @@
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -4094,10 +4094,10 @@
         <v>125</v>
       </c>
       <c r="C7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E7" t="s">
         <v>127</v>
@@ -4109,7 +4109,7 @@
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I7" s="2">
         <v>20</v>
@@ -4142,10 +4142,10 @@
         <v>125</v>
       </c>
       <c r="C8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E8" t="s">
         <v>128</v>
@@ -4157,7 +4157,7 @@
         <v>100000</v>
       </c>
       <c r="H8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -4190,10 +4190,10 @@
         <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E9" t="s">
         <v>128</v>
@@ -4205,7 +4205,7 @@
         <v>100000</v>
       </c>
       <c r="H9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I9" s="2">
         <v>17</v>
@@ -4238,10 +4238,10 @@
         <v>125</v>
       </c>
       <c r="C10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E10" t="s">
         <v>128</v>
@@ -4253,7 +4253,7 @@
         <v>100000</v>
       </c>
       <c r="H10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I10" s="2">
         <v>70</v>
@@ -4286,11 +4286,11 @@
         <v>137</v>
       </c>
       <c r="C11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" t="s">
         <v>153</v>
       </c>
-      <c r="D11" t="s">
-        <v>154</v>
-      </c>
       <c r="E11" t="s">
         <v>32</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>32</v>
       </c>
       <c r="H11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -4334,11 +4334,11 @@
         <v>137</v>
       </c>
       <c r="C12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" t="s">
         <v>153</v>
       </c>
-      <c r="D12" t="s">
-        <v>154</v>
-      </c>
       <c r="E12" t="s">
         <v>32</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I12" s="2">
         <v>2</v>
@@ -4382,11 +4382,11 @@
         <v>137</v>
       </c>
       <c r="C13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" t="s">
         <v>153</v>
       </c>
-      <c r="D13" t="s">
-        <v>154</v>
-      </c>
       <c r="E13" t="s">
         <v>32</v>
       </c>
@@ -4397,7 +4397,7 @@
         <v>32</v>
       </c>
       <c r="H13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I13" s="2">
         <v>5</v>
@@ -4430,11 +4430,11 @@
         <v>140</v>
       </c>
       <c r="C14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" t="s">
         <v>166</v>
       </c>
-      <c r="D14" t="s">
-        <v>167</v>
-      </c>
       <c r="E14" t="s">
         <v>32</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>32</v>
       </c>
       <c r="H14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -4478,11 +4478,11 @@
         <v>140</v>
       </c>
       <c r="C15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D15" t="s">
         <v>166</v>
       </c>
-      <c r="D15" t="s">
-        <v>167</v>
-      </c>
       <c r="E15" t="s">
         <v>32</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>32</v>
       </c>
       <c r="H15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I15" s="2">
         <v>0.1</v>
@@ -4525,11 +4525,11 @@
         <v>140</v>
       </c>
       <c r="C16" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16" t="s">
         <v>166</v>
       </c>
-      <c r="D16" t="s">
-        <v>167</v>
-      </c>
       <c r="E16" t="s">
         <v>32</v>
       </c>
@@ -4540,7 +4540,7 @@
         <v>32</v>
       </c>
       <c r="H16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I16" s="2">
         <v>20</v>
@@ -4573,10 +4573,10 @@
         <v>140</v>
       </c>
       <c r="C17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E17" t="s">
         <v>32</v>
@@ -4588,7 +4588,7 @@
         <v>32</v>
       </c>
       <c r="H17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I17" s="2">
         <v>0</v>
@@ -4621,10 +4621,10 @@
         <v>140</v>
       </c>
       <c r="C18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -4636,7 +4636,7 @@
         <v>32</v>
       </c>
       <c r="H18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I18" s="2">
         <v>0.1</v>
@@ -4669,10 +4669,10 @@
         <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E19" t="s">
         <v>32</v>
@@ -4684,7 +4684,7 @@
         <v>32</v>
       </c>
       <c r="H19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I19" s="2">
         <v>5</v>
@@ -4724,7 +4724,7 @@
       <c r="F20" s="36"/>
       <c r="G20" s="36"/>
       <c r="H20" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I20" s="37">
         <v>0</v>
@@ -4765,7 +4765,7 @@
       <c r="F21" s="36"/>
       <c r="G21" s="36"/>
       <c r="H21" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I21" s="37">
         <v>5</v>
@@ -4806,7 +4806,7 @@
       <c r="F22" s="36"/>
       <c r="G22" s="36"/>
       <c r="H22" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I22" s="37">
         <v>20</v>
@@ -4840,11 +4840,11 @@
         <v>140</v>
       </c>
       <c r="C23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D23" t="s">
         <v>163</v>
       </c>
-      <c r="D23" t="s">
-        <v>164</v>
-      </c>
       <c r="E23" t="s">
         <v>32</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>32</v>
       </c>
       <c r="H23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I23" s="2">
         <v>0</v>
@@ -4888,11 +4888,11 @@
         <v>140</v>
       </c>
       <c r="C24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D24" t="s">
         <v>163</v>
       </c>
-      <c r="D24" t="s">
-        <v>164</v>
-      </c>
       <c r="E24" t="s">
         <v>32</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>32</v>
       </c>
       <c r="H24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I24" s="2">
         <v>10</v>
@@ -4936,11 +4936,11 @@
         <v>140</v>
       </c>
       <c r="C25" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" t="s">
         <v>163</v>
       </c>
-      <c r="D25" t="s">
-        <v>164</v>
-      </c>
       <c r="E25" t="s">
         <v>32</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>32</v>
       </c>
       <c r="H25" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I25" s="2">
         <v>20</v>
@@ -4984,10 +4984,10 @@
         <v>140</v>
       </c>
       <c r="C26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E26" t="s">
         <v>86</v>
@@ -5000,7 +5000,7 @@
         <v>1.524</v>
       </c>
       <c r="H26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I26" s="2">
         <v>0</v>
@@ -5033,10 +5033,10 @@
         <v>140</v>
       </c>
       <c r="C27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E27" t="s">
         <v>86</v>
@@ -5049,7 +5049,7 @@
         <v>1.524</v>
       </c>
       <c r="H27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I27" s="2">
         <v>184</v>
@@ -5082,10 +5082,10 @@
         <v>140</v>
       </c>
       <c r="C28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E28" t="s">
         <v>86</v>
@@ -5098,7 +5098,7 @@
         <v>1.524</v>
       </c>
       <c r="H28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>32</v>
@@ -5131,10 +5131,10 @@
         <v>140</v>
       </c>
       <c r="C29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E29" t="s">
         <v>93</v>
@@ -5148,7 +5148,7 @@
         <v>3.048</v>
       </c>
       <c r="H29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I29" s="2">
         <v>0</v>
@@ -5181,10 +5181,10 @@
         <v>140</v>
       </c>
       <c r="C30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E30" t="s">
         <v>93</v>
@@ -5198,7 +5198,7 @@
         <v>3.048</v>
       </c>
       <c r="H30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I30" s="2">
         <v>95</v>
@@ -5231,10 +5231,10 @@
         <v>140</v>
       </c>
       <c r="C31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E31" t="s">
         <v>93</v>
@@ -5248,7 +5248,7 @@
         <v>3.048</v>
       </c>
       <c r="H31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>32</v>
@@ -5279,10 +5279,10 @@
         <v>140</v>
       </c>
       <c r="C32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E32" t="s">
         <v>98</v>
@@ -5296,7 +5296,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I32" s="2">
         <v>0</v>
@@ -5329,10 +5329,10 @@
         <v>140</v>
       </c>
       <c r="C33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E33" t="s">
         <v>98</v>
@@ -5346,7 +5346,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H33" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I33" s="2">
         <v>70</v>
@@ -5379,10 +5379,10 @@
         <v>140</v>
       </c>
       <c r="C34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E34" t="s">
         <v>98</v>
@@ -5396,7 +5396,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>32</v>
@@ -5429,10 +5429,10 @@
         <v>140</v>
       </c>
       <c r="C35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E35" t="s">
         <v>102</v>
@@ -5446,7 +5446,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
@@ -5479,10 +5479,10 @@
         <v>140</v>
       </c>
       <c r="C36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E36" t="s">
         <v>102</v>
@@ -5496,7 +5496,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I36" s="2">
         <v>55</v>
@@ -5529,10 +5529,10 @@
         <v>140</v>
       </c>
       <c r="C37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E37" t="s">
         <v>102</v>
@@ -5546,7 +5546,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>32</v>
@@ -5579,10 +5579,10 @@
         <v>140</v>
       </c>
       <c r="C38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E38" t="s">
         <v>107</v>
@@ -5596,7 +5596,7 @@
         <v>7.62</v>
       </c>
       <c r="H38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I38" s="2">
         <v>0</v>
@@ -5629,10 +5629,10 @@
         <v>140</v>
       </c>
       <c r="C39" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E39" t="s">
         <v>107</v>
@@ -5646,7 +5646,7 @@
         <v>7.62</v>
       </c>
       <c r="H39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I39" s="2">
         <v>47</v>
@@ -5679,10 +5679,10 @@
         <v>140</v>
       </c>
       <c r="C40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E40" t="s">
         <v>107</v>
@@ -5696,7 +5696,7 @@
         <v>7.62</v>
       </c>
       <c r="H40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>32</v>
@@ -5729,10 +5729,10 @@
         <v>140</v>
       </c>
       <c r="C41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E41" t="s">
         <v>113</v>
@@ -5746,7 +5746,7 @@
         <v>15.24</v>
       </c>
       <c r="H41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I41" s="2">
         <v>0</v>
@@ -5779,10 +5779,10 @@
         <v>140</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E42" t="s">
         <v>113</v>
@@ -5796,7 +5796,7 @@
         <v>15.24</v>
       </c>
       <c r="H42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I42" s="2">
         <v>25</v>
@@ -5829,10 +5829,10 @@
         <v>140</v>
       </c>
       <c r="C43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E43" t="s">
         <v>113</v>
@@ -5846,7 +5846,7 @@
         <v>15.24</v>
       </c>
       <c r="H43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>32</v>
@@ -5879,10 +5879,10 @@
         <v>140</v>
       </c>
       <c r="C44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D44" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E44" t="s">
         <v>116</v>
@@ -5896,7 +5896,7 @@
         <v>22.86</v>
       </c>
       <c r="H44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I44" s="2">
         <v>0</v>
@@ -5929,10 +5929,10 @@
         <v>140</v>
       </c>
       <c r="C45" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D45" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E45" t="s">
         <v>116</v>
@@ -5946,7 +5946,7 @@
         <v>22.86</v>
       </c>
       <c r="H45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I45" s="2">
         <v>23</v>
@@ -5979,10 +5979,10 @@
         <v>140</v>
       </c>
       <c r="C46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E46" t="s">
         <v>116</v>
@@ -5996,7 +5996,7 @@
         <v>22.86</v>
       </c>
       <c r="H46" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>32</v>
@@ -6029,10 +6029,10 @@
         <v>140</v>
       </c>
       <c r="C47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D47" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E47" t="s">
         <v>119</v>
@@ -6045,7 +6045,7 @@
         <v>100000</v>
       </c>
       <c r="H47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I47" s="2">
         <v>0</v>
@@ -6078,10 +6078,10 @@
         <v>140</v>
       </c>
       <c r="C48" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D48" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E48" t="s">
         <v>119</v>
@@ -6094,7 +6094,7 @@
         <v>100000</v>
       </c>
       <c r="H48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I48" s="2">
         <v>18</v>
@@ -6127,10 +6127,10 @@
         <v>140</v>
       </c>
       <c r="C49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E49" t="s">
         <v>119</v>
@@ -6143,7 +6143,7 @@
         <v>100000</v>
       </c>
       <c r="H49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>32</v>
@@ -6170,22 +6170,22 @@
     </row>
     <row r="50" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B50" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E50" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H50" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I50" s="41">
         <v>0</v>
@@ -6213,22 +6213,22 @@
     </row>
     <row r="51" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B51" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D51" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E51" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H51" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I51" s="41">
         <v>50</v>
@@ -6255,22 +6255,22 @@
     </row>
     <row r="52" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B52" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E52" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H52" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I52" s="41">
         <v>80</v>
@@ -6303,11 +6303,11 @@
         <v>138</v>
       </c>
       <c r="C53" t="s">
+        <v>160</v>
+      </c>
+      <c r="D53" t="s">
         <v>161</v>
       </c>
-      <c r="D53" t="s">
-        <v>162</v>
-      </c>
       <c r="E53" t="s">
         <v>32</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>32</v>
       </c>
       <c r="H53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I53" s="2">
         <v>0</v>
@@ -6351,11 +6351,11 @@
         <v>138</v>
       </c>
       <c r="C54" t="s">
+        <v>160</v>
+      </c>
+      <c r="D54" t="s">
         <v>161</v>
       </c>
-      <c r="D54" t="s">
-        <v>162</v>
-      </c>
       <c r="E54" t="s">
         <v>32</v>
       </c>
@@ -6366,7 +6366,7 @@
         <v>32</v>
       </c>
       <c r="H54" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I54" s="2">
         <v>2</v>
@@ -6399,11 +6399,11 @@
         <v>138</v>
       </c>
       <c r="C55" t="s">
+        <v>160</v>
+      </c>
+      <c r="D55" t="s">
         <v>161</v>
       </c>
-      <c r="D55" t="s">
-        <v>162</v>
-      </c>
       <c r="E55" t="s">
         <v>32</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>32</v>
       </c>
       <c r="H55" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I55" s="2">
         <v>5</v>
@@ -6447,11 +6447,11 @@
         <v>136</v>
       </c>
       <c r="C56" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" t="s">
         <v>157</v>
       </c>
-      <c r="D56" t="s">
-        <v>158</v>
-      </c>
       <c r="E56" t="s">
         <v>32</v>
       </c>
@@ -6462,7 +6462,7 @@
         <v>32</v>
       </c>
       <c r="H56" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I56" s="2">
         <v>-5</v>
@@ -6494,11 +6494,11 @@
         <v>136</v>
       </c>
       <c r="C57" t="s">
+        <v>156</v>
+      </c>
+      <c r="D57" t="s">
         <v>157</v>
       </c>
-      <c r="D57" t="s">
-        <v>158</v>
-      </c>
       <c r="E57" t="s">
         <v>32</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>32</v>
       </c>
       <c r="H57" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I57" s="2">
         <v>1</v>
@@ -6541,11 +6541,11 @@
         <v>136</v>
       </c>
       <c r="C58" t="s">
+        <v>156</v>
+      </c>
+      <c r="D58" t="s">
         <v>157</v>
       </c>
-      <c r="D58" t="s">
-        <v>158</v>
-      </c>
       <c r="E58" t="s">
         <v>32</v>
       </c>
@@ -6556,7 +6556,7 @@
         <v>32</v>
       </c>
       <c r="H58" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I58" s="2">
         <v>4</v>
@@ -6588,11 +6588,11 @@
         <v>124</v>
       </c>
       <c r="C59" t="s">
+        <v>149</v>
+      </c>
+      <c r="D59" t="s">
         <v>150</v>
       </c>
-      <c r="D59" t="s">
-        <v>151</v>
-      </c>
       <c r="E59" t="s">
         <v>32</v>
       </c>
@@ -6603,14 +6603,13 @@
         <v>32</v>
       </c>
       <c r="H59" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I59" s="2">
         <v>0</v>
       </c>
       <c r="J59" s="2">
-        <f t="shared" ref="J59:J82" si="2">I59</f>
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="K59" s="2">
         <v>2</v>
@@ -6619,7 +6618,7 @@
         <v>1</v>
       </c>
       <c r="M59" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>18</v>
@@ -6636,11 +6635,11 @@
         <v>124</v>
       </c>
       <c r="C60" t="s">
+        <v>149</v>
+      </c>
+      <c r="D60" t="s">
         <v>150</v>
       </c>
-      <c r="D60" t="s">
-        <v>151</v>
-      </c>
       <c r="E60" t="s">
         <v>32</v>
       </c>
@@ -6651,13 +6650,13 @@
         <v>32</v>
       </c>
       <c r="H60" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I60" s="2">
         <v>2</v>
       </c>
       <c r="J60" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J59:J82" si="2">I60</f>
         <v>2</v>
       </c>
       <c r="K60" s="2">
@@ -6684,11 +6683,11 @@
         <v>124</v>
       </c>
       <c r="C61" t="s">
+        <v>149</v>
+      </c>
+      <c r="D61" t="s">
         <v>150</v>
       </c>
-      <c r="D61" t="s">
-        <v>151</v>
-      </c>
       <c r="E61" t="s">
         <v>32</v>
       </c>
@@ -6699,7 +6698,7 @@
         <v>32</v>
       </c>
       <c r="H61" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I61" s="2">
         <v>5</v>
@@ -6735,7 +6734,7 @@
         <v>148</v>
       </c>
       <c r="D62" t="s">
-        <v>149</v>
+        <v>208</v>
       </c>
       <c r="E62" t="s">
         <v>32</v>
@@ -6747,17 +6746,16 @@
         <v>32</v>
       </c>
       <c r="H62" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I62" s="2">
         <v>0</v>
       </c>
       <c r="J62" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="K62" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="L62" s="34">
         <v>1</v>
@@ -6783,7 +6781,7 @@
         <v>148</v>
       </c>
       <c r="D63" t="s">
-        <v>149</v>
+        <v>208</v>
       </c>
       <c r="E63" t="s">
         <v>32</v>
@@ -6795,14 +6793,13 @@
         <v>32</v>
       </c>
       <c r="H63" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I63" s="2">
         <v>1</v>
       </c>
       <c r="J63" s="2">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="K63" s="2">
         <v>50</v>
@@ -6831,7 +6828,7 @@
         <v>148</v>
       </c>
       <c r="D64" t="s">
-        <v>149</v>
+        <v>208</v>
       </c>
       <c r="E64" t="s">
         <v>32</v>
@@ -6843,7 +6840,7 @@
         <v>32</v>
       </c>
       <c r="H64" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I64" s="2">
         <v>50</v>
@@ -6879,7 +6876,7 @@
         <v>146</v>
       </c>
       <c r="D65" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E65" t="s">
         <v>32</v>
@@ -6891,14 +6888,13 @@
         <v>32</v>
       </c>
       <c r="H65" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I65" s="2">
         <v>0</v>
       </c>
       <c r="J65" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="K65" s="2">
         <v>12</v>
@@ -6927,7 +6923,7 @@
         <v>146</v>
       </c>
       <c r="D66" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E66" t="s">
         <v>32</v>
@@ -6939,7 +6935,7 @@
         <v>32</v>
       </c>
       <c r="H66" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I66" s="2">
         <v>12</v>
@@ -6975,7 +6971,7 @@
         <v>146</v>
       </c>
       <c r="D67" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E67" t="s">
         <v>32</v>
@@ -6987,7 +6983,7 @@
         <v>32</v>
       </c>
       <c r="H67" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I67" s="2">
         <v>20</v>
@@ -7035,14 +7031,13 @@
         <v>32</v>
       </c>
       <c r="H68" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I68" s="41">
         <v>0</v>
       </c>
       <c r="J68" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="K68" s="41">
         <v>10</v>
@@ -7083,7 +7078,7 @@
         <v>32</v>
       </c>
       <c r="H69" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I69" s="41">
         <v>10</v>
@@ -7131,7 +7126,7 @@
         <v>32</v>
       </c>
       <c r="H70" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I70" s="41">
         <v>20</v>
@@ -7167,7 +7162,7 @@
         <v>148</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E71" s="40" t="s">
         <v>32</v>
@@ -7179,14 +7174,13 @@
         <v>32</v>
       </c>
       <c r="H71" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I71" s="41">
         <v>0</v>
       </c>
       <c r="J71" s="41">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="K71" s="41">
         <v>15</v>
@@ -7215,7 +7209,7 @@
         <v>148</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E72" s="40" t="s">
         <v>32</v>
@@ -7227,7 +7221,7 @@
         <v>32</v>
       </c>
       <c r="H72" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I72" s="41">
         <v>15</v>
@@ -7263,7 +7257,7 @@
         <v>148</v>
       </c>
       <c r="D73" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E73" s="40" t="s">
         <v>32</v>
@@ -7275,7 +7269,7 @@
         <v>32</v>
       </c>
       <c r="H73" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I73" s="41">
         <v>30</v>
@@ -7308,11 +7302,11 @@
         <v>141</v>
       </c>
       <c r="C74" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="D74" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="D74" s="40" t="s">
-        <v>170</v>
-      </c>
       <c r="E74" s="40" t="s">
         <v>32</v>
       </c>
@@ -7323,7 +7317,7 @@
         <v>32</v>
       </c>
       <c r="H74" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I74" s="41">
         <v>0</v>
@@ -7357,11 +7351,11 @@
         <v>141</v>
       </c>
       <c r="C75" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="D75" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="D75" s="40" t="s">
-        <v>170</v>
-      </c>
       <c r="E75" s="40" t="s">
         <v>32</v>
       </c>
@@ -7372,7 +7366,7 @@
         <v>32</v>
       </c>
       <c r="H75" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I75" s="41">
         <v>12</v>
@@ -7406,11 +7400,11 @@
         <v>141</v>
       </c>
       <c r="C76" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="D76" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="D76" s="40" t="s">
-        <v>170</v>
-      </c>
       <c r="E76" s="40" t="s">
         <v>32</v>
       </c>
@@ -7421,7 +7415,7 @@
         <v>32</v>
       </c>
       <c r="H76" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I76" s="41">
         <v>14</v>
@@ -7455,10 +7449,10 @@
         <v>141</v>
       </c>
       <c r="C77" s="40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D77" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E77" s="40" t="s">
         <v>32</v>
@@ -7470,7 +7464,7 @@
         <v>32</v>
       </c>
       <c r="H77" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I77" s="41">
         <v>0</v>
@@ -7503,10 +7497,10 @@
         <v>141</v>
       </c>
       <c r="C78" s="40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D78" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E78" s="40" t="s">
         <v>32</v>
@@ -7518,7 +7512,7 @@
         <v>32</v>
       </c>
       <c r="H78" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I78" s="41">
         <v>10</v>
@@ -7551,10 +7545,10 @@
         <v>141</v>
       </c>
       <c r="C79" s="40" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D79" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E79" s="40" t="s">
         <v>32</v>
@@ -7566,7 +7560,7 @@
         <v>32</v>
       </c>
       <c r="H79" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I79" s="41">
         <v>14</v>
@@ -7599,10 +7593,10 @@
         <v>141</v>
       </c>
       <c r="C80" s="40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D80" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E80" s="40" t="s">
         <v>32</v>
@@ -7614,7 +7608,7 @@
         <v>32</v>
       </c>
       <c r="H80" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I80" s="41">
         <v>0</v>
@@ -7630,7 +7624,7 @@
         <v>5</v>
       </c>
       <c r="M80" s="41" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N80" s="41" t="s">
         <v>20</v>
@@ -7647,10 +7641,10 @@
         <v>141</v>
       </c>
       <c r="C81" s="40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D81" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E81" s="40" t="s">
         <v>32</v>
@@ -7662,7 +7656,7 @@
         <v>32</v>
       </c>
       <c r="H81" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I81" s="41">
         <v>16</v>
@@ -7678,7 +7672,7 @@
         <v>3</v>
       </c>
       <c r="M81" s="41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N81" s="41" t="s">
         <v>22</v>
@@ -7695,10 +7689,10 @@
         <v>141</v>
       </c>
       <c r="C82" s="40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D82" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E82" s="40" t="s">
         <v>32</v>
@@ -7710,7 +7704,7 @@
         <v>32</v>
       </c>
       <c r="H82" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I82" s="41">
         <v>22</v>
@@ -7726,7 +7720,7 @@
         <v>1</v>
       </c>
       <c r="M82" s="41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N82" s="41" t="s">
         <v>18</v>
@@ -7737,7 +7731,7 @@
     </row>
     <row r="83" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B83" s="40" t="s">
         <v>124</v>
@@ -7746,7 +7740,7 @@
         <v>148</v>
       </c>
       <c r="D83" s="40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E83" s="40" t="s">
         <v>32</v>
@@ -7758,7 +7752,7 @@
         <v>32</v>
       </c>
       <c r="H83" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I83" s="41">
         <v>99</v>
@@ -7773,18 +7767,18 @@
         <v>1</v>
       </c>
       <c r="M83" s="41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N83" s="41" t="s">
         <v>18</v>
       </c>
       <c r="O83" s="40" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="84" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B84" s="40" t="s">
         <v>124</v>
@@ -7793,7 +7787,7 @@
         <v>148</v>
       </c>
       <c r="D84" s="40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E84" s="40" t="s">
         <v>32</v>
@@ -7805,7 +7799,7 @@
         <v>32</v>
       </c>
       <c r="H84" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I84" s="41">
         <v>50</v>
@@ -7820,18 +7814,18 @@
         <v>3</v>
       </c>
       <c r="M84" s="41" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N84" s="41" t="s">
         <v>22</v>
       </c>
       <c r="O84" s="40" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="85" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B85" s="40" t="s">
         <v>124</v>
@@ -7840,7 +7834,7 @@
         <v>148</v>
       </c>
       <c r="D85" s="40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E85" s="40" t="s">
         <v>32</v>
@@ -7852,7 +7846,7 @@
         <v>32</v>
       </c>
       <c r="H85" s="40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I85" s="41">
         <v>0</v>
@@ -7867,13 +7861,13 @@
         <v>5</v>
       </c>
       <c r="M85" s="41" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N85" s="41" t="s">
         <v>20</v>
       </c>
       <c r="O85" s="40" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="86" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
@@ -7884,7 +7878,7 @@
         <v>142</v>
       </c>
       <c r="D86" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E86" s="40" t="s">
         <v>32</v>
@@ -7896,7 +7890,7 @@
         <v>32</v>
       </c>
       <c r="H86" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I86" s="41" t="s">
         <v>24</v>
@@ -7911,7 +7905,7 @@
         <v>1</v>
       </c>
       <c r="M86" s="41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N86" s="41" t="s">
         <v>32</v>
@@ -7928,7 +7922,7 @@
         <v>142</v>
       </c>
       <c r="D87" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E87" s="40" t="s">
         <v>32</v>
@@ -7940,7 +7934,7 @@
         <v>32</v>
       </c>
       <c r="H87" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I87" s="41" t="s">
         <v>28</v>
@@ -7955,7 +7949,7 @@
         <v>3</v>
       </c>
       <c r="M87" s="41" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N87" s="41" t="s">
         <v>32</v>
@@ -7972,7 +7966,7 @@
         <v>142</v>
       </c>
       <c r="D88" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E88" s="40" t="s">
         <v>32</v>
@@ -7984,7 +7978,7 @@
         <v>32</v>
       </c>
       <c r="H88" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I88" s="41" t="s">
         <v>31</v>
@@ -8016,10 +8010,10 @@
         <v>142</v>
       </c>
       <c r="C89" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D89" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E89" t="s">
         <v>32</v>
@@ -8031,7 +8025,7 @@
         <v>32</v>
       </c>
       <c r="H89" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I89" s="3" t="s">
         <v>32</v>
@@ -8063,10 +8057,10 @@
         <v>142</v>
       </c>
       <c r="C90" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D90" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E90" t="s">
         <v>32</v>
@@ -8078,7 +8072,7 @@
         <v>32</v>
       </c>
       <c r="H90" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I90" s="3">
         <v>1</v>
@@ -8110,10 +8104,10 @@
         <v>142</v>
       </c>
       <c r="C91" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D91" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E91" t="s">
         <v>32</v>
@@ -8125,7 +8119,7 @@
         <v>32</v>
       </c>
       <c r="H91" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I91" s="3">
         <v>2</v>
@@ -8157,10 +8151,10 @@
         <v>142</v>
       </c>
       <c r="C92" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E92" t="s">
         <v>32</v>
@@ -8172,7 +8166,7 @@
         <v>32</v>
       </c>
       <c r="H92" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I92" s="3" t="s">
         <v>51</v>
@@ -8204,10 +8198,10 @@
         <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D93" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E93" t="s">
         <v>32</v>
@@ -8219,7 +8213,7 @@
         <v>32</v>
       </c>
       <c r="H93" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I93" s="3" t="s">
         <v>56</v>
@@ -8251,10 +8245,10 @@
         <v>142</v>
       </c>
       <c r="C94" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D94" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E94" t="s">
         <v>32</v>
@@ -8266,7 +8260,7 @@
         <v>32</v>
       </c>
       <c r="H94" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I94" s="3" t="s">
         <v>59</v>
@@ -8298,10 +8292,10 @@
         <v>142</v>
       </c>
       <c r="C95" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D95" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E95" t="s">
         <v>32</v>
@@ -8313,7 +8307,7 @@
         <v>32</v>
       </c>
       <c r="H95" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I95" s="3">
         <v>5</v>
@@ -8348,7 +8342,7 @@
         <v>144</v>
       </c>
       <c r="D96" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E96" t="s">
         <v>32</v>
@@ -8360,7 +8354,7 @@
         <v>32</v>
       </c>
       <c r="H96" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>20</v>
@@ -8395,7 +8389,7 @@
         <v>144</v>
       </c>
       <c r="D97" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E97" t="s">
         <v>32</v>
@@ -8407,7 +8401,7 @@
         <v>32</v>
       </c>
       <c r="H97" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>22</v>
@@ -8442,7 +8436,7 @@
         <v>144</v>
       </c>
       <c r="D98" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E98" t="s">
         <v>32</v>
@@ -8454,7 +8448,7 @@
         <v>32</v>
       </c>
       <c r="H98" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>18</v>
@@ -8489,7 +8483,7 @@
         <v>144</v>
       </c>
       <c r="D99" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E99" t="s">
         <v>32</v>
@@ -8501,7 +8495,7 @@
         <v>32</v>
       </c>
       <c r="H99" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>32</v>
@@ -8527,16 +8521,16 @@
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B100" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C100" t="s">
         <v>144</v>
       </c>
       <c r="D100" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E100" t="s">
         <v>32</v>
@@ -8548,7 +8542,7 @@
         <v>32</v>
       </c>
       <c r="H100" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I100" s="3" t="s">
         <v>32</v>
@@ -8583,7 +8577,7 @@
         <v>144</v>
       </c>
       <c r="D101" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E101" t="s">
         <v>32</v>
@@ -8595,7 +8589,7 @@
         <v>32</v>
       </c>
       <c r="H101" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I101">
         <v>1</v>
@@ -8616,7 +8610,7 @@
         <v>32</v>
       </c>
       <c r="O101" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.3">
@@ -8630,7 +8624,7 @@
         <v>144</v>
       </c>
       <c r="D102" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E102" t="s">
         <v>32</v>
@@ -8642,7 +8636,7 @@
         <v>32</v>
       </c>
       <c r="H102" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I102">
         <v>3</v>
@@ -8663,7 +8657,7 @@
         <v>32</v>
       </c>
       <c r="O102" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.3">
@@ -8677,7 +8671,7 @@
         <v>144</v>
       </c>
       <c r="D103" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E103" t="s">
         <v>32</v>
@@ -8689,7 +8683,7 @@
         <v>32</v>
       </c>
       <c r="H103" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I103">
         <v>5</v>
@@ -8710,7 +8704,7 @@
         <v>32</v>
       </c>
       <c r="O103" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.3">
@@ -8724,45 +8718,45 @@
         <v>144</v>
       </c>
       <c r="D104" t="s">
+        <v>197</v>
+      </c>
+      <c r="E104" t="s">
+        <v>32</v>
+      </c>
+      <c r="F104" t="s">
+        <v>32</v>
+      </c>
+      <c r="G104" t="s">
+        <v>32</v>
+      </c>
+      <c r="H104" t="s">
+        <v>178</v>
+      </c>
+      <c r="I104" t="s">
+        <v>32</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L104" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="M104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O104" t="s">
         <v>198</v>
-      </c>
-      <c r="E104" t="s">
-        <v>32</v>
-      </c>
-      <c r="F104" t="s">
-        <v>32</v>
-      </c>
-      <c r="G104" t="s">
-        <v>32</v>
-      </c>
-      <c r="H104" t="s">
-        <v>179</v>
-      </c>
-      <c r="I104" t="s">
-        <v>32</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L104" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="M104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O104" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B105" t="s">
         <v>136</v>
@@ -8771,7 +8765,7 @@
         <v>144</v>
       </c>
       <c r="D105" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E105" t="s">
         <v>32</v>
@@ -8783,7 +8777,7 @@
         <v>32</v>
       </c>
       <c r="H105" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I105" s="2">
         <v>3</v>
@@ -8798,7 +8792,7 @@
         <v>5</v>
       </c>
       <c r="M105" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N105" s="2" t="s">
         <v>20</v>
@@ -8809,7 +8803,7 @@
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B106" t="s">
         <v>136</v>
@@ -8818,7 +8812,7 @@
         <v>144</v>
       </c>
       <c r="D106" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E106" t="s">
         <v>32</v>
@@ -8830,7 +8824,7 @@
         <v>32</v>
       </c>
       <c r="H106" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I106" s="2">
         <v>2</v>
@@ -8845,7 +8839,7 @@
         <v>3</v>
       </c>
       <c r="M106" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N106" s="2" t="s">
         <v>22</v>
@@ -8856,7 +8850,7 @@
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B107" t="s">
         <v>136</v>
@@ -8865,7 +8859,7 @@
         <v>144</v>
       </c>
       <c r="D107" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E107" t="s">
         <v>32</v>
@@ -8877,7 +8871,7 @@
         <v>32</v>
       </c>
       <c r="H107" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I107" s="2">
         <v>1</v>
@@ -8892,7 +8886,7 @@
         <v>1</v>
       </c>
       <c r="M107" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N107" s="2" t="s">
         <v>18</v>
@@ -8903,7 +8897,7 @@
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B108" t="s">
         <v>136</v>
@@ -8912,7 +8906,7 @@
         <v>144</v>
       </c>
       <c r="D108" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E108" t="s">
         <v>32</v>
@@ -8924,7 +8918,7 @@
         <v>32</v>
       </c>
       <c r="H108" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I108" s="2">
         <v>0</v>
@@ -8939,7 +8933,7 @@
         <v>32</v>
       </c>
       <c r="M108" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N108" s="2" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Updates to Rank and other scripts
</commit_message>
<xml_diff>
--- a/Data/Criteria_and_Scoring/Habitat_Limiting_Factor_Rating_Criteria.xlsx
+++ b/Data/Criteria_and_Scoring/Habitat_Limiting_Factor_Rating_Criteria.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439D82FA-020C-4330-88D5-B5FBA7F89504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F7DCEA-334D-49D6-AA8E-0A9276E8A258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17520" windowHeight="11184" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
+    <workbookView xWindow="924" yWindow="2556" windowWidth="22200" windowHeight="11100" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$111</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="217">
   <si>
     <t>Habitat Limiting Factor Scoring Rules</t>
   </si>
@@ -586,9 +586,6 @@
     <t>Contaminants_303d</t>
   </si>
   <si>
-    <t>Dominant_Substrate_CATEGORY_1,Bank_Stability_CATEGORY_1,Structure_CATEGORY_1,Pieces_per_mile_CATEGORY_1,Floodplain_Connectivity_CATEGORY_1,Entrenchment_CATEGORY_2,Connectivity_CATEGORY_1,Pools_CATEGORY_1,RAWatershed_Rating_Flow,RAWatershed_Rating_Temp</t>
-  </si>
-  <si>
     <t>Category_Type</t>
   </si>
   <si>
@@ -682,7 +679,34 @@
     <t>NorWEST Canopy Cover</t>
   </si>
   <si>
-    <t>GravelCobble_UCSRB_pct,GRVL_COBL_UCSRB_CHAMP</t>
+    <t>GravelCobble_UCSRB_pct,GRVL_COBL_UCSRB_CHAMP,EDT_UCSRBCoarseSub pct</t>
+  </si>
+  <si>
+    <t>Dominant_Substrate_CATEGORY_1,Bank_Stability_CATEGORY_1,Structure_CATEGORY_1,Pieces_per_mile_CATEGORY_1,Floodplain_Connectivity_CATEGORY_1,Entrenchment_CATEGORY_2,Connectivity_CATEGORY_1,Pools_CATEGORY_1,RAWatershed_Rating_Flow,RAWatershed_Rating_Temp,EDT_Level 2 Benthic Richness,EDT_Level 2 Confinement: Artificial,EDT_Level 2,Embeddedness,EDT_Level 2 Fine Sediment,EDT_Level 2 Fish Pathogens,EDT_Level 2 Flow: Inter-Annual High Flow Variation,EDT_Level 2 Flow: Inter-Annual Low Flow Variation,EDT_Level 2 Predation Risk,EDT_Level 2 Riparian/stream interface,EDT_Temperature: Daily Maximum,EDT_Temperature: Food Effect,EDT_Width,EDT_Woody Debris,EDT_Predation Risk</t>
+  </si>
+  <si>
+    <t>EDT_Floodplain</t>
+  </si>
+  <si>
+    <t>Floodplain- EDT</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>EDT_Floodplain pct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0% channel wetted edge that has been diked or ditched to prevent floodplain access during approximately 10 year return interval floods events. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-50% channel wetted edge that has been diked or ditched to prevent floodplain access during approximately 10 year return interval floods events. </t>
+  </si>
+  <si>
+    <t>&gt;50% side channel area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLOODPLAIN- EDT the fraction of channel wetted edge that has been diked or ditched to prevent floodplain access during approximately 10 year return interval floods events. </t>
   </si>
 </sst>
 </file>
@@ -3781,12 +3805,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FD6E8C-F414-4D9F-82CB-33D09B6D4DCD}">
-  <dimension ref="A1:O108"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:O111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="J74" sqref="J74"/>
+      <selection pane="bottomLeft" activeCell="L112" sqref="L112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3817,22 +3842,22 @@
         <v>126</v>
       </c>
       <c r="F1" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="38" t="s">
-        <v>183</v>
-      </c>
       <c r="H1" s="38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I1" s="38" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="K1" s="38" t="s">
         <v>180</v>
-      </c>
-      <c r="K1" s="38" t="s">
-        <v>181</v>
       </c>
       <c r="L1" s="39" t="s">
         <v>10</v>
@@ -3847,7 +3872,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -3870,7 +3895,7 @@
         <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I2" s="2">
         <v>0</v>
@@ -3895,7 +3920,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -3918,7 +3943,7 @@
         <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I3" s="2">
         <v>1.4</v>
@@ -3943,7 +3968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -3966,7 +3991,7 @@
         <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I4" s="2">
         <v>2.2000000000000002</v>
@@ -3991,7 +4016,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -4014,7 +4039,7 @@
         <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -4039,7 +4064,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -4062,7 +4087,7 @@
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -4086,7 +4111,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>95</v>
       </c>
@@ -4109,7 +4134,7 @@
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I7" s="2">
         <v>20</v>
@@ -4134,7 +4159,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -4157,7 +4182,7 @@
         <v>100000</v>
       </c>
       <c r="H8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -4182,7 +4207,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -4205,7 +4230,7 @@
         <v>100000</v>
       </c>
       <c r="H9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I9" s="2">
         <v>17</v>
@@ -4230,7 +4255,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -4253,7 +4278,7 @@
         <v>100000</v>
       </c>
       <c r="H10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I10" s="2">
         <v>70</v>
@@ -4278,7 +4303,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -4301,7 +4326,7 @@
         <v>32</v>
       </c>
       <c r="H11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -4326,7 +4351,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -4349,7 +4374,7 @@
         <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I12" s="2">
         <v>2</v>
@@ -4374,7 +4399,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -4397,7 +4422,7 @@
         <v>32</v>
       </c>
       <c r="H13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I13" s="2">
         <v>5</v>
@@ -4422,7 +4447,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -4445,7 +4470,7 @@
         <v>32</v>
       </c>
       <c r="H14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -4470,7 +4495,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -4493,7 +4518,7 @@
         <v>32</v>
       </c>
       <c r="H15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I15" s="2">
         <v>0.1</v>
@@ -4517,7 +4542,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -4540,7 +4565,7 @@
         <v>32</v>
       </c>
       <c r="H16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I16" s="2">
         <v>20</v>
@@ -4565,7 +4590,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -4588,7 +4613,7 @@
         <v>32</v>
       </c>
       <c r="H17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I17" s="2">
         <v>0</v>
@@ -4613,7 +4638,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -4636,7 +4661,7 @@
         <v>32</v>
       </c>
       <c r="H18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I18" s="2">
         <v>0.1</v>
@@ -4661,7 +4686,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -4684,7 +4709,7 @@
         <v>32</v>
       </c>
       <c r="H19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I19" s="2">
         <v>5</v>
@@ -4709,7 +4734,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="36" t="s">
         <v>54</v>
       </c>
@@ -4724,7 +4749,7 @@
       <c r="F20" s="36"/>
       <c r="G20" s="36"/>
       <c r="H20" s="36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I20" s="37">
         <v>0</v>
@@ -4750,7 +4775,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="36" t="s">
         <v>54</v>
       </c>
@@ -4765,7 +4790,7 @@
       <c r="F21" s="36"/>
       <c r="G21" s="36"/>
       <c r="H21" s="36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I21" s="37">
         <v>5</v>
@@ -4791,7 +4816,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36" t="s">
         <v>54</v>
       </c>
@@ -4806,7 +4831,7 @@
       <c r="F22" s="36"/>
       <c r="G22" s="36"/>
       <c r="H22" s="36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I22" s="37">
         <v>20</v>
@@ -4832,7 +4857,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -4855,7 +4880,7 @@
         <v>32</v>
       </c>
       <c r="H23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I23" s="2">
         <v>0</v>
@@ -4880,7 +4905,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -4903,7 +4928,7 @@
         <v>32</v>
       </c>
       <c r="H24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I24" s="2">
         <v>10</v>
@@ -4928,7 +4953,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -4951,7 +4976,7 @@
         <v>32</v>
       </c>
       <c r="H25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I25" s="2">
         <v>20</v>
@@ -4976,7 +5001,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -5000,7 +5025,7 @@
         <v>1.524</v>
       </c>
       <c r="H26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I26" s="2">
         <v>0</v>
@@ -5025,7 +5050,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -5049,7 +5074,7 @@
         <v>1.524</v>
       </c>
       <c r="H27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I27" s="2">
         <v>184</v>
@@ -5074,7 +5099,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -5098,7 +5123,7 @@
         <v>1.524</v>
       </c>
       <c r="H28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>32</v>
@@ -5123,7 +5148,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -5148,7 +5173,7 @@
         <v>3.048</v>
       </c>
       <c r="H29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I29" s="2">
         <v>0</v>
@@ -5173,7 +5198,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -5198,7 +5223,7 @@
         <v>3.048</v>
       </c>
       <c r="H30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I30" s="2">
         <v>95</v>
@@ -5223,7 +5248,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -5248,7 +5273,7 @@
         <v>3.048</v>
       </c>
       <c r="H31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>32</v>
@@ -5271,7 +5296,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -5296,7 +5321,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I32" s="2">
         <v>0</v>
@@ -5321,7 +5346,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -5346,7 +5371,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H33" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I33" s="2">
         <v>70</v>
@@ -5371,7 +5396,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -5396,7 +5421,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>32</v>
@@ -5421,7 +5446,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -5446,7 +5471,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
@@ -5471,7 +5496,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -5496,7 +5521,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I36" s="2">
         <v>55</v>
@@ -5521,7 +5546,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>84</v>
       </c>
@@ -5546,7 +5571,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>32</v>
@@ -5571,7 +5596,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -5596,7 +5621,7 @@
         <v>7.62</v>
       </c>
       <c r="H38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I38" s="2">
         <v>0</v>
@@ -5621,7 +5646,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -5646,7 +5671,7 @@
         <v>7.62</v>
       </c>
       <c r="H39" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I39" s="2">
         <v>47</v>
@@ -5671,7 +5696,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -5696,7 +5721,7 @@
         <v>7.62</v>
       </c>
       <c r="H40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>32</v>
@@ -5721,7 +5746,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -5746,7 +5771,7 @@
         <v>15.24</v>
       </c>
       <c r="H41" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I41" s="2">
         <v>0</v>
@@ -5771,7 +5796,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -5796,7 +5821,7 @@
         <v>15.24</v>
       </c>
       <c r="H42" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I42" s="2">
         <v>25</v>
@@ -5821,7 +5846,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -5846,7 +5871,7 @@
         <v>15.24</v>
       </c>
       <c r="H43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>32</v>
@@ -5871,7 +5896,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -5896,7 +5921,7 @@
         <v>22.86</v>
       </c>
       <c r="H44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I44" s="2">
         <v>0</v>
@@ -5921,7 +5946,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -5946,7 +5971,7 @@
         <v>22.86</v>
       </c>
       <c r="H45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I45" s="2">
         <v>23</v>
@@ -5971,7 +5996,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -5996,7 +6021,7 @@
         <v>22.86</v>
       </c>
       <c r="H46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>32</v>
@@ -6021,7 +6046,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -6045,7 +6070,7 @@
         <v>100000</v>
       </c>
       <c r="H47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I47" s="2">
         <v>0</v>
@@ -6070,7 +6095,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>84</v>
       </c>
@@ -6094,7 +6119,7 @@
         <v>100000</v>
       </c>
       <c r="H48" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I48" s="2">
         <v>18</v>
@@ -6119,7 +6144,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>84</v>
       </c>
@@ -6143,7 +6168,7 @@
         <v>100000</v>
       </c>
       <c r="H49" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>32</v>
@@ -6168,24 +6193,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B50" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E50" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H50" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I50" s="41">
         <v>0</v>
@@ -6211,24 +6236,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B51" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D51" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E51" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H51" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I51" s="41">
         <v>50</v>
@@ -6253,24 +6278,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B52" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E52" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H52" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I52" s="41">
         <v>80</v>
@@ -6295,7 +6320,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -6318,7 +6343,7 @@
         <v>32</v>
       </c>
       <c r="H53" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I53" s="2">
         <v>0</v>
@@ -6343,7 +6368,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -6366,7 +6391,7 @@
         <v>32</v>
       </c>
       <c r="H54" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I54" s="2">
         <v>2</v>
@@ -6391,7 +6416,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -6414,7 +6439,7 @@
         <v>32</v>
       </c>
       <c r="H55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I55" s="2">
         <v>5</v>
@@ -6439,7 +6464,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -6462,7 +6487,7 @@
         <v>32</v>
       </c>
       <c r="H56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I56" s="2">
         <v>-5</v>
@@ -6486,7 +6511,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -6509,7 +6534,7 @@
         <v>32</v>
       </c>
       <c r="H57" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I57" s="2">
         <v>1</v>
@@ -6533,7 +6558,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -6556,7 +6581,7 @@
         <v>32</v>
       </c>
       <c r="H58" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I58" s="2">
         <v>4</v>
@@ -6580,7 +6605,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -6603,7 +6628,7 @@
         <v>32</v>
       </c>
       <c r="H59" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I59" s="2">
         <v>0</v>
@@ -6618,7 +6643,7 @@
         <v>1</v>
       </c>
       <c r="M59" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>18</v>
@@ -6627,7 +6652,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -6650,13 +6675,13 @@
         <v>32</v>
       </c>
       <c r="H60" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I60" s="2">
         <v>2</v>
       </c>
       <c r="J60" s="2">
-        <f t="shared" ref="J59:J82" si="2">I60</f>
+        <f t="shared" ref="J60:J82" si="2">I60</f>
         <v>2</v>
       </c>
       <c r="K60" s="2">
@@ -6675,7 +6700,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -6698,7 +6723,7 @@
         <v>32</v>
       </c>
       <c r="H61" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I61" s="2">
         <v>5</v>
@@ -6723,7 +6748,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>37</v>
       </c>
@@ -6734,7 +6759,7 @@
         <v>148</v>
       </c>
       <c r="D62" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E62" t="s">
         <v>32</v>
@@ -6746,7 +6771,7 @@
         <v>32</v>
       </c>
       <c r="H62" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I62" s="2">
         <v>0</v>
@@ -6770,7 +6795,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>37</v>
       </c>
@@ -6781,7 +6806,7 @@
         <v>148</v>
       </c>
       <c r="D63" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E63" t="s">
         <v>32</v>
@@ -6793,7 +6818,7 @@
         <v>32</v>
       </c>
       <c r="H63" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I63" s="2">
         <v>1</v>
@@ -6817,7 +6842,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -6828,7 +6853,7 @@
         <v>148</v>
       </c>
       <c r="D64" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E64" t="s">
         <v>32</v>
@@ -6840,7 +6865,7 @@
         <v>32</v>
       </c>
       <c r="H64" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I64" s="2">
         <v>50</v>
@@ -6865,7 +6890,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>58</v>
       </c>
@@ -6888,7 +6913,7 @@
         <v>32</v>
       </c>
       <c r="H65" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I65" s="2">
         <v>0</v>
@@ -6912,7 +6937,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>58</v>
       </c>
@@ -6935,7 +6960,7 @@
         <v>32</v>
       </c>
       <c r="H66" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I66" s="2">
         <v>12</v>
@@ -6960,7 +6985,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>58</v>
       </c>
@@ -6983,7 +7008,7 @@
         <v>32</v>
       </c>
       <c r="H67" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I67" s="2">
         <v>20</v>
@@ -7008,7 +7033,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="40" t="s">
         <v>73</v>
       </c>
@@ -7031,7 +7056,7 @@
         <v>32</v>
       </c>
       <c r="H68" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I68" s="41">
         <v>0</v>
@@ -7055,7 +7080,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="40" t="s">
         <v>73</v>
       </c>
@@ -7078,7 +7103,7 @@
         <v>32</v>
       </c>
       <c r="H69" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I69" s="41">
         <v>10</v>
@@ -7103,7 +7128,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="40" t="s">
         <v>73</v>
       </c>
@@ -7126,7 +7151,7 @@
         <v>32</v>
       </c>
       <c r="H70" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I70" s="41">
         <v>20</v>
@@ -7151,7 +7176,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="40" t="s">
         <v>85</v>
       </c>
@@ -7162,7 +7187,7 @@
         <v>148</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E71" s="40" t="s">
         <v>32</v>
@@ -7174,7 +7199,7 @@
         <v>32</v>
       </c>
       <c r="H71" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I71" s="41">
         <v>0</v>
@@ -7198,7 +7223,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="40" t="s">
         <v>85</v>
       </c>
@@ -7209,7 +7234,7 @@
         <v>148</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E72" s="40" t="s">
         <v>32</v>
@@ -7221,7 +7246,7 @@
         <v>32</v>
       </c>
       <c r="H72" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I72" s="41">
         <v>15</v>
@@ -7246,7 +7271,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="40" t="s">
         <v>85</v>
       </c>
@@ -7257,7 +7282,7 @@
         <v>148</v>
       </c>
       <c r="D73" s="40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E73" s="40" t="s">
         <v>32</v>
@@ -7269,7 +7294,7 @@
         <v>32</v>
       </c>
       <c r="H73" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I73" s="41">
         <v>30</v>
@@ -7294,7 +7319,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="40" t="s">
         <v>14</v>
       </c>
@@ -7317,7 +7342,7 @@
         <v>32</v>
       </c>
       <c r="H74" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I74" s="41">
         <v>0</v>
@@ -7343,7 +7368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="40" t="s">
         <v>14</v>
       </c>
@@ -7366,7 +7391,7 @@
         <v>32</v>
       </c>
       <c r="H75" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I75" s="41">
         <v>12</v>
@@ -7392,7 +7417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="40" t="s">
         <v>14</v>
       </c>
@@ -7415,7 +7440,7 @@
         <v>32</v>
       </c>
       <c r="H76" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I76" s="41">
         <v>14</v>
@@ -7441,7 +7466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="40" t="s">
         <v>35</v>
       </c>
@@ -7464,7 +7489,7 @@
         <v>32</v>
       </c>
       <c r="H77" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I77" s="41">
         <v>0</v>
@@ -7489,7 +7514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="40" t="s">
         <v>35</v>
       </c>
@@ -7512,7 +7537,7 @@
         <v>32</v>
       </c>
       <c r="H78" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I78" s="41">
         <v>10</v>
@@ -7537,7 +7562,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="40" t="s">
         <v>35</v>
       </c>
@@ -7560,7 +7585,7 @@
         <v>32</v>
       </c>
       <c r="H79" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I79" s="41">
         <v>14</v>
@@ -7593,7 +7618,7 @@
         <v>141</v>
       </c>
       <c r="C80" s="40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D80" s="40" t="s">
         <v>169</v>
@@ -7608,7 +7633,7 @@
         <v>32</v>
       </c>
       <c r="H80" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I80" s="41">
         <v>0</v>
@@ -7624,7 +7649,7 @@
         <v>5</v>
       </c>
       <c r="M80" s="41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N80" s="41" t="s">
         <v>20</v>
@@ -7641,7 +7666,7 @@
         <v>141</v>
       </c>
       <c r="C81" s="40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D81" s="40" t="s">
         <v>169</v>
@@ -7656,7 +7681,7 @@
         <v>32</v>
       </c>
       <c r="H81" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I81" s="41">
         <v>16</v>
@@ -7672,7 +7697,7 @@
         <v>3</v>
       </c>
       <c r="M81" s="41" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N81" s="41" t="s">
         <v>22</v>
@@ -7689,7 +7714,7 @@
         <v>141</v>
       </c>
       <c r="C82" s="40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D82" s="40" t="s">
         <v>169</v>
@@ -7704,7 +7729,7 @@
         <v>32</v>
       </c>
       <c r="H82" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I82" s="41">
         <v>22</v>
@@ -7720,7 +7745,7 @@
         <v>1</v>
       </c>
       <c r="M82" s="41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N82" s="41" t="s">
         <v>18</v>
@@ -7729,9 +7754,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B83" s="40" t="s">
         <v>124</v>
@@ -7740,7 +7765,7 @@
         <v>148</v>
       </c>
       <c r="D83" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E83" s="40" t="s">
         <v>32</v>
@@ -7752,7 +7777,7 @@
         <v>32</v>
       </c>
       <c r="H83" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I83" s="41">
         <v>99</v>
@@ -7767,18 +7792,18 @@
         <v>1</v>
       </c>
       <c r="M83" s="41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N83" s="41" t="s">
         <v>18</v>
       </c>
       <c r="O83" s="40" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B84" s="40" t="s">
         <v>124</v>
@@ -7787,7 +7812,7 @@
         <v>148</v>
       </c>
       <c r="D84" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E84" s="40" t="s">
         <v>32</v>
@@ -7799,7 +7824,7 @@
         <v>32</v>
       </c>
       <c r="H84" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I84" s="41">
         <v>50</v>
@@ -7814,18 +7839,18 @@
         <v>3</v>
       </c>
       <c r="M84" s="41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N84" s="41" t="s">
         <v>22</v>
       </c>
       <c r="O84" s="40" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B85" s="40" t="s">
         <v>124</v>
@@ -7834,7 +7859,7 @@
         <v>148</v>
       </c>
       <c r="D85" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E85" s="40" t="s">
         <v>32</v>
@@ -7846,7 +7871,7 @@
         <v>32</v>
       </c>
       <c r="H85" s="40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I85" s="41">
         <v>0</v>
@@ -7861,16 +7886,16 @@
         <v>5</v>
       </c>
       <c r="M85" s="41" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N85" s="41" t="s">
         <v>20</v>
       </c>
       <c r="O85" s="40" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="40" t="s">
         <v>15</v>
       </c>
@@ -7890,7 +7915,7 @@
         <v>32</v>
       </c>
       <c r="H86" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I86" s="41" t="s">
         <v>24</v>
@@ -7905,7 +7930,7 @@
         <v>1</v>
       </c>
       <c r="M86" s="41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N86" s="41" t="s">
         <v>32</v>
@@ -7914,7 +7939,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="40" t="s">
         <v>15</v>
       </c>
@@ -7934,7 +7959,7 @@
         <v>32</v>
       </c>
       <c r="H87" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I87" s="41" t="s">
         <v>28</v>
@@ -7949,7 +7974,7 @@
         <v>3</v>
       </c>
       <c r="M87" s="41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N87" s="41" t="s">
         <v>32</v>
@@ -7958,7 +7983,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="40" t="s">
         <v>15</v>
       </c>
@@ -7978,7 +8003,7 @@
         <v>32</v>
       </c>
       <c r="H88" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I88" s="41" t="s">
         <v>31</v>
@@ -8002,7 +8027,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -8025,7 +8050,7 @@
         <v>32</v>
       </c>
       <c r="H89" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I89" s="3" t="s">
         <v>32</v>
@@ -8049,7 +8074,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>36</v>
       </c>
@@ -8072,7 +8097,7 @@
         <v>32</v>
       </c>
       <c r="H90" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I90" s="3">
         <v>1</v>
@@ -8096,7 +8121,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>36</v>
       </c>
@@ -8119,7 +8144,7 @@
         <v>32</v>
       </c>
       <c r="H91" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I91" s="3">
         <v>2</v>
@@ -8143,7 +8168,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>36</v>
       </c>
@@ -8166,7 +8191,7 @@
         <v>32</v>
       </c>
       <c r="H92" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I92" s="3" t="s">
         <v>51</v>
@@ -8190,7 +8215,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="93" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>36</v>
       </c>
@@ -8213,7 +8238,7 @@
         <v>32</v>
       </c>
       <c r="H93" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I93" s="3" t="s">
         <v>56</v>
@@ -8237,7 +8262,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>36</v>
       </c>
@@ -8260,7 +8285,7 @@
         <v>32</v>
       </c>
       <c r="H94" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I94" s="3" t="s">
         <v>59</v>
@@ -8284,7 +8309,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>36</v>
       </c>
@@ -8307,7 +8332,7 @@
         <v>32</v>
       </c>
       <c r="H95" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I95" s="3">
         <v>5</v>
@@ -8331,7 +8356,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -8342,7 +8367,7 @@
         <v>144</v>
       </c>
       <c r="D96" t="s">
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="E96" t="s">
         <v>32</v>
@@ -8354,7 +8379,7 @@
         <v>32</v>
       </c>
       <c r="H96" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>20</v>
@@ -8378,7 +8403,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -8389,7 +8414,7 @@
         <v>144</v>
       </c>
       <c r="D97" t="s">
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="E97" t="s">
         <v>32</v>
@@ -8401,7 +8426,7 @@
         <v>32</v>
       </c>
       <c r="H97" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>22</v>
@@ -8425,7 +8450,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -8436,7 +8461,7 @@
         <v>144</v>
       </c>
       <c r="D98" t="s">
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="E98" t="s">
         <v>32</v>
@@ -8448,7 +8473,7 @@
         <v>32</v>
       </c>
       <c r="H98" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>18</v>
@@ -8472,7 +8497,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -8483,7 +8508,7 @@
         <v>144</v>
       </c>
       <c r="D99" t="s">
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="E99" t="s">
         <v>32</v>
@@ -8495,7 +8520,7 @@
         <v>32</v>
       </c>
       <c r="H99" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>32</v>
@@ -8519,7 +8544,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>173</v>
       </c>
@@ -8542,7 +8567,7 @@
         <v>32</v>
       </c>
       <c r="H100" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I100" s="3" t="s">
         <v>32</v>
@@ -8566,7 +8591,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -8577,7 +8602,7 @@
         <v>144</v>
       </c>
       <c r="D101" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E101" t="s">
         <v>32</v>
@@ -8589,7 +8614,7 @@
         <v>32</v>
       </c>
       <c r="H101" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I101">
         <v>1</v>
@@ -8610,10 +8635,10 @@
         <v>32</v>
       </c>
       <c r="O101" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -8624,7 +8649,7 @@
         <v>144</v>
       </c>
       <c r="D102" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E102" t="s">
         <v>32</v>
@@ -8636,7 +8661,7 @@
         <v>32</v>
       </c>
       <c r="H102" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I102">
         <v>3</v>
@@ -8657,10 +8682,10 @@
         <v>32</v>
       </c>
       <c r="O102" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -8671,7 +8696,7 @@
         <v>144</v>
       </c>
       <c r="D103" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E103" t="s">
         <v>32</v>
@@ -8683,7 +8708,7 @@
         <v>32</v>
       </c>
       <c r="H103" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I103">
         <v>5</v>
@@ -8704,10 +8729,10 @@
         <v>32</v>
       </c>
       <c r="O103" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>7</v>
       </c>
@@ -8718,45 +8743,45 @@
         <v>144</v>
       </c>
       <c r="D104" t="s">
+        <v>196</v>
+      </c>
+      <c r="E104" t="s">
+        <v>32</v>
+      </c>
+      <c r="F104" t="s">
+        <v>32</v>
+      </c>
+      <c r="G104" t="s">
+        <v>32</v>
+      </c>
+      <c r="H104" t="s">
+        <v>177</v>
+      </c>
+      <c r="I104" t="s">
+        <v>32</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L104" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="M104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O104" t="s">
         <v>197</v>
       </c>
-      <c r="E104" t="s">
-        <v>32</v>
-      </c>
-      <c r="F104" t="s">
-        <v>32</v>
-      </c>
-      <c r="G104" t="s">
-        <v>32</v>
-      </c>
-      <c r="H104" t="s">
-        <v>178</v>
-      </c>
-      <c r="I104" t="s">
-        <v>32</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L104" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="M104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O104" t="s">
+    </row>
+    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>199</v>
       </c>
       <c r="B105" t="s">
         <v>136</v>
@@ -8765,7 +8790,7 @@
         <v>144</v>
       </c>
       <c r="D105" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E105" t="s">
         <v>32</v>
@@ -8777,7 +8802,7 @@
         <v>32</v>
       </c>
       <c r="H105" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I105" s="2">
         <v>3</v>
@@ -8792,7 +8817,7 @@
         <v>5</v>
       </c>
       <c r="M105" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N105" s="2" t="s">
         <v>20</v>
@@ -8801,9 +8826,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B106" t="s">
         <v>136</v>
@@ -8812,7 +8837,7 @@
         <v>144</v>
       </c>
       <c r="D106" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E106" t="s">
         <v>32</v>
@@ -8824,7 +8849,7 @@
         <v>32</v>
       </c>
       <c r="H106" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I106" s="2">
         <v>2</v>
@@ -8839,7 +8864,7 @@
         <v>3</v>
       </c>
       <c r="M106" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N106" s="2" t="s">
         <v>22</v>
@@ -8848,9 +8873,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B107" t="s">
         <v>136</v>
@@ -8859,7 +8884,7 @@
         <v>144</v>
       </c>
       <c r="D107" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E107" t="s">
         <v>32</v>
@@ -8871,7 +8896,7 @@
         <v>32</v>
       </c>
       <c r="H107" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I107" s="2">
         <v>1</v>
@@ -8886,7 +8911,7 @@
         <v>1</v>
       </c>
       <c r="M107" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N107" s="2" t="s">
         <v>18</v>
@@ -8895,9 +8920,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B108" t="s">
         <v>136</v>
@@ -8906,7 +8931,7 @@
         <v>144</v>
       </c>
       <c r="D108" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E108" t="s">
         <v>32</v>
@@ -8918,7 +8943,7 @@
         <v>32</v>
       </c>
       <c r="H108" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I108" s="2">
         <v>0</v>
@@ -8933,7 +8958,7 @@
         <v>32</v>
       </c>
       <c r="M108" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N108" s="2" t="s">
         <v>32</v>
@@ -8942,8 +8967,159 @@
         <v>32</v>
       </c>
     </row>
+    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>209</v>
+      </c>
+      <c r="B109" t="s">
+        <v>210</v>
+      </c>
+      <c r="C109" t="s">
+        <v>211</v>
+      </c>
+      <c r="D109" t="s">
+        <v>212</v>
+      </c>
+      <c r="E109" t="s">
+        <v>32</v>
+      </c>
+      <c r="F109" t="s">
+        <v>32</v>
+      </c>
+      <c r="G109" t="s">
+        <v>32</v>
+      </c>
+      <c r="H109" t="s">
+        <v>178</v>
+      </c>
+      <c r="I109" s="2">
+        <v>0</v>
+      </c>
+      <c r="J109" s="2">
+        <v>0</v>
+      </c>
+      <c r="K109">
+        <v>1E-4</v>
+      </c>
+      <c r="L109" s="35">
+        <v>5</v>
+      </c>
+      <c r="M109" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="N109" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O109" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>209</v>
+      </c>
+      <c r="B110" t="s">
+        <v>210</v>
+      </c>
+      <c r="C110" t="s">
+        <v>211</v>
+      </c>
+      <c r="D110" t="s">
+        <v>212</v>
+      </c>
+      <c r="E110" t="s">
+        <v>32</v>
+      </c>
+      <c r="F110" t="s">
+        <v>32</v>
+      </c>
+      <c r="G110" t="s">
+        <v>32</v>
+      </c>
+      <c r="H110" t="s">
+        <v>178</v>
+      </c>
+      <c r="I110" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="J110" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="K110">
+        <v>49.9</v>
+      </c>
+      <c r="L110" s="35">
+        <v>3</v>
+      </c>
+      <c r="M110" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="N110" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O110" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>209</v>
+      </c>
+      <c r="B111" t="s">
+        <v>210</v>
+      </c>
+      <c r="C111" t="s">
+        <v>211</v>
+      </c>
+      <c r="D111" t="s">
+        <v>212</v>
+      </c>
+      <c r="E111" t="s">
+        <v>32</v>
+      </c>
+      <c r="F111" t="s">
+        <v>32</v>
+      </c>
+      <c r="G111" t="s">
+        <v>32</v>
+      </c>
+      <c r="H111" t="s">
+        <v>178</v>
+      </c>
+      <c r="I111" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J111" s="2">
+        <v>49.9</v>
+      </c>
+      <c r="K111">
+        <v>101</v>
+      </c>
+      <c r="L111" s="35">
+        <v>1</v>
+      </c>
+      <c r="M111" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="N111" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O111" t="s">
+        <v>216</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O100" xr:uid="{964DF2B0-6B32-465A-9085-889E032C36AD}">
+  <autoFilter ref="A1:O111" xr:uid="{964DF2B0-6B32-465A-9085-889E032C36AD}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Temperature- Rearing"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="NORWEST_Temperature"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O100">
       <sortCondition descending="1" ref="H1:H100"/>
     </sortState>

</xml_diff>

<commit_message>
Minor updates to data being read in, etc.
</commit_message>
<xml_diff>
--- a/Data/Criteria_and_Scoring/Habitat_Limiting_Factor_Rating_Criteria.xlsx
+++ b/Data/Criteria_and_Scoring/Habitat_Limiting_Factor_Rating_Criteria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F7DCEA-334D-49D6-AA8E-0A9276E8A258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817915E2-1E8F-416D-8660-8838B6E40127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="924" yWindow="2556" windowWidth="22200" windowHeight="11100" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
+    <workbookView xWindow="2760" yWindow="1224" windowWidth="20244" windowHeight="10896" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="218">
   <si>
     <t>Habitat Limiting Factor Scoring Rules</t>
   </si>
@@ -559,9 +559,6 @@
     <t>Pools_deeper_3_ft_prcnt_INDICATOR_3</t>
   </si>
   <si>
-    <t>Pools_deeper_3_ft_per_mile_INDICATOR_4</t>
-  </si>
-  <si>
     <t>Temperature- Adult Holding</t>
   </si>
   <si>
@@ -707,6 +704,12 @@
   </si>
   <si>
     <t xml:space="preserve">FLOODPLAIN- EDT the fraction of channel wetted edge that has been diked or ditched to prevent floodplain access during approximately 10 year return interval floods events. </t>
+  </si>
+  <si>
+    <t>Pools_deeper_3_ft_per_mile_INDICATOR_4,Pools_deeper_5_ft_per_mile_INDICATOR_5</t>
+  </si>
+  <si>
+    <t>no pools are &gt;3ft (or 5 ft for 5 ft deep pools indicator)</t>
   </si>
 </sst>
 </file>
@@ -3805,13 +3808,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FD6E8C-F414-4D9F-82CB-33D09B6D4DCD}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="L112" sqref="L112"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3842,22 +3844,22 @@
         <v>126</v>
       </c>
       <c r="F1" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="G1" s="38" t="s">
-        <v>182</v>
-      </c>
       <c r="H1" s="38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I1" s="38" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="K1" s="38" t="s">
         <v>179</v>
-      </c>
-      <c r="K1" s="38" t="s">
-        <v>180</v>
       </c>
       <c r="L1" s="39" t="s">
         <v>10</v>
@@ -3872,7 +3874,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -3895,7 +3897,7 @@
         <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I2" s="2">
         <v>0</v>
@@ -3920,7 +3922,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -3943,7 +3945,7 @@
         <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I3" s="2">
         <v>1.4</v>
@@ -3968,7 +3970,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -3991,7 +3993,7 @@
         <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I4" s="2">
         <v>2.2000000000000002</v>
@@ -4016,7 +4018,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -4039,7 +4041,7 @@
         <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -4064,7 +4066,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -4087,7 +4089,7 @@
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -4111,7 +4113,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>95</v>
       </c>
@@ -4134,7 +4136,7 @@
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I7" s="2">
         <v>20</v>
@@ -4159,7 +4161,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -4182,7 +4184,7 @@
         <v>100000</v>
       </c>
       <c r="H8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -4207,7 +4209,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -4230,7 +4232,7 @@
         <v>100000</v>
       </c>
       <c r="H9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I9" s="2">
         <v>17</v>
@@ -4255,7 +4257,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -4278,7 +4280,7 @@
         <v>100000</v>
       </c>
       <c r="H10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I10" s="2">
         <v>70</v>
@@ -4303,7 +4305,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -4326,7 +4328,7 @@
         <v>32</v>
       </c>
       <c r="H11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -4351,7 +4353,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -4374,7 +4376,7 @@
         <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I12" s="2">
         <v>2</v>
@@ -4399,7 +4401,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -4422,7 +4424,7 @@
         <v>32</v>
       </c>
       <c r="H13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I13" s="2">
         <v>5</v>
@@ -4447,7 +4449,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -4470,7 +4472,7 @@
         <v>32</v>
       </c>
       <c r="H14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -4495,7 +4497,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -4518,7 +4520,7 @@
         <v>32</v>
       </c>
       <c r="H15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I15" s="2">
         <v>0.1</v>
@@ -4542,7 +4544,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -4565,7 +4567,7 @@
         <v>32</v>
       </c>
       <c r="H16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I16" s="2">
         <v>20</v>
@@ -4590,7 +4592,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -4601,7 +4603,7 @@
         <v>165</v>
       </c>
       <c r="D17" t="s">
-        <v>167</v>
+        <v>216</v>
       </c>
       <c r="E17" t="s">
         <v>32</v>
@@ -4613,7 +4615,7 @@
         <v>32</v>
       </c>
       <c r="H17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I17" s="2">
         <v>0</v>
@@ -4629,7 +4631,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>23</v>
+        <v>217</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>18</v>
@@ -4638,7 +4640,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -4649,7 +4651,7 @@
         <v>165</v>
       </c>
       <c r="D18" t="s">
-        <v>167</v>
+        <v>216</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -4661,7 +4663,7 @@
         <v>32</v>
       </c>
       <c r="H18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I18" s="2">
         <v>0.1</v>
@@ -4686,7 +4688,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -4697,7 +4699,7 @@
         <v>165</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>216</v>
       </c>
       <c r="E19" t="s">
         <v>32</v>
@@ -4709,7 +4711,7 @@
         <v>32</v>
       </c>
       <c r="H19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I19" s="2">
         <v>5</v>
@@ -4734,7 +4736,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="36" t="s">
         <v>54</v>
       </c>
@@ -4749,7 +4751,7 @@
       <c r="F20" s="36"/>
       <c r="G20" s="36"/>
       <c r="H20" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I20" s="37">
         <v>0</v>
@@ -4775,7 +4777,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="36" t="s">
         <v>54</v>
       </c>
@@ -4790,7 +4792,7 @@
       <c r="F21" s="36"/>
       <c r="G21" s="36"/>
       <c r="H21" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I21" s="37">
         <v>5</v>
@@ -4816,7 +4818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="36" t="s">
         <v>54</v>
       </c>
@@ -4831,7 +4833,7 @@
       <c r="F22" s="36"/>
       <c r="G22" s="36"/>
       <c r="H22" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I22" s="37">
         <v>20</v>
@@ -4857,7 +4859,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -4880,7 +4882,7 @@
         <v>32</v>
       </c>
       <c r="H23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I23" s="2">
         <v>0</v>
@@ -4905,7 +4907,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -4928,7 +4930,7 @@
         <v>32</v>
       </c>
       <c r="H24" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I24" s="2">
         <v>10</v>
@@ -4953,7 +4955,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -4976,7 +4978,7 @@
         <v>32</v>
       </c>
       <c r="H25" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I25" s="2">
         <v>20</v>
@@ -5001,7 +5003,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -5025,7 +5027,7 @@
         <v>1.524</v>
       </c>
       <c r="H26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I26" s="2">
         <v>0</v>
@@ -5050,7 +5052,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -5074,7 +5076,7 @@
         <v>1.524</v>
       </c>
       <c r="H27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I27" s="2">
         <v>184</v>
@@ -5099,7 +5101,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>84</v>
       </c>
@@ -5123,7 +5125,7 @@
         <v>1.524</v>
       </c>
       <c r="H28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>32</v>
@@ -5148,7 +5150,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -5173,7 +5175,7 @@
         <v>3.048</v>
       </c>
       <c r="H29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I29" s="2">
         <v>0</v>
@@ -5198,7 +5200,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -5223,7 +5225,7 @@
         <v>3.048</v>
       </c>
       <c r="H30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I30" s="2">
         <v>95</v>
@@ -5248,7 +5250,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -5273,7 +5275,7 @@
         <v>3.048</v>
       </c>
       <c r="H31" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>32</v>
@@ -5296,7 +5298,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -5321,7 +5323,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I32" s="2">
         <v>0</v>
@@ -5346,7 +5348,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -5371,7 +5373,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H33" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I33" s="2">
         <v>70</v>
@@ -5396,7 +5398,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>84</v>
       </c>
@@ -5421,7 +5423,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>32</v>
@@ -5446,7 +5448,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -5471,7 +5473,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
@@ -5496,7 +5498,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>84</v>
       </c>
@@ -5521,7 +5523,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I36" s="2">
         <v>55</v>
@@ -5546,7 +5548,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>84</v>
       </c>
@@ -5571,7 +5573,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H37" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>32</v>
@@ -5596,7 +5598,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -5621,7 +5623,7 @@
         <v>7.62</v>
       </c>
       <c r="H38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I38" s="2">
         <v>0</v>
@@ -5646,7 +5648,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -5671,7 +5673,7 @@
         <v>7.62</v>
       </c>
       <c r="H39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I39" s="2">
         <v>47</v>
@@ -5696,7 +5698,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>84</v>
       </c>
@@ -5721,7 +5723,7 @@
         <v>7.62</v>
       </c>
       <c r="H40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>32</v>
@@ -5746,7 +5748,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -5771,7 +5773,7 @@
         <v>15.24</v>
       </c>
       <c r="H41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I41" s="2">
         <v>0</v>
@@ -5796,7 +5798,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>84</v>
       </c>
@@ -5821,7 +5823,7 @@
         <v>15.24</v>
       </c>
       <c r="H42" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I42" s="2">
         <v>25</v>
@@ -5846,7 +5848,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -5871,7 +5873,7 @@
         <v>15.24</v>
       </c>
       <c r="H43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>32</v>
@@ -5896,7 +5898,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -5921,7 +5923,7 @@
         <v>22.86</v>
       </c>
       <c r="H44" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I44" s="2">
         <v>0</v>
@@ -5946,7 +5948,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -5971,7 +5973,7 @@
         <v>22.86</v>
       </c>
       <c r="H45" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I45" s="2">
         <v>23</v>
@@ -5996,7 +5998,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -6021,7 +6023,7 @@
         <v>22.86</v>
       </c>
       <c r="H46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>32</v>
@@ -6046,7 +6048,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -6070,7 +6072,7 @@
         <v>100000</v>
       </c>
       <c r="H47" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I47" s="2">
         <v>0</v>
@@ -6095,7 +6097,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:15" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>84</v>
       </c>
@@ -6119,7 +6121,7 @@
         <v>100000</v>
       </c>
       <c r="H48" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I48" s="2">
         <v>18</v>
@@ -6144,7 +6146,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="36" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>84</v>
       </c>
@@ -6168,7 +6170,7 @@
         <v>100000</v>
       </c>
       <c r="H49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>32</v>
@@ -6193,24 +6195,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B50" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E50" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H50" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I50" s="41">
         <v>0</v>
@@ -6236,24 +6238,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B51" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D51" s="40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E51" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H51" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I51" s="41">
         <v>50</v>
@@ -6278,24 +6280,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B52" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E52" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H52" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I52" s="41">
         <v>80</v>
@@ -6320,7 +6322,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -6343,7 +6345,7 @@
         <v>32</v>
       </c>
       <c r="H53" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I53" s="2">
         <v>0</v>
@@ -6368,7 +6370,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -6391,7 +6393,7 @@
         <v>32</v>
       </c>
       <c r="H54" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I54" s="2">
         <v>2</v>
@@ -6416,7 +6418,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -6439,7 +6441,7 @@
         <v>32</v>
       </c>
       <c r="H55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I55" s="2">
         <v>5</v>
@@ -6464,7 +6466,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -6487,7 +6489,7 @@
         <v>32</v>
       </c>
       <c r="H56" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I56" s="2">
         <v>-5</v>
@@ -6511,7 +6513,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -6534,7 +6536,7 @@
         <v>32</v>
       </c>
       <c r="H57" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I57" s="2">
         <v>1</v>
@@ -6558,7 +6560,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -6581,7 +6583,7 @@
         <v>32</v>
       </c>
       <c r="H58" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I58" s="2">
         <v>4</v>
@@ -6605,7 +6607,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -6628,7 +6630,7 @@
         <v>32</v>
       </c>
       <c r="H59" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I59" s="2">
         <v>0</v>
@@ -6643,7 +6645,7 @@
         <v>1</v>
       </c>
       <c r="M59" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>18</v>
@@ -6652,7 +6654,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -6675,7 +6677,7 @@
         <v>32</v>
       </c>
       <c r="H60" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I60" s="2">
         <v>2</v>
@@ -6700,7 +6702,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -6723,7 +6725,7 @@
         <v>32</v>
       </c>
       <c r="H61" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I61" s="2">
         <v>5</v>
@@ -6748,7 +6750,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>37</v>
       </c>
@@ -6759,7 +6761,7 @@
         <v>148</v>
       </c>
       <c r="D62" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E62" t="s">
         <v>32</v>
@@ -6771,7 +6773,7 @@
         <v>32</v>
       </c>
       <c r="H62" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I62" s="2">
         <v>0</v>
@@ -6795,7 +6797,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>37</v>
       </c>
@@ -6806,7 +6808,7 @@
         <v>148</v>
       </c>
       <c r="D63" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E63" t="s">
         <v>32</v>
@@ -6818,7 +6820,7 @@
         <v>32</v>
       </c>
       <c r="H63" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I63" s="2">
         <v>1</v>
@@ -6842,7 +6844,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -6853,7 +6855,7 @@
         <v>148</v>
       </c>
       <c r="D64" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E64" t="s">
         <v>32</v>
@@ -6865,7 +6867,7 @@
         <v>32</v>
       </c>
       <c r="H64" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I64" s="2">
         <v>50</v>
@@ -6890,7 +6892,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>58</v>
       </c>
@@ -6913,7 +6915,7 @@
         <v>32</v>
       </c>
       <c r="H65" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I65" s="2">
         <v>0</v>
@@ -6937,7 +6939,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>58</v>
       </c>
@@ -6960,7 +6962,7 @@
         <v>32</v>
       </c>
       <c r="H66" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I66" s="2">
         <v>12</v>
@@ -6985,7 +6987,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>58</v>
       </c>
@@ -7008,7 +7010,7 @@
         <v>32</v>
       </c>
       <c r="H67" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I67" s="2">
         <v>20</v>
@@ -7033,7 +7035,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="40" t="s">
         <v>73</v>
       </c>
@@ -7056,7 +7058,7 @@
         <v>32</v>
       </c>
       <c r="H68" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I68" s="41">
         <v>0</v>
@@ -7080,7 +7082,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="40" t="s">
         <v>73</v>
       </c>
@@ -7103,7 +7105,7 @@
         <v>32</v>
       </c>
       <c r="H69" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I69" s="41">
         <v>10</v>
@@ -7128,7 +7130,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="40" t="s">
         <v>73</v>
       </c>
@@ -7151,7 +7153,7 @@
         <v>32</v>
       </c>
       <c r="H70" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I70" s="41">
         <v>20</v>
@@ -7176,7 +7178,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="40" t="s">
         <v>85</v>
       </c>
@@ -7187,7 +7189,7 @@
         <v>148</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E71" s="40" t="s">
         <v>32</v>
@@ -7199,7 +7201,7 @@
         <v>32</v>
       </c>
       <c r="H71" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I71" s="41">
         <v>0</v>
@@ -7223,7 +7225,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="40" t="s">
         <v>85</v>
       </c>
@@ -7234,7 +7236,7 @@
         <v>148</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E72" s="40" t="s">
         <v>32</v>
@@ -7246,7 +7248,7 @@
         <v>32</v>
       </c>
       <c r="H72" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I72" s="41">
         <v>15</v>
@@ -7271,7 +7273,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="40" t="s">
         <v>85</v>
       </c>
@@ -7282,7 +7284,7 @@
         <v>148</v>
       </c>
       <c r="D73" s="40" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E73" s="40" t="s">
         <v>32</v>
@@ -7294,7 +7296,7 @@
         <v>32</v>
       </c>
       <c r="H73" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I73" s="41">
         <v>30</v>
@@ -7319,7 +7321,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="40" t="s">
         <v>14</v>
       </c>
@@ -7327,11 +7329,11 @@
         <v>141</v>
       </c>
       <c r="C74" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="D74" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="D74" s="40" t="s">
-        <v>169</v>
-      </c>
       <c r="E74" s="40" t="s">
         <v>32</v>
       </c>
@@ -7342,7 +7344,7 @@
         <v>32</v>
       </c>
       <c r="H74" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I74" s="41">
         <v>0</v>
@@ -7368,7 +7370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="40" t="s">
         <v>14</v>
       </c>
@@ -7376,11 +7378,11 @@
         <v>141</v>
       </c>
       <c r="C75" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="D75" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="D75" s="40" t="s">
-        <v>169</v>
-      </c>
       <c r="E75" s="40" t="s">
         <v>32</v>
       </c>
@@ -7391,7 +7393,7 @@
         <v>32</v>
       </c>
       <c r="H75" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I75" s="41">
         <v>12</v>
@@ -7417,7 +7419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="40" t="s">
         <v>14</v>
       </c>
@@ -7425,11 +7427,11 @@
         <v>141</v>
       </c>
       <c r="C76" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="D76" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="D76" s="40" t="s">
-        <v>169</v>
-      </c>
       <c r="E76" s="40" t="s">
         <v>32</v>
       </c>
@@ -7440,7 +7442,7 @@
         <v>32</v>
       </c>
       <c r="H76" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I76" s="41">
         <v>14</v>
@@ -7466,7 +7468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="40" t="s">
         <v>35</v>
       </c>
@@ -7474,10 +7476,10 @@
         <v>141</v>
       </c>
       <c r="C77" s="40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D77" s="40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E77" s="40" t="s">
         <v>32</v>
@@ -7489,7 +7491,7 @@
         <v>32</v>
       </c>
       <c r="H77" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I77" s="41">
         <v>0</v>
@@ -7514,7 +7516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="40" t="s">
         <v>35</v>
       </c>
@@ -7522,10 +7524,10 @@
         <v>141</v>
       </c>
       <c r="C78" s="40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D78" s="40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E78" s="40" t="s">
         <v>32</v>
@@ -7537,7 +7539,7 @@
         <v>32</v>
       </c>
       <c r="H78" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I78" s="41">
         <v>10</v>
@@ -7562,7 +7564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="40" t="s">
         <v>35</v>
       </c>
@@ -7570,10 +7572,10 @@
         <v>141</v>
       </c>
       <c r="C79" s="40" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D79" s="40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E79" s="40" t="s">
         <v>32</v>
@@ -7585,7 +7587,7 @@
         <v>32</v>
       </c>
       <c r="H79" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I79" s="41">
         <v>14</v>
@@ -7618,10 +7620,10 @@
         <v>141</v>
       </c>
       <c r="C80" s="40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D80" s="40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E80" s="40" t="s">
         <v>32</v>
@@ -7633,7 +7635,7 @@
         <v>32</v>
       </c>
       <c r="H80" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I80" s="41">
         <v>0</v>
@@ -7649,7 +7651,7 @@
         <v>5</v>
       </c>
       <c r="M80" s="41" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N80" s="41" t="s">
         <v>20</v>
@@ -7666,10 +7668,10 @@
         <v>141</v>
       </c>
       <c r="C81" s="40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D81" s="40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E81" s="40" t="s">
         <v>32</v>
@@ -7681,7 +7683,7 @@
         <v>32</v>
       </c>
       <c r="H81" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I81" s="41">
         <v>16</v>
@@ -7697,7 +7699,7 @@
         <v>3</v>
       </c>
       <c r="M81" s="41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N81" s="41" t="s">
         <v>22</v>
@@ -7714,10 +7716,10 @@
         <v>141</v>
       </c>
       <c r="C82" s="40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D82" s="40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E82" s="40" t="s">
         <v>32</v>
@@ -7729,7 +7731,7 @@
         <v>32</v>
       </c>
       <c r="H82" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I82" s="41">
         <v>22</v>
@@ -7745,7 +7747,7 @@
         <v>1</v>
       </c>
       <c r="M82" s="41" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N82" s="41" t="s">
         <v>18</v>
@@ -7754,9 +7756,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B83" s="40" t="s">
         <v>124</v>
@@ -7765,7 +7767,7 @@
         <v>148</v>
       </c>
       <c r="D83" s="40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E83" s="40" t="s">
         <v>32</v>
@@ -7777,7 +7779,7 @@
         <v>32</v>
       </c>
       <c r="H83" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I83" s="41">
         <v>99</v>
@@ -7792,18 +7794,18 @@
         <v>1</v>
       </c>
       <c r="M83" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N83" s="41" t="s">
         <v>18</v>
       </c>
       <c r="O83" s="40" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B84" s="40" t="s">
         <v>124</v>
@@ -7812,7 +7814,7 @@
         <v>148</v>
       </c>
       <c r="D84" s="40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E84" s="40" t="s">
         <v>32</v>
@@ -7824,7 +7826,7 @@
         <v>32</v>
       </c>
       <c r="H84" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I84" s="41">
         <v>50</v>
@@ -7839,18 +7841,18 @@
         <v>3</v>
       </c>
       <c r="M84" s="41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N84" s="41" t="s">
         <v>22</v>
       </c>
       <c r="O84" s="40" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B85" s="40" t="s">
         <v>124</v>
@@ -7859,7 +7861,7 @@
         <v>148</v>
       </c>
       <c r="D85" s="40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E85" s="40" t="s">
         <v>32</v>
@@ -7871,7 +7873,7 @@
         <v>32</v>
       </c>
       <c r="H85" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I85" s="41">
         <v>0</v>
@@ -7886,16 +7888,16 @@
         <v>5</v>
       </c>
       <c r="M85" s="41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N85" s="41" t="s">
         <v>20</v>
       </c>
       <c r="O85" s="40" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="40" t="s">
         <v>15</v>
       </c>
@@ -7903,7 +7905,7 @@
         <v>142</v>
       </c>
       <c r="D86" s="40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E86" s="40" t="s">
         <v>32</v>
@@ -7915,7 +7917,7 @@
         <v>32</v>
       </c>
       <c r="H86" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I86" s="41" t="s">
         <v>24</v>
@@ -7930,7 +7932,7 @@
         <v>1</v>
       </c>
       <c r="M86" s="41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N86" s="41" t="s">
         <v>32</v>
@@ -7939,7 +7941,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="40" t="s">
         <v>15</v>
       </c>
@@ -7947,7 +7949,7 @@
         <v>142</v>
       </c>
       <c r="D87" s="40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E87" s="40" t="s">
         <v>32</v>
@@ -7959,7 +7961,7 @@
         <v>32</v>
       </c>
       <c r="H87" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I87" s="41" t="s">
         <v>28</v>
@@ -7974,7 +7976,7 @@
         <v>3</v>
       </c>
       <c r="M87" s="41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N87" s="41" t="s">
         <v>32</v>
@@ -7983,7 +7985,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="40" t="s">
         <v>15</v>
       </c>
@@ -7991,7 +7993,7 @@
         <v>142</v>
       </c>
       <c r="D88" s="40" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E88" s="40" t="s">
         <v>32</v>
@@ -8003,7 +8005,7 @@
         <v>32</v>
       </c>
       <c r="H88" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I88" s="41" t="s">
         <v>31</v>
@@ -8027,7 +8029,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -8035,10 +8037,10 @@
         <v>142</v>
       </c>
       <c r="C89" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D89" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E89" t="s">
         <v>32</v>
@@ -8050,7 +8052,7 @@
         <v>32</v>
       </c>
       <c r="H89" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I89" s="3" t="s">
         <v>32</v>
@@ -8074,7 +8076,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>36</v>
       </c>
@@ -8082,10 +8084,10 @@
         <v>142</v>
       </c>
       <c r="C90" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D90" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E90" t="s">
         <v>32</v>
@@ -8097,7 +8099,7 @@
         <v>32</v>
       </c>
       <c r="H90" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I90" s="3">
         <v>1</v>
@@ -8121,7 +8123,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>36</v>
       </c>
@@ -8129,10 +8131,10 @@
         <v>142</v>
       </c>
       <c r="C91" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D91" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E91" t="s">
         <v>32</v>
@@ -8144,7 +8146,7 @@
         <v>32</v>
       </c>
       <c r="H91" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I91" s="3">
         <v>2</v>
@@ -8168,7 +8170,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>36</v>
       </c>
@@ -8176,10 +8178,10 @@
         <v>142</v>
       </c>
       <c r="C92" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D92" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E92" t="s">
         <v>32</v>
@@ -8191,7 +8193,7 @@
         <v>32</v>
       </c>
       <c r="H92" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I92" s="3" t="s">
         <v>51</v>
@@ -8215,7 +8217,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="93" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>36</v>
       </c>
@@ -8223,10 +8225,10 @@
         <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D93" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E93" t="s">
         <v>32</v>
@@ -8238,7 +8240,7 @@
         <v>32</v>
       </c>
       <c r="H93" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I93" s="3" t="s">
         <v>56</v>
@@ -8262,7 +8264,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>36</v>
       </c>
@@ -8270,10 +8272,10 @@
         <v>142</v>
       </c>
       <c r="C94" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D94" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E94" t="s">
         <v>32</v>
@@ -8285,7 +8287,7 @@
         <v>32</v>
       </c>
       <c r="H94" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I94" s="3" t="s">
         <v>59</v>
@@ -8309,7 +8311,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>36</v>
       </c>
@@ -8317,10 +8319,10 @@
         <v>142</v>
       </c>
       <c r="C95" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D95" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E95" t="s">
         <v>32</v>
@@ -8332,7 +8334,7 @@
         <v>32</v>
       </c>
       <c r="H95" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I95" s="3">
         <v>5</v>
@@ -8356,7 +8358,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -8367,7 +8369,7 @@
         <v>144</v>
       </c>
       <c r="D96" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E96" t="s">
         <v>32</v>
@@ -8379,7 +8381,7 @@
         <v>32</v>
       </c>
       <c r="H96" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>20</v>
@@ -8403,7 +8405,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -8414,7 +8416,7 @@
         <v>144</v>
       </c>
       <c r="D97" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E97" t="s">
         <v>32</v>
@@ -8426,7 +8428,7 @@
         <v>32</v>
       </c>
       <c r="H97" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>22</v>
@@ -8450,7 +8452,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -8461,7 +8463,7 @@
         <v>144</v>
       </c>
       <c r="D98" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E98" t="s">
         <v>32</v>
@@ -8473,7 +8475,7 @@
         <v>32</v>
       </c>
       <c r="H98" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>18</v>
@@ -8497,7 +8499,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -8508,7 +8510,7 @@
         <v>144</v>
       </c>
       <c r="D99" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E99" t="s">
         <v>32</v>
@@ -8520,7 +8522,7 @@
         <v>32</v>
       </c>
       <c r="H99" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>32</v>
@@ -8544,18 +8546,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B100" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C100" t="s">
         <v>144</v>
       </c>
       <c r="D100" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E100" t="s">
         <v>32</v>
@@ -8567,7 +8569,7 @@
         <v>32</v>
       </c>
       <c r="H100" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I100" s="3" t="s">
         <v>32</v>
@@ -8591,7 +8593,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -8602,7 +8604,7 @@
         <v>144</v>
       </c>
       <c r="D101" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E101" t="s">
         <v>32</v>
@@ -8614,7 +8616,7 @@
         <v>32</v>
       </c>
       <c r="H101" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I101">
         <v>1</v>
@@ -8635,10 +8637,10 @@
         <v>32</v>
       </c>
       <c r="O101" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -8649,7 +8651,7 @@
         <v>144</v>
       </c>
       <c r="D102" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E102" t="s">
         <v>32</v>
@@ -8661,7 +8663,7 @@
         <v>32</v>
       </c>
       <c r="H102" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I102">
         <v>3</v>
@@ -8682,10 +8684,10 @@
         <v>32</v>
       </c>
       <c r="O102" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -8696,7 +8698,7 @@
         <v>144</v>
       </c>
       <c r="D103" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E103" t="s">
         <v>32</v>
@@ -8708,7 +8710,7 @@
         <v>32</v>
       </c>
       <c r="H103" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I103">
         <v>5</v>
@@ -8729,10 +8731,10 @@
         <v>32</v>
       </c>
       <c r="O103" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>7</v>
       </c>
@@ -8743,45 +8745,45 @@
         <v>144</v>
       </c>
       <c r="D104" t="s">
+        <v>195</v>
+      </c>
+      <c r="E104" t="s">
+        <v>32</v>
+      </c>
+      <c r="F104" t="s">
+        <v>32</v>
+      </c>
+      <c r="G104" t="s">
+        <v>32</v>
+      </c>
+      <c r="H104" t="s">
+        <v>176</v>
+      </c>
+      <c r="I104" t="s">
+        <v>32</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L104" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="M104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O104" t="s">
         <v>196</v>
       </c>
-      <c r="E104" t="s">
-        <v>32</v>
-      </c>
-      <c r="F104" t="s">
-        <v>32</v>
-      </c>
-      <c r="G104" t="s">
-        <v>32</v>
-      </c>
-      <c r="H104" t="s">
-        <v>177</v>
-      </c>
-      <c r="I104" t="s">
-        <v>32</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L104" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="M104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O104" t="s">
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>198</v>
       </c>
       <c r="B105" t="s">
         <v>136</v>
@@ -8790,7 +8792,7 @@
         <v>144</v>
       </c>
       <c r="D105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E105" t="s">
         <v>32</v>
@@ -8802,7 +8804,7 @@
         <v>32</v>
       </c>
       <c r="H105" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I105" s="2">
         <v>3</v>
@@ -8817,7 +8819,7 @@
         <v>5</v>
       </c>
       <c r="M105" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N105" s="2" t="s">
         <v>20</v>
@@ -8826,9 +8828,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B106" t="s">
         <v>136</v>
@@ -8837,7 +8839,7 @@
         <v>144</v>
       </c>
       <c r="D106" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E106" t="s">
         <v>32</v>
@@ -8849,7 +8851,7 @@
         <v>32</v>
       </c>
       <c r="H106" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I106" s="2">
         <v>2</v>
@@ -8864,7 +8866,7 @@
         <v>3</v>
       </c>
       <c r="M106" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N106" s="2" t="s">
         <v>22</v>
@@ -8873,9 +8875,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B107" t="s">
         <v>136</v>
@@ -8884,7 +8886,7 @@
         <v>144</v>
       </c>
       <c r="D107" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E107" t="s">
         <v>32</v>
@@ -8896,7 +8898,7 @@
         <v>32</v>
       </c>
       <c r="H107" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I107" s="2">
         <v>1</v>
@@ -8911,7 +8913,7 @@
         <v>1</v>
       </c>
       <c r="M107" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N107" s="2" t="s">
         <v>18</v>
@@ -8920,9 +8922,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B108" t="s">
         <v>136</v>
@@ -8931,7 +8933,7 @@
         <v>144</v>
       </c>
       <c r="D108" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E108" t="s">
         <v>32</v>
@@ -8943,7 +8945,7 @@
         <v>32</v>
       </c>
       <c r="H108" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I108" s="2">
         <v>0</v>
@@ -8958,7 +8960,7 @@
         <v>32</v>
       </c>
       <c r="M108" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N108" s="2" t="s">
         <v>32</v>
@@ -8967,19 +8969,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
+        <v>208</v>
+      </c>
+      <c r="B109" t="s">
         <v>209</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>210</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>211</v>
       </c>
-      <c r="D109" t="s">
-        <v>212</v>
-      </c>
       <c r="E109" t="s">
         <v>32</v>
       </c>
@@ -8990,7 +8992,7 @@
         <v>32</v>
       </c>
       <c r="H109" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I109" s="2">
         <v>0</v>
@@ -9005,28 +9007,28 @@
         <v>5</v>
       </c>
       <c r="M109" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N109" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O109" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>208</v>
+      </c>
+      <c r="B110" t="s">
         <v>209</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>210</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="s">
         <v>211</v>
       </c>
-      <c r="D110" t="s">
-        <v>212</v>
-      </c>
       <c r="E110" t="s">
         <v>32</v>
       </c>
@@ -9037,7 +9039,7 @@
         <v>32</v>
       </c>
       <c r="H110" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I110" s="2">
         <v>0.01</v>
@@ -9052,28 +9054,28 @@
         <v>3</v>
       </c>
       <c r="M110" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N110" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O110" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
+        <v>208</v>
+      </c>
+      <c r="B111" t="s">
         <v>209</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>210</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
         <v>211</v>
       </c>
-      <c r="D111" t="s">
-        <v>212</v>
-      </c>
       <c r="E111" t="s">
         <v>32</v>
       </c>
@@ -9084,7 +9086,7 @@
         <v>32</v>
       </c>
       <c r="H111" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I111" s="2">
         <v>0.5</v>
@@ -9099,31 +9101,17 @@
         <v>1</v>
       </c>
       <c r="M111" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N111" s="2" t="s">
         <v>18</v>
       </c>
       <c r="O111" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O111" xr:uid="{964DF2B0-6B32-465A-9085-889E032C36AD}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Temperature- Rearing"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters>
-        <filter val="NORWEST_Temperature"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O100">
-      <sortCondition descending="1" ref="H1:H100"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:O111" xr:uid="{E0FD6E8C-F414-4D9F-82CB-33D09B6D4DCD}"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="O74" r:id="rId1" xr:uid="{3DD1971B-CBAE-41F4-A49E-E6B715DE820C}"/>

</xml_diff>

<commit_message>
Various updates to the R Code
</commit_message>
<xml_diff>
--- a/Data/Criteria_and_Scoring/Habitat_Limiting_Factor_Rating_Criteria.xlsx
+++ b/Data/Criteria_and_Scoring/Habitat_Limiting_Factor_Rating_Criteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817915E2-1E8F-416D-8660-8838B6E40127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13924116-6A7A-47D1-9F98-FED74797B728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="1224" windowWidth="20244" windowHeight="10896" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
+    <workbookView xWindow="1620" yWindow="1308" windowWidth="20340" windowHeight="10620" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -547,9 +547,6 @@
     <t>Pool Quantity &amp; Quality</t>
   </si>
   <si>
-    <t>Pool_Habitat_Prcnt_INDICATOR_4</t>
-  </si>
-  <si>
     <t>Pools_per_mile_INDICATOR_2</t>
   </si>
   <si>
@@ -710,6 +707,9 @@
   </si>
   <si>
     <t>no pools are &gt;3ft (or 5 ft for 5 ft deep pools indicator)</t>
+  </si>
+  <si>
+    <t>Pool_Habitat_Prcnt_INDICATOR_4,EDT_Scour Pool pct</t>
   </si>
 </sst>
 </file>
@@ -3808,12 +3808,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FD6E8C-F414-4D9F-82CB-33D09B6D4DCD}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:O111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3844,22 +3845,22 @@
         <v>126</v>
       </c>
       <c r="F1" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="G1" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="38" t="s">
-        <v>181</v>
-      </c>
       <c r="H1" s="38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I1" s="38" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1" s="38" t="s">
         <v>178</v>
-      </c>
-      <c r="K1" s="38" t="s">
-        <v>179</v>
       </c>
       <c r="L1" s="39" t="s">
         <v>10</v>
@@ -3874,7 +3875,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -3897,7 +3898,7 @@
         <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I2" s="2">
         <v>0</v>
@@ -3922,7 +3923,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -3945,7 +3946,7 @@
         <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I3" s="2">
         <v>1.4</v>
@@ -3970,7 +3971,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -3993,7 +3994,7 @@
         <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I4" s="2">
         <v>2.2000000000000002</v>
@@ -4018,7 +4019,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -4041,7 +4042,7 @@
         <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -4066,7 +4067,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -4089,7 +4090,7 @@
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -4113,7 +4114,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>95</v>
       </c>
@@ -4136,7 +4137,7 @@
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I7" s="2">
         <v>20</v>
@@ -4161,7 +4162,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -4184,7 +4185,7 @@
         <v>100000</v>
       </c>
       <c r="H8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -4209,7 +4210,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -4232,7 +4233,7 @@
         <v>100000</v>
       </c>
       <c r="H9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I9" s="2">
         <v>17</v>
@@ -4257,7 +4258,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -4280,7 +4281,7 @@
         <v>100000</v>
       </c>
       <c r="H10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I10" s="2">
         <v>70</v>
@@ -4305,7 +4306,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -4328,7 +4329,7 @@
         <v>32</v>
       </c>
       <c r="H11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -4353,7 +4354,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -4376,7 +4377,7 @@
         <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I12" s="2">
         <v>2</v>
@@ -4401,7 +4402,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -4424,7 +4425,7 @@
         <v>32</v>
       </c>
       <c r="H13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I13" s="2">
         <v>5</v>
@@ -4457,11 +4458,11 @@
         <v>140</v>
       </c>
       <c r="C14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D14" t="s">
         <v>165</v>
       </c>
-      <c r="D14" t="s">
-        <v>166</v>
-      </c>
       <c r="E14" t="s">
         <v>32</v>
       </c>
@@ -4472,7 +4473,7 @@
         <v>32</v>
       </c>
       <c r="H14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -4505,11 +4506,11 @@
         <v>140</v>
       </c>
       <c r="C15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" t="s">
         <v>165</v>
       </c>
-      <c r="D15" t="s">
-        <v>166</v>
-      </c>
       <c r="E15" t="s">
         <v>32</v>
       </c>
@@ -4520,7 +4521,7 @@
         <v>32</v>
       </c>
       <c r="H15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I15" s="2">
         <v>0.1</v>
@@ -4552,11 +4553,11 @@
         <v>140</v>
       </c>
       <c r="C16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" t="s">
         <v>165</v>
       </c>
-      <c r="D16" t="s">
-        <v>166</v>
-      </c>
       <c r="E16" t="s">
         <v>32</v>
       </c>
@@ -4567,7 +4568,7 @@
         <v>32</v>
       </c>
       <c r="H16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I16" s="2">
         <v>20</v>
@@ -4600,10 +4601,10 @@
         <v>140</v>
       </c>
       <c r="C17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E17" t="s">
         <v>32</v>
@@ -4615,7 +4616,7 @@
         <v>32</v>
       </c>
       <c r="H17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I17" s="2">
         <v>0</v>
@@ -4631,7 +4632,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>18</v>
@@ -4648,10 +4649,10 @@
         <v>140</v>
       </c>
       <c r="C18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -4663,7 +4664,7 @@
         <v>32</v>
       </c>
       <c r="H18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I18" s="2">
         <v>0.1</v>
@@ -4696,10 +4697,10 @@
         <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E19" t="s">
         <v>32</v>
@@ -4711,7 +4712,7 @@
         <v>32</v>
       </c>
       <c r="H19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I19" s="2">
         <v>5</v>
@@ -4736,7 +4737,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="36" t="s">
         <v>54</v>
       </c>
@@ -4751,7 +4752,7 @@
       <c r="F20" s="36"/>
       <c r="G20" s="36"/>
       <c r="H20" s="36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I20" s="37">
         <v>0</v>
@@ -4777,7 +4778,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="36" t="s">
         <v>54</v>
       </c>
@@ -4792,7 +4793,7 @@
       <c r="F21" s="36"/>
       <c r="G21" s="36"/>
       <c r="H21" s="36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I21" s="37">
         <v>5</v>
@@ -4818,7 +4819,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36" t="s">
         <v>54</v>
       </c>
@@ -4833,7 +4834,7 @@
       <c r="F22" s="36"/>
       <c r="G22" s="36"/>
       <c r="H22" s="36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I22" s="37">
         <v>20</v>
@@ -4870,7 +4871,7 @@
         <v>162</v>
       </c>
       <c r="D23" t="s">
-        <v>163</v>
+        <v>217</v>
       </c>
       <c r="E23" t="s">
         <v>32</v>
@@ -4882,7 +4883,7 @@
         <v>32</v>
       </c>
       <c r="H23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I23" s="2">
         <v>0</v>
@@ -4918,7 +4919,7 @@
         <v>162</v>
       </c>
       <c r="D24" t="s">
-        <v>163</v>
+        <v>217</v>
       </c>
       <c r="E24" t="s">
         <v>32</v>
@@ -4930,7 +4931,7 @@
         <v>32</v>
       </c>
       <c r="H24" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I24" s="2">
         <v>10</v>
@@ -4966,7 +4967,7 @@
         <v>162</v>
       </c>
       <c r="D25" t="s">
-        <v>163</v>
+        <v>217</v>
       </c>
       <c r="E25" t="s">
         <v>32</v>
@@ -4978,7 +4979,7 @@
         <v>32</v>
       </c>
       <c r="H25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I25" s="2">
         <v>20</v>
@@ -5014,7 +5015,7 @@
         <v>162</v>
       </c>
       <c r="D26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E26" t="s">
         <v>86</v>
@@ -5027,7 +5028,7 @@
         <v>1.524</v>
       </c>
       <c r="H26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I26" s="2">
         <v>0</v>
@@ -5063,7 +5064,7 @@
         <v>162</v>
       </c>
       <c r="D27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E27" t="s">
         <v>86</v>
@@ -5076,7 +5077,7 @@
         <v>1.524</v>
       </c>
       <c r="H27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I27" s="2">
         <v>184</v>
@@ -5112,7 +5113,7 @@
         <v>162</v>
       </c>
       <c r="D28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E28" t="s">
         <v>86</v>
@@ -5125,7 +5126,7 @@
         <v>1.524</v>
       </c>
       <c r="H28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>32</v>
@@ -5161,7 +5162,7 @@
         <v>162</v>
       </c>
       <c r="D29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E29" t="s">
         <v>93</v>
@@ -5175,7 +5176,7 @@
         <v>3.048</v>
       </c>
       <c r="H29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I29" s="2">
         <v>0</v>
@@ -5211,7 +5212,7 @@
         <v>162</v>
       </c>
       <c r="D30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E30" t="s">
         <v>93</v>
@@ -5225,7 +5226,7 @@
         <v>3.048</v>
       </c>
       <c r="H30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I30" s="2">
         <v>95</v>
@@ -5261,7 +5262,7 @@
         <v>162</v>
       </c>
       <c r="D31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E31" t="s">
         <v>93</v>
@@ -5275,7 +5276,7 @@
         <v>3.048</v>
       </c>
       <c r="H31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>32</v>
@@ -5309,7 +5310,7 @@
         <v>162</v>
       </c>
       <c r="D32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E32" t="s">
         <v>98</v>
@@ -5323,7 +5324,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H32" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I32" s="2">
         <v>0</v>
@@ -5359,7 +5360,7 @@
         <v>162</v>
       </c>
       <c r="D33" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E33" t="s">
         <v>98</v>
@@ -5373,7 +5374,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H33" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I33" s="2">
         <v>70</v>
@@ -5409,7 +5410,7 @@
         <v>162</v>
       </c>
       <c r="D34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E34" t="s">
         <v>98</v>
@@ -5423,7 +5424,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>32</v>
@@ -5459,7 +5460,7 @@
         <v>162</v>
       </c>
       <c r="D35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E35" t="s">
         <v>102</v>
@@ -5473,7 +5474,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
@@ -5509,7 +5510,7 @@
         <v>162</v>
       </c>
       <c r="D36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E36" t="s">
         <v>102</v>
@@ -5523,7 +5524,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I36" s="2">
         <v>55</v>
@@ -5559,7 +5560,7 @@
         <v>162</v>
       </c>
       <c r="D37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E37" t="s">
         <v>102</v>
@@ -5573,7 +5574,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H37" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>32</v>
@@ -5609,7 +5610,7 @@
         <v>162</v>
       </c>
       <c r="D38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E38" t="s">
         <v>107</v>
@@ -5623,7 +5624,7 @@
         <v>7.62</v>
       </c>
       <c r="H38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I38" s="2">
         <v>0</v>
@@ -5659,7 +5660,7 @@
         <v>162</v>
       </c>
       <c r="D39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E39" t="s">
         <v>107</v>
@@ -5673,7 +5674,7 @@
         <v>7.62</v>
       </c>
       <c r="H39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I39" s="2">
         <v>47</v>
@@ -5709,7 +5710,7 @@
         <v>162</v>
       </c>
       <c r="D40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E40" t="s">
         <v>107</v>
@@ -5723,7 +5724,7 @@
         <v>7.62</v>
       </c>
       <c r="H40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>32</v>
@@ -5759,7 +5760,7 @@
         <v>162</v>
       </c>
       <c r="D41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E41" t="s">
         <v>113</v>
@@ -5773,7 +5774,7 @@
         <v>15.24</v>
       </c>
       <c r="H41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I41" s="2">
         <v>0</v>
@@ -5809,7 +5810,7 @@
         <v>162</v>
       </c>
       <c r="D42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E42" t="s">
         <v>113</v>
@@ -5823,7 +5824,7 @@
         <v>15.24</v>
       </c>
       <c r="H42" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I42" s="2">
         <v>25</v>
@@ -5859,7 +5860,7 @@
         <v>162</v>
       </c>
       <c r="D43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E43" t="s">
         <v>113</v>
@@ -5873,7 +5874,7 @@
         <v>15.24</v>
       </c>
       <c r="H43" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>32</v>
@@ -5909,7 +5910,7 @@
         <v>162</v>
       </c>
       <c r="D44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E44" t="s">
         <v>116</v>
@@ -5923,7 +5924,7 @@
         <v>22.86</v>
       </c>
       <c r="H44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I44" s="2">
         <v>0</v>
@@ -5959,7 +5960,7 @@
         <v>162</v>
       </c>
       <c r="D45" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E45" t="s">
         <v>116</v>
@@ -5973,7 +5974,7 @@
         <v>22.86</v>
       </c>
       <c r="H45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I45" s="2">
         <v>23</v>
@@ -6009,7 +6010,7 @@
         <v>162</v>
       </c>
       <c r="D46" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E46" t="s">
         <v>116</v>
@@ -6023,7 +6024,7 @@
         <v>22.86</v>
       </c>
       <c r="H46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>32</v>
@@ -6059,7 +6060,7 @@
         <v>162</v>
       </c>
       <c r="D47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E47" t="s">
         <v>119</v>
@@ -6072,7 +6073,7 @@
         <v>100000</v>
       </c>
       <c r="H47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I47" s="2">
         <v>0</v>
@@ -6108,7 +6109,7 @@
         <v>162</v>
       </c>
       <c r="D48" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E48" t="s">
         <v>119</v>
@@ -6121,7 +6122,7 @@
         <v>100000</v>
       </c>
       <c r="H48" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I48" s="2">
         <v>18</v>
@@ -6157,7 +6158,7 @@
         <v>162</v>
       </c>
       <c r="D49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E49" t="s">
         <v>119</v>
@@ -6170,7 +6171,7 @@
         <v>100000</v>
       </c>
       <c r="H49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>32</v>
@@ -6195,24 +6196,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B50" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E50" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H50" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I50" s="41">
         <v>0</v>
@@ -6238,24 +6239,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B51" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D51" s="40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E51" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H51" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I51" s="41">
         <v>50</v>
@@ -6280,24 +6281,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B52" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E52" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H52" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I52" s="41">
         <v>80</v>
@@ -6322,7 +6323,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -6345,7 +6346,7 @@
         <v>32</v>
       </c>
       <c r="H53" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I53" s="2">
         <v>0</v>
@@ -6370,7 +6371,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -6393,7 +6394,7 @@
         <v>32</v>
       </c>
       <c r="H54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I54" s="2">
         <v>2</v>
@@ -6418,7 +6419,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -6441,7 +6442,7 @@
         <v>32</v>
       </c>
       <c r="H55" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I55" s="2">
         <v>5</v>
@@ -6466,7 +6467,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -6489,7 +6490,7 @@
         <v>32</v>
       </c>
       <c r="H56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I56" s="2">
         <v>-5</v>
@@ -6513,7 +6514,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -6536,7 +6537,7 @@
         <v>32</v>
       </c>
       <c r="H57" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I57" s="2">
         <v>1</v>
@@ -6560,7 +6561,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -6583,7 +6584,7 @@
         <v>32</v>
       </c>
       <c r="H58" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I58" s="2">
         <v>4</v>
@@ -6607,7 +6608,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -6630,7 +6631,7 @@
         <v>32</v>
       </c>
       <c r="H59" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I59" s="2">
         <v>0</v>
@@ -6645,7 +6646,7 @@
         <v>1</v>
       </c>
       <c r="M59" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>18</v>
@@ -6654,7 +6655,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -6677,7 +6678,7 @@
         <v>32</v>
       </c>
       <c r="H60" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I60" s="2">
         <v>2</v>
@@ -6702,7 +6703,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -6725,7 +6726,7 @@
         <v>32</v>
       </c>
       <c r="H61" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I61" s="2">
         <v>5</v>
@@ -6750,7 +6751,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>37</v>
       </c>
@@ -6761,7 +6762,7 @@
         <v>148</v>
       </c>
       <c r="D62" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E62" t="s">
         <v>32</v>
@@ -6773,7 +6774,7 @@
         <v>32</v>
       </c>
       <c r="H62" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I62" s="2">
         <v>0</v>
@@ -6797,7 +6798,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>37</v>
       </c>
@@ -6808,7 +6809,7 @@
         <v>148</v>
       </c>
       <c r="D63" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E63" t="s">
         <v>32</v>
@@ -6820,7 +6821,7 @@
         <v>32</v>
       </c>
       <c r="H63" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I63" s="2">
         <v>1</v>
@@ -6844,7 +6845,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -6855,7 +6856,7 @@
         <v>148</v>
       </c>
       <c r="D64" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E64" t="s">
         <v>32</v>
@@ -6867,7 +6868,7 @@
         <v>32</v>
       </c>
       <c r="H64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I64" s="2">
         <v>50</v>
@@ -6892,7 +6893,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>58</v>
       </c>
@@ -6915,7 +6916,7 @@
         <v>32</v>
       </c>
       <c r="H65" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I65" s="2">
         <v>0</v>
@@ -6939,7 +6940,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>58</v>
       </c>
@@ -6962,7 +6963,7 @@
         <v>32</v>
       </c>
       <c r="H66" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I66" s="2">
         <v>12</v>
@@ -6987,7 +6988,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>58</v>
       </c>
@@ -7010,7 +7011,7 @@
         <v>32</v>
       </c>
       <c r="H67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I67" s="2">
         <v>20</v>
@@ -7035,7 +7036,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="40" t="s">
         <v>73</v>
       </c>
@@ -7058,7 +7059,7 @@
         <v>32</v>
       </c>
       <c r="H68" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I68" s="41">
         <v>0</v>
@@ -7082,7 +7083,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="40" t="s">
         <v>73</v>
       </c>
@@ -7105,7 +7106,7 @@
         <v>32</v>
       </c>
       <c r="H69" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I69" s="41">
         <v>10</v>
@@ -7130,7 +7131,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="40" t="s">
         <v>73</v>
       </c>
@@ -7153,7 +7154,7 @@
         <v>32</v>
       </c>
       <c r="H70" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I70" s="41">
         <v>20</v>
@@ -7178,7 +7179,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="40" t="s">
         <v>85</v>
       </c>
@@ -7189,7 +7190,7 @@
         <v>148</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E71" s="40" t="s">
         <v>32</v>
@@ -7201,7 +7202,7 @@
         <v>32</v>
       </c>
       <c r="H71" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I71" s="41">
         <v>0</v>
@@ -7225,7 +7226,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="40" t="s">
         <v>85</v>
       </c>
@@ -7236,7 +7237,7 @@
         <v>148</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E72" s="40" t="s">
         <v>32</v>
@@ -7248,7 +7249,7 @@
         <v>32</v>
       </c>
       <c r="H72" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I72" s="41">
         <v>15</v>
@@ -7273,7 +7274,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="40" t="s">
         <v>85</v>
       </c>
@@ -7284,7 +7285,7 @@
         <v>148</v>
       </c>
       <c r="D73" s="40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E73" s="40" t="s">
         <v>32</v>
@@ -7296,7 +7297,7 @@
         <v>32</v>
       </c>
       <c r="H73" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I73" s="41">
         <v>30</v>
@@ -7321,7 +7322,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="40" t="s">
         <v>14</v>
       </c>
@@ -7329,11 +7330,11 @@
         <v>141</v>
       </c>
       <c r="C74" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="D74" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="D74" s="40" t="s">
-        <v>168</v>
-      </c>
       <c r="E74" s="40" t="s">
         <v>32</v>
       </c>
@@ -7344,7 +7345,7 @@
         <v>32</v>
       </c>
       <c r="H74" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I74" s="41">
         <v>0</v>
@@ -7370,7 +7371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="40" t="s">
         <v>14</v>
       </c>
@@ -7378,11 +7379,11 @@
         <v>141</v>
       </c>
       <c r="C75" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="D75" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="D75" s="40" t="s">
-        <v>168</v>
-      </c>
       <c r="E75" s="40" t="s">
         <v>32</v>
       </c>
@@ -7393,7 +7394,7 @@
         <v>32</v>
       </c>
       <c r="H75" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I75" s="41">
         <v>12</v>
@@ -7419,7 +7420,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="40" t="s">
         <v>14</v>
       </c>
@@ -7427,11 +7428,11 @@
         <v>141</v>
       </c>
       <c r="C76" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="D76" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="D76" s="40" t="s">
-        <v>168</v>
-      </c>
       <c r="E76" s="40" t="s">
         <v>32</v>
       </c>
@@ -7442,7 +7443,7 @@
         <v>32</v>
       </c>
       <c r="H76" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I76" s="41">
         <v>14</v>
@@ -7468,7 +7469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="40" t="s">
         <v>35</v>
       </c>
@@ -7476,10 +7477,10 @@
         <v>141</v>
       </c>
       <c r="C77" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D77" s="40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E77" s="40" t="s">
         <v>32</v>
@@ -7491,7 +7492,7 @@
         <v>32</v>
       </c>
       <c r="H77" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I77" s="41">
         <v>0</v>
@@ -7516,7 +7517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="40" t="s">
         <v>35</v>
       </c>
@@ -7524,10 +7525,10 @@
         <v>141</v>
       </c>
       <c r="C78" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D78" s="40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E78" s="40" t="s">
         <v>32</v>
@@ -7539,7 +7540,7 @@
         <v>32</v>
       </c>
       <c r="H78" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I78" s="41">
         <v>10</v>
@@ -7564,7 +7565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="40" t="s">
         <v>35</v>
       </c>
@@ -7572,10 +7573,10 @@
         <v>141</v>
       </c>
       <c r="C79" s="40" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D79" s="40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E79" s="40" t="s">
         <v>32</v>
@@ -7587,7 +7588,7 @@
         <v>32</v>
       </c>
       <c r="H79" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I79" s="41">
         <v>14</v>
@@ -7612,7 +7613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="40" t="s">
         <v>55</v>
       </c>
@@ -7620,10 +7621,10 @@
         <v>141</v>
       </c>
       <c r="C80" s="40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D80" s="40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E80" s="40" t="s">
         <v>32</v>
@@ -7635,7 +7636,7 @@
         <v>32</v>
       </c>
       <c r="H80" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I80" s="41">
         <v>0</v>
@@ -7651,7 +7652,7 @@
         <v>5</v>
       </c>
       <c r="M80" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N80" s="41" t="s">
         <v>20</v>
@@ -7660,7 +7661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="40" t="s">
         <v>55</v>
       </c>
@@ -7668,10 +7669,10 @@
         <v>141</v>
       </c>
       <c r="C81" s="40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D81" s="40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E81" s="40" t="s">
         <v>32</v>
@@ -7683,7 +7684,7 @@
         <v>32</v>
       </c>
       <c r="H81" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I81" s="41">
         <v>16</v>
@@ -7699,7 +7700,7 @@
         <v>3</v>
       </c>
       <c r="M81" s="41" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N81" s="41" t="s">
         <v>22</v>
@@ -7708,7 +7709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="40" t="s">
         <v>55</v>
       </c>
@@ -7716,10 +7717,10 @@
         <v>141</v>
       </c>
       <c r="C82" s="40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D82" s="40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E82" s="40" t="s">
         <v>32</v>
@@ -7731,7 +7732,7 @@
         <v>32</v>
       </c>
       <c r="H82" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I82" s="41">
         <v>22</v>
@@ -7747,7 +7748,7 @@
         <v>1</v>
       </c>
       <c r="M82" s="41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N82" s="41" t="s">
         <v>18</v>
@@ -7756,9 +7757,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B83" s="40" t="s">
         <v>124</v>
@@ -7767,7 +7768,7 @@
         <v>148</v>
       </c>
       <c r="D83" s="40" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E83" s="40" t="s">
         <v>32</v>
@@ -7779,7 +7780,7 @@
         <v>32</v>
       </c>
       <c r="H83" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I83" s="41">
         <v>99</v>
@@ -7794,18 +7795,18 @@
         <v>1</v>
       </c>
       <c r="M83" s="41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N83" s="41" t="s">
         <v>18</v>
       </c>
       <c r="O83" s="40" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B84" s="40" t="s">
         <v>124</v>
@@ -7814,7 +7815,7 @@
         <v>148</v>
       </c>
       <c r="D84" s="40" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E84" s="40" t="s">
         <v>32</v>
@@ -7826,7 +7827,7 @@
         <v>32</v>
       </c>
       <c r="H84" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I84" s="41">
         <v>50</v>
@@ -7841,18 +7842,18 @@
         <v>3</v>
       </c>
       <c r="M84" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N84" s="41" t="s">
         <v>22</v>
       </c>
       <c r="O84" s="40" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B85" s="40" t="s">
         <v>124</v>
@@ -7861,7 +7862,7 @@
         <v>148</v>
       </c>
       <c r="D85" s="40" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E85" s="40" t="s">
         <v>32</v>
@@ -7873,7 +7874,7 @@
         <v>32</v>
       </c>
       <c r="H85" s="40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I85" s="41">
         <v>0</v>
@@ -7888,16 +7889,16 @@
         <v>5</v>
       </c>
       <c r="M85" s="41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N85" s="41" t="s">
         <v>20</v>
       </c>
       <c r="O85" s="40" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="40" t="s">
         <v>15</v>
       </c>
@@ -7905,7 +7906,7 @@
         <v>142</v>
       </c>
       <c r="D86" s="40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E86" s="40" t="s">
         <v>32</v>
@@ -7917,7 +7918,7 @@
         <v>32</v>
       </c>
       <c r="H86" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I86" s="41" t="s">
         <v>24</v>
@@ -7932,7 +7933,7 @@
         <v>1</v>
       </c>
       <c r="M86" s="41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N86" s="41" t="s">
         <v>32</v>
@@ -7941,7 +7942,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="40" t="s">
         <v>15</v>
       </c>
@@ -7949,7 +7950,7 @@
         <v>142</v>
       </c>
       <c r="D87" s="40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E87" s="40" t="s">
         <v>32</v>
@@ -7961,7 +7962,7 @@
         <v>32</v>
       </c>
       <c r="H87" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I87" s="41" t="s">
         <v>28</v>
@@ -7976,7 +7977,7 @@
         <v>3</v>
       </c>
       <c r="M87" s="41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N87" s="41" t="s">
         <v>32</v>
@@ -7985,7 +7986,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="40" t="s">
         <v>15</v>
       </c>
@@ -7993,7 +7994,7 @@
         <v>142</v>
       </c>
       <c r="D88" s="40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E88" s="40" t="s">
         <v>32</v>
@@ -8005,7 +8006,7 @@
         <v>32</v>
       </c>
       <c r="H88" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I88" s="41" t="s">
         <v>31</v>
@@ -8029,7 +8030,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -8037,10 +8038,10 @@
         <v>142</v>
       </c>
       <c r="C89" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D89" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E89" t="s">
         <v>32</v>
@@ -8052,7 +8053,7 @@
         <v>32</v>
       </c>
       <c r="H89" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I89" s="3" t="s">
         <v>32</v>
@@ -8076,7 +8077,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>36</v>
       </c>
@@ -8084,10 +8085,10 @@
         <v>142</v>
       </c>
       <c r="C90" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D90" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E90" t="s">
         <v>32</v>
@@ -8099,7 +8100,7 @@
         <v>32</v>
       </c>
       <c r="H90" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I90" s="3">
         <v>1</v>
@@ -8123,7 +8124,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>36</v>
       </c>
@@ -8131,10 +8132,10 @@
         <v>142</v>
       </c>
       <c r="C91" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D91" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E91" t="s">
         <v>32</v>
@@ -8146,7 +8147,7 @@
         <v>32</v>
       </c>
       <c r="H91" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I91" s="3">
         <v>2</v>
@@ -8170,7 +8171,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>36</v>
       </c>
@@ -8178,10 +8179,10 @@
         <v>142</v>
       </c>
       <c r="C92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D92" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E92" t="s">
         <v>32</v>
@@ -8193,7 +8194,7 @@
         <v>32</v>
       </c>
       <c r="H92" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I92" s="3" t="s">
         <v>51</v>
@@ -8217,7 +8218,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="93" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>36</v>
       </c>
@@ -8225,10 +8226,10 @@
         <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D93" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E93" t="s">
         <v>32</v>
@@ -8240,7 +8241,7 @@
         <v>32</v>
       </c>
       <c r="H93" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I93" s="3" t="s">
         <v>56</v>
@@ -8264,7 +8265,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>36</v>
       </c>
@@ -8272,10 +8273,10 @@
         <v>142</v>
       </c>
       <c r="C94" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D94" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E94" t="s">
         <v>32</v>
@@ -8287,7 +8288,7 @@
         <v>32</v>
       </c>
       <c r="H94" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I94" s="3" t="s">
         <v>59</v>
@@ -8311,7 +8312,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>36</v>
       </c>
@@ -8319,10 +8320,10 @@
         <v>142</v>
       </c>
       <c r="C95" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D95" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E95" t="s">
         <v>32</v>
@@ -8334,7 +8335,7 @@
         <v>32</v>
       </c>
       <c r="H95" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I95" s="3">
         <v>5</v>
@@ -8358,7 +8359,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -8369,7 +8370,7 @@
         <v>144</v>
       </c>
       <c r="D96" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E96" t="s">
         <v>32</v>
@@ -8381,7 +8382,7 @@
         <v>32</v>
       </c>
       <c r="H96" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>20</v>
@@ -8405,7 +8406,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -8416,7 +8417,7 @@
         <v>144</v>
       </c>
       <c r="D97" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E97" t="s">
         <v>32</v>
@@ -8428,7 +8429,7 @@
         <v>32</v>
       </c>
       <c r="H97" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>22</v>
@@ -8452,7 +8453,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -8463,7 +8464,7 @@
         <v>144</v>
       </c>
       <c r="D98" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E98" t="s">
         <v>32</v>
@@ -8475,7 +8476,7 @@
         <v>32</v>
       </c>
       <c r="H98" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>18</v>
@@ -8499,7 +8500,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -8510,7 +8511,7 @@
         <v>144</v>
       </c>
       <c r="D99" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E99" t="s">
         <v>32</v>
@@ -8522,7 +8523,7 @@
         <v>32</v>
       </c>
       <c r="H99" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>32</v>
@@ -8546,18 +8547,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B100" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C100" t="s">
         <v>144</v>
       </c>
       <c r="D100" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E100" t="s">
         <v>32</v>
@@ -8569,7 +8570,7 @@
         <v>32</v>
       </c>
       <c r="H100" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I100" s="3" t="s">
         <v>32</v>
@@ -8593,7 +8594,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -8604,7 +8605,7 @@
         <v>144</v>
       </c>
       <c r="D101" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E101" t="s">
         <v>32</v>
@@ -8616,7 +8617,7 @@
         <v>32</v>
       </c>
       <c r="H101" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I101">
         <v>1</v>
@@ -8637,10 +8638,10 @@
         <v>32</v>
       </c>
       <c r="O101" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -8651,7 +8652,7 @@
         <v>144</v>
       </c>
       <c r="D102" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E102" t="s">
         <v>32</v>
@@ -8663,7 +8664,7 @@
         <v>32</v>
       </c>
       <c r="H102" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I102">
         <v>3</v>
@@ -8684,10 +8685,10 @@
         <v>32</v>
       </c>
       <c r="O102" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -8698,7 +8699,7 @@
         <v>144</v>
       </c>
       <c r="D103" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E103" t="s">
         <v>32</v>
@@ -8710,7 +8711,7 @@
         <v>32</v>
       </c>
       <c r="H103" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I103">
         <v>5</v>
@@ -8731,10 +8732,10 @@
         <v>32</v>
       </c>
       <c r="O103" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>7</v>
       </c>
@@ -8745,45 +8746,45 @@
         <v>144</v>
       </c>
       <c r="D104" t="s">
+        <v>194</v>
+      </c>
+      <c r="E104" t="s">
+        <v>32</v>
+      </c>
+      <c r="F104" t="s">
+        <v>32</v>
+      </c>
+      <c r="G104" t="s">
+        <v>32</v>
+      </c>
+      <c r="H104" t="s">
+        <v>175</v>
+      </c>
+      <c r="I104" t="s">
+        <v>32</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L104" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="M104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O104" t="s">
         <v>195</v>
       </c>
-      <c r="E104" t="s">
-        <v>32</v>
-      </c>
-      <c r="F104" t="s">
-        <v>32</v>
-      </c>
-      <c r="G104" t="s">
-        <v>32</v>
-      </c>
-      <c r="H104" t="s">
-        <v>176</v>
-      </c>
-      <c r="I104" t="s">
-        <v>32</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L104" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="M104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O104" t="s">
+    </row>
+    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>197</v>
       </c>
       <c r="B105" t="s">
         <v>136</v>
@@ -8792,7 +8793,7 @@
         <v>144</v>
       </c>
       <c r="D105" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E105" t="s">
         <v>32</v>
@@ -8804,7 +8805,7 @@
         <v>32</v>
       </c>
       <c r="H105" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I105" s="2">
         <v>3</v>
@@ -8819,7 +8820,7 @@
         <v>5</v>
       </c>
       <c r="M105" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N105" s="2" t="s">
         <v>20</v>
@@ -8828,9 +8829,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B106" t="s">
         <v>136</v>
@@ -8839,7 +8840,7 @@
         <v>144</v>
       </c>
       <c r="D106" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E106" t="s">
         <v>32</v>
@@ -8851,7 +8852,7 @@
         <v>32</v>
       </c>
       <c r="H106" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I106" s="2">
         <v>2</v>
@@ -8866,7 +8867,7 @@
         <v>3</v>
       </c>
       <c r="M106" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N106" s="2" t="s">
         <v>22</v>
@@ -8875,9 +8876,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B107" t="s">
         <v>136</v>
@@ -8886,7 +8887,7 @@
         <v>144</v>
       </c>
       <c r="D107" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E107" t="s">
         <v>32</v>
@@ -8898,7 +8899,7 @@
         <v>32</v>
       </c>
       <c r="H107" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I107" s="2">
         <v>1</v>
@@ -8913,7 +8914,7 @@
         <v>1</v>
       </c>
       <c r="M107" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N107" s="2" t="s">
         <v>18</v>
@@ -8922,9 +8923,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B108" t="s">
         <v>136</v>
@@ -8933,7 +8934,7 @@
         <v>144</v>
       </c>
       <c r="D108" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E108" t="s">
         <v>32</v>
@@ -8945,7 +8946,7 @@
         <v>32</v>
       </c>
       <c r="H108" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I108" s="2">
         <v>0</v>
@@ -8960,7 +8961,7 @@
         <v>32</v>
       </c>
       <c r="M108" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N108" s="2" t="s">
         <v>32</v>
@@ -8969,19 +8970,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
+        <v>207</v>
+      </c>
+      <c r="B109" t="s">
         <v>208</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>209</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>210</v>
       </c>
-      <c r="D109" t="s">
-        <v>211</v>
-      </c>
       <c r="E109" t="s">
         <v>32</v>
       </c>
@@ -8992,7 +8993,7 @@
         <v>32</v>
       </c>
       <c r="H109" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I109" s="2">
         <v>0</v>
@@ -9007,28 +9008,28 @@
         <v>5</v>
       </c>
       <c r="M109" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N109" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O109" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>207</v>
+      </c>
+      <c r="B110" t="s">
         <v>208</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>209</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="s">
         <v>210</v>
       </c>
-      <c r="D110" t="s">
-        <v>211</v>
-      </c>
       <c r="E110" t="s">
         <v>32</v>
       </c>
@@ -9039,7 +9040,7 @@
         <v>32</v>
       </c>
       <c r="H110" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I110" s="2">
         <v>0.01</v>
@@ -9054,28 +9055,28 @@
         <v>3</v>
       </c>
       <c r="M110" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N110" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O110" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
+        <v>207</v>
+      </c>
+      <c r="B111" t="s">
         <v>208</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>209</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
         <v>210</v>
       </c>
-      <c r="D111" t="s">
-        <v>211</v>
-      </c>
       <c r="E111" t="s">
         <v>32</v>
       </c>
@@ -9086,7 +9087,7 @@
         <v>32</v>
       </c>
       <c r="H111" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I111" s="2">
         <v>0.5</v>
@@ -9101,17 +9102,24 @@
         <v>1</v>
       </c>
       <c r="M111" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N111" s="2" t="s">
         <v>18</v>
       </c>
       <c r="O111" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O111" xr:uid="{E0FD6E8C-F414-4D9F-82CB-33D09B6D4DCD}"/>
+  <autoFilter ref="A1:O111" xr:uid="{E0FD6E8C-F414-4D9F-82CB-33D09B6D4DCD}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Pool Quantity &amp; Quality"/>
+        <filter val="Pools- Deep Pools"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="O74" r:id="rId1" xr:uid="{3DD1971B-CBAE-41F4-A49E-E6B715DE820C}"/>

</xml_diff>

<commit_message>
Misc updates to code
</commit_message>
<xml_diff>
--- a/Data/Criteria_and_Scoring/Habitat_Limiting_Factor_Rating_Criteria.xlsx
+++ b/Data/Criteria_and_Scoring/Habitat_Limiting_Factor_Rating_Criteria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13924116-6A7A-47D1-9F98-FED74797B728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFC4B4D-094A-427E-A704-6837CC060870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1308" windowWidth="20340" windowHeight="10620" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="20208" windowHeight="10320" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -532,9 +532,6 @@
     <t>PROSPER</t>
   </si>
   <si>
-    <t>Off-Channel- Floodplain</t>
-  </si>
-  <si>
     <t>Channel_Confinementor_or_Entrenchment_Ratio_INDICATOR_9</t>
   </si>
   <si>
@@ -577,9 +574,6 @@
     <t>PROFESSIONAL JUDGEMENT</t>
   </si>
   <si>
-    <t>Contaminants_303d</t>
-  </si>
-  <si>
     <t>Category_Type</t>
   </si>
   <si>
@@ -649,9 +643,6 @@
     <t>ATLAS_FlowBin</t>
   </si>
   <si>
-    <t>ATLAS_Flow</t>
-  </si>
-  <si>
     <t>ATLAS flow class 3</t>
   </si>
   <si>
@@ -710,6 +701,15 @@
   </si>
   <si>
     <t>Pool_Habitat_Prcnt_INDICATOR_4,EDT_Scour Pool pct</t>
+  </si>
+  <si>
+    <t>ATLAS Flow</t>
+  </si>
+  <si>
+    <t>Contaminants_303d (not pH bacteria or DO listings)</t>
+  </si>
+  <si>
+    <t>Floodplain Connectivity</t>
   </si>
 </sst>
 </file>
@@ -3808,13 +3808,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FD6E8C-F414-4D9F-82CB-33D09B6D4DCD}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomLeft" activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3845,22 +3844,22 @@
         <v>126</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I1" s="38" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="38" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K1" s="38" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L1" s="39" t="s">
         <v>10</v>
@@ -3875,7 +3874,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -3883,11 +3882,11 @@
         <v>139</v>
       </c>
       <c r="C2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" t="s">
         <v>158</v>
       </c>
-      <c r="D2" t="s">
-        <v>159</v>
-      </c>
       <c r="E2" t="s">
         <v>32</v>
       </c>
@@ -3898,7 +3897,7 @@
         <v>32</v>
       </c>
       <c r="H2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I2" s="2">
         <v>0</v>
@@ -3923,7 +3922,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -3931,11 +3930,11 @@
         <v>139</v>
       </c>
       <c r="C3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" t="s">
         <v>158</v>
       </c>
-      <c r="D3" t="s">
-        <v>159</v>
-      </c>
       <c r="E3" t="s">
         <v>32</v>
       </c>
@@ -3946,7 +3945,7 @@
         <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I3" s="2">
         <v>1.4</v>
@@ -3971,7 +3970,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -3979,11 +3978,11 @@
         <v>139</v>
       </c>
       <c r="C4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" t="s">
         <v>158</v>
       </c>
-      <c r="D4" t="s">
-        <v>159</v>
-      </c>
       <c r="E4" t="s">
         <v>32</v>
       </c>
@@ -3994,7 +3993,7 @@
         <v>32</v>
       </c>
       <c r="H4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I4" s="2">
         <v>2.2000000000000002</v>
@@ -4019,7 +4018,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -4042,7 +4041,7 @@
         <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
@@ -4067,7 +4066,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -4090,7 +4089,7 @@
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I6" s="2">
         <v>0</v>
@@ -4114,7 +4113,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>95</v>
       </c>
@@ -4137,7 +4136,7 @@
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I7" s="2">
         <v>20</v>
@@ -4162,7 +4161,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -4185,7 +4184,7 @@
         <v>100000</v>
       </c>
       <c r="H8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I8" s="2">
         <v>0</v>
@@ -4210,7 +4209,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -4233,7 +4232,7 @@
         <v>100000</v>
       </c>
       <c r="H9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I9" s="2">
         <v>17</v>
@@ -4258,7 +4257,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -4281,7 +4280,7 @@
         <v>100000</v>
       </c>
       <c r="H10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I10" s="2">
         <v>70</v>
@@ -4306,7 +4305,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -4329,7 +4328,7 @@
         <v>32</v>
       </c>
       <c r="H11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -4354,7 +4353,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -4377,7 +4376,7 @@
         <v>32</v>
       </c>
       <c r="H12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I12" s="2">
         <v>2</v>
@@ -4402,7 +4401,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -4425,7 +4424,7 @@
         <v>32</v>
       </c>
       <c r="H13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I13" s="2">
         <v>5</v>
@@ -4458,11 +4457,11 @@
         <v>140</v>
       </c>
       <c r="C14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D14" t="s">
         <v>164</v>
       </c>
-      <c r="D14" t="s">
-        <v>165</v>
-      </c>
       <c r="E14" t="s">
         <v>32</v>
       </c>
@@ -4473,7 +4472,7 @@
         <v>32</v>
       </c>
       <c r="H14" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I14" s="2">
         <v>0</v>
@@ -4506,11 +4505,11 @@
         <v>140</v>
       </c>
       <c r="C15" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" t="s">
         <v>164</v>
       </c>
-      <c r="D15" t="s">
-        <v>165</v>
-      </c>
       <c r="E15" t="s">
         <v>32</v>
       </c>
@@ -4521,7 +4520,7 @@
         <v>32</v>
       </c>
       <c r="H15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I15" s="2">
         <v>0.1</v>
@@ -4553,11 +4552,11 @@
         <v>140</v>
       </c>
       <c r="C16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" t="s">
         <v>164</v>
       </c>
-      <c r="D16" t="s">
-        <v>165</v>
-      </c>
       <c r="E16" t="s">
         <v>32</v>
       </c>
@@ -4568,7 +4567,7 @@
         <v>32</v>
       </c>
       <c r="H16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I16" s="2">
         <v>20</v>
@@ -4601,10 +4600,10 @@
         <v>140</v>
       </c>
       <c r="C17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D17" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E17" t="s">
         <v>32</v>
@@ -4616,7 +4615,7 @@
         <v>32</v>
       </c>
       <c r="H17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I17" s="2">
         <v>0</v>
@@ -4632,7 +4631,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>18</v>
@@ -4649,10 +4648,10 @@
         <v>140</v>
       </c>
       <c r="C18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D18" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -4664,7 +4663,7 @@
         <v>32</v>
       </c>
       <c r="H18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I18" s="2">
         <v>0.1</v>
@@ -4697,10 +4696,10 @@
         <v>140</v>
       </c>
       <c r="C19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D19" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E19" t="s">
         <v>32</v>
@@ -4712,7 +4711,7 @@
         <v>32</v>
       </c>
       <c r="H19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I19" s="2">
         <v>5</v>
@@ -4737,7 +4736,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="36" t="s">
         <v>54</v>
       </c>
@@ -4752,7 +4751,7 @@
       <c r="F20" s="36"/>
       <c r="G20" s="36"/>
       <c r="H20" s="36" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I20" s="37">
         <v>0</v>
@@ -4778,7 +4777,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="36" t="s">
         <v>54</v>
       </c>
@@ -4793,7 +4792,7 @@
       <c r="F21" s="36"/>
       <c r="G21" s="36"/>
       <c r="H21" s="36" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I21" s="37">
         <v>5</v>
@@ -4819,7 +4818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="36" t="s">
         <v>54</v>
       </c>
@@ -4834,7 +4833,7 @@
       <c r="F22" s="36"/>
       <c r="G22" s="36"/>
       <c r="H22" s="36" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I22" s="37">
         <v>20</v>
@@ -4868,10 +4867,10 @@
         <v>140</v>
       </c>
       <c r="C23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D23" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E23" t="s">
         <v>32</v>
@@ -4883,7 +4882,7 @@
         <v>32</v>
       </c>
       <c r="H23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I23" s="2">
         <v>0</v>
@@ -4916,10 +4915,10 @@
         <v>140</v>
       </c>
       <c r="C24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D24" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E24" t="s">
         <v>32</v>
@@ -4931,7 +4930,7 @@
         <v>32</v>
       </c>
       <c r="H24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I24" s="2">
         <v>10</v>
@@ -4964,10 +4963,10 @@
         <v>140</v>
       </c>
       <c r="C25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D25" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E25" t="s">
         <v>32</v>
@@ -4979,7 +4978,7 @@
         <v>32</v>
       </c>
       <c r="H25" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I25" s="2">
         <v>20</v>
@@ -5012,10 +5011,10 @@
         <v>140</v>
       </c>
       <c r="C26" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" t="s">
         <v>162</v>
-      </c>
-      <c r="D26" t="s">
-        <v>163</v>
       </c>
       <c r="E26" t="s">
         <v>86</v>
@@ -5028,7 +5027,7 @@
         <v>1.524</v>
       </c>
       <c r="H26" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I26" s="2">
         <v>0</v>
@@ -5061,10 +5060,10 @@
         <v>140</v>
       </c>
       <c r="C27" t="s">
+        <v>161</v>
+      </c>
+      <c r="D27" t="s">
         <v>162</v>
-      </c>
-      <c r="D27" t="s">
-        <v>163</v>
       </c>
       <c r="E27" t="s">
         <v>86</v>
@@ -5077,7 +5076,7 @@
         <v>1.524</v>
       </c>
       <c r="H27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I27" s="2">
         <v>184</v>
@@ -5110,10 +5109,10 @@
         <v>140</v>
       </c>
       <c r="C28" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" t="s">
         <v>162</v>
-      </c>
-      <c r="D28" t="s">
-        <v>163</v>
       </c>
       <c r="E28" t="s">
         <v>86</v>
@@ -5126,7 +5125,7 @@
         <v>1.524</v>
       </c>
       <c r="H28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>32</v>
@@ -5159,10 +5158,10 @@
         <v>140</v>
       </c>
       <c r="C29" t="s">
+        <v>161</v>
+      </c>
+      <c r="D29" t="s">
         <v>162</v>
-      </c>
-      <c r="D29" t="s">
-        <v>163</v>
       </c>
       <c r="E29" t="s">
         <v>93</v>
@@ -5176,7 +5175,7 @@
         <v>3.048</v>
       </c>
       <c r="H29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I29" s="2">
         <v>0</v>
@@ -5209,10 +5208,10 @@
         <v>140</v>
       </c>
       <c r="C30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D30" t="s">
         <v>162</v>
-      </c>
-      <c r="D30" t="s">
-        <v>163</v>
       </c>
       <c r="E30" t="s">
         <v>93</v>
@@ -5226,7 +5225,7 @@
         <v>3.048</v>
       </c>
       <c r="H30" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I30" s="2">
         <v>95</v>
@@ -5259,10 +5258,10 @@
         <v>140</v>
       </c>
       <c r="C31" t="s">
+        <v>161</v>
+      </c>
+      <c r="D31" t="s">
         <v>162</v>
-      </c>
-      <c r="D31" t="s">
-        <v>163</v>
       </c>
       <c r="E31" t="s">
         <v>93</v>
@@ -5276,7 +5275,7 @@
         <v>3.048</v>
       </c>
       <c r="H31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>32</v>
@@ -5307,10 +5306,10 @@
         <v>140</v>
       </c>
       <c r="C32" t="s">
+        <v>161</v>
+      </c>
+      <c r="D32" t="s">
         <v>162</v>
-      </c>
-      <c r="D32" t="s">
-        <v>163</v>
       </c>
       <c r="E32" t="s">
         <v>98</v>
@@ -5324,7 +5323,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H32" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I32" s="2">
         <v>0</v>
@@ -5357,10 +5356,10 @@
         <v>140</v>
       </c>
       <c r="C33" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" t="s">
         <v>162</v>
-      </c>
-      <c r="D33" t="s">
-        <v>163</v>
       </c>
       <c r="E33" t="s">
         <v>98</v>
@@ -5374,7 +5373,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H33" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I33" s="2">
         <v>70</v>
@@ -5407,10 +5406,10 @@
         <v>140</v>
       </c>
       <c r="C34" t="s">
+        <v>161</v>
+      </c>
+      <c r="D34" t="s">
         <v>162</v>
-      </c>
-      <c r="D34" t="s">
-        <v>163</v>
       </c>
       <c r="E34" t="s">
         <v>98</v>
@@ -5424,7 +5423,7 @@
         <v>4.5720000000000001</v>
       </c>
       <c r="H34" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>32</v>
@@ -5457,10 +5456,10 @@
         <v>140</v>
       </c>
       <c r="C35" t="s">
+        <v>161</v>
+      </c>
+      <c r="D35" t="s">
         <v>162</v>
-      </c>
-      <c r="D35" t="s">
-        <v>163</v>
       </c>
       <c r="E35" t="s">
         <v>102</v>
@@ -5474,7 +5473,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H35" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I35" s="2">
         <v>0</v>
@@ -5507,10 +5506,10 @@
         <v>140</v>
       </c>
       <c r="C36" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" t="s">
         <v>162</v>
-      </c>
-      <c r="D36" t="s">
-        <v>163</v>
       </c>
       <c r="E36" t="s">
         <v>102</v>
@@ -5524,7 +5523,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H36" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I36" s="2">
         <v>55</v>
@@ -5557,10 +5556,10 @@
         <v>140</v>
       </c>
       <c r="C37" t="s">
+        <v>161</v>
+      </c>
+      <c r="D37" t="s">
         <v>162</v>
-      </c>
-      <c r="D37" t="s">
-        <v>163</v>
       </c>
       <c r="E37" t="s">
         <v>102</v>
@@ -5574,7 +5573,7 @@
         <v>6.0960000000000001</v>
       </c>
       <c r="H37" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>32</v>
@@ -5607,10 +5606,10 @@
         <v>140</v>
       </c>
       <c r="C38" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" t="s">
         <v>162</v>
-      </c>
-      <c r="D38" t="s">
-        <v>163</v>
       </c>
       <c r="E38" t="s">
         <v>107</v>
@@ -5624,7 +5623,7 @@
         <v>7.62</v>
       </c>
       <c r="H38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I38" s="2">
         <v>0</v>
@@ -5657,10 +5656,10 @@
         <v>140</v>
       </c>
       <c r="C39" t="s">
+        <v>161</v>
+      </c>
+      <c r="D39" t="s">
         <v>162</v>
-      </c>
-      <c r="D39" t="s">
-        <v>163</v>
       </c>
       <c r="E39" t="s">
         <v>107</v>
@@ -5674,7 +5673,7 @@
         <v>7.62</v>
       </c>
       <c r="H39" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I39" s="2">
         <v>47</v>
@@ -5707,10 +5706,10 @@
         <v>140</v>
       </c>
       <c r="C40" t="s">
+        <v>161</v>
+      </c>
+      <c r="D40" t="s">
         <v>162</v>
-      </c>
-      <c r="D40" t="s">
-        <v>163</v>
       </c>
       <c r="E40" t="s">
         <v>107</v>
@@ -5724,7 +5723,7 @@
         <v>7.62</v>
       </c>
       <c r="H40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>32</v>
@@ -5757,10 +5756,10 @@
         <v>140</v>
       </c>
       <c r="C41" t="s">
+        <v>161</v>
+      </c>
+      <c r="D41" t="s">
         <v>162</v>
-      </c>
-      <c r="D41" t="s">
-        <v>163</v>
       </c>
       <c r="E41" t="s">
         <v>113</v>
@@ -5774,7 +5773,7 @@
         <v>15.24</v>
       </c>
       <c r="H41" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I41" s="2">
         <v>0</v>
@@ -5807,10 +5806,10 @@
         <v>140</v>
       </c>
       <c r="C42" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42" t="s">
         <v>162</v>
-      </c>
-      <c r="D42" t="s">
-        <v>163</v>
       </c>
       <c r="E42" t="s">
         <v>113</v>
@@ -5824,7 +5823,7 @@
         <v>15.24</v>
       </c>
       <c r="H42" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I42" s="2">
         <v>25</v>
@@ -5857,10 +5856,10 @@
         <v>140</v>
       </c>
       <c r="C43" t="s">
+        <v>161</v>
+      </c>
+      <c r="D43" t="s">
         <v>162</v>
-      </c>
-      <c r="D43" t="s">
-        <v>163</v>
       </c>
       <c r="E43" t="s">
         <v>113</v>
@@ -5874,7 +5873,7 @@
         <v>15.24</v>
       </c>
       <c r="H43" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>32</v>
@@ -5907,10 +5906,10 @@
         <v>140</v>
       </c>
       <c r="C44" t="s">
+        <v>161</v>
+      </c>
+      <c r="D44" t="s">
         <v>162</v>
-      </c>
-      <c r="D44" t="s">
-        <v>163</v>
       </c>
       <c r="E44" t="s">
         <v>116</v>
@@ -5924,7 +5923,7 @@
         <v>22.86</v>
       </c>
       <c r="H44" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I44" s="2">
         <v>0</v>
@@ -5957,10 +5956,10 @@
         <v>140</v>
       </c>
       <c r="C45" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" t="s">
         <v>162</v>
-      </c>
-      <c r="D45" t="s">
-        <v>163</v>
       </c>
       <c r="E45" t="s">
         <v>116</v>
@@ -5974,7 +5973,7 @@
         <v>22.86</v>
       </c>
       <c r="H45" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I45" s="2">
         <v>23</v>
@@ -6007,10 +6006,10 @@
         <v>140</v>
       </c>
       <c r="C46" t="s">
+        <v>161</v>
+      </c>
+      <c r="D46" t="s">
         <v>162</v>
-      </c>
-      <c r="D46" t="s">
-        <v>163</v>
       </c>
       <c r="E46" t="s">
         <v>116</v>
@@ -6024,7 +6023,7 @@
         <v>22.86</v>
       </c>
       <c r="H46" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>32</v>
@@ -6057,10 +6056,10 @@
         <v>140</v>
       </c>
       <c r="C47" t="s">
+        <v>161</v>
+      </c>
+      <c r="D47" t="s">
         <v>162</v>
-      </c>
-      <c r="D47" t="s">
-        <v>163</v>
       </c>
       <c r="E47" t="s">
         <v>119</v>
@@ -6073,7 +6072,7 @@
         <v>100000</v>
       </c>
       <c r="H47" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I47" s="2">
         <v>0</v>
@@ -6106,10 +6105,10 @@
         <v>140</v>
       </c>
       <c r="C48" t="s">
+        <v>161</v>
+      </c>
+      <c r="D48" t="s">
         <v>162</v>
-      </c>
-      <c r="D48" t="s">
-        <v>163</v>
       </c>
       <c r="E48" t="s">
         <v>119</v>
@@ -6122,7 +6121,7 @@
         <v>100000</v>
       </c>
       <c r="H48" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I48" s="2">
         <v>18</v>
@@ -6155,10 +6154,10 @@
         <v>140</v>
       </c>
       <c r="C49" t="s">
+        <v>161</v>
+      </c>
+      <c r="D49" t="s">
         <v>162</v>
-      </c>
-      <c r="D49" t="s">
-        <v>163</v>
       </c>
       <c r="E49" t="s">
         <v>119</v>
@@ -6171,7 +6170,7 @@
         <v>100000</v>
       </c>
       <c r="H49" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>32</v>
@@ -6196,24 +6195,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="40" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B50" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D50" s="40" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E50" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H50" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I50" s="41">
         <v>0</v>
@@ -6239,24 +6238,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="40" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B51" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D51" s="40" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E51" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H51" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I51" s="41">
         <v>50</v>
@@ -6281,24 +6280,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="40" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B52" s="40" t="s">
         <v>135</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D52" s="40" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E52" s="40" t="s">
         <v>32</v>
       </c>
       <c r="H52" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I52" s="41">
         <v>80</v>
@@ -6323,7 +6322,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -6331,11 +6330,11 @@
         <v>138</v>
       </c>
       <c r="C53" t="s">
+        <v>159</v>
+      </c>
+      <c r="D53" t="s">
         <v>160</v>
       </c>
-      <c r="D53" t="s">
-        <v>161</v>
-      </c>
       <c r="E53" t="s">
         <v>32</v>
       </c>
@@ -6346,7 +6345,7 @@
         <v>32</v>
       </c>
       <c r="H53" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I53" s="2">
         <v>0</v>
@@ -6371,7 +6370,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -6379,11 +6378,11 @@
         <v>138</v>
       </c>
       <c r="C54" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" t="s">
         <v>160</v>
       </c>
-      <c r="D54" t="s">
-        <v>161</v>
-      </c>
       <c r="E54" t="s">
         <v>32</v>
       </c>
@@ -6394,7 +6393,7 @@
         <v>32</v>
       </c>
       <c r="H54" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I54" s="2">
         <v>2</v>
@@ -6419,7 +6418,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -6427,11 +6426,11 @@
         <v>138</v>
       </c>
       <c r="C55" t="s">
+        <v>159</v>
+      </c>
+      <c r="D55" t="s">
         <v>160</v>
       </c>
-      <c r="D55" t="s">
-        <v>161</v>
-      </c>
       <c r="E55" t="s">
         <v>32</v>
       </c>
@@ -6442,7 +6441,7 @@
         <v>32</v>
       </c>
       <c r="H55" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I55" s="2">
         <v>5</v>
@@ -6467,7 +6466,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -6490,7 +6489,7 @@
         <v>32</v>
       </c>
       <c r="H56" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I56" s="2">
         <v>-5</v>
@@ -6514,7 +6513,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -6537,7 +6536,7 @@
         <v>32</v>
       </c>
       <c r="H57" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I57" s="2">
         <v>1</v>
@@ -6561,7 +6560,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -6584,7 +6583,7 @@
         <v>32</v>
       </c>
       <c r="H58" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I58" s="2">
         <v>4</v>
@@ -6608,7 +6607,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -6631,7 +6630,7 @@
         <v>32</v>
       </c>
       <c r="H59" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I59" s="2">
         <v>0</v>
@@ -6646,7 +6645,7 @@
         <v>1</v>
       </c>
       <c r="M59" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>18</v>
@@ -6655,7 +6654,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -6678,7 +6677,7 @@
         <v>32</v>
       </c>
       <c r="H60" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I60" s="2">
         <v>2</v>
@@ -6703,7 +6702,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -6726,7 +6725,7 @@
         <v>32</v>
       </c>
       <c r="H61" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I61" s="2">
         <v>5</v>
@@ -6751,7 +6750,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>37</v>
       </c>
@@ -6762,7 +6761,7 @@
         <v>148</v>
       </c>
       <c r="D62" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E62" t="s">
         <v>32</v>
@@ -6774,7 +6773,7 @@
         <v>32</v>
       </c>
       <c r="H62" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I62" s="2">
         <v>0</v>
@@ -6798,7 +6797,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>37</v>
       </c>
@@ -6809,7 +6808,7 @@
         <v>148</v>
       </c>
       <c r="D63" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E63" t="s">
         <v>32</v>
@@ -6821,7 +6820,7 @@
         <v>32</v>
       </c>
       <c r="H63" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I63" s="2">
         <v>1</v>
@@ -6845,7 +6844,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -6856,7 +6855,7 @@
         <v>148</v>
       </c>
       <c r="D64" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E64" t="s">
         <v>32</v>
@@ -6868,7 +6867,7 @@
         <v>32</v>
       </c>
       <c r="H64" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I64" s="2">
         <v>50</v>
@@ -6893,7 +6892,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>58</v>
       </c>
@@ -6916,7 +6915,7 @@
         <v>32</v>
       </c>
       <c r="H65" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I65" s="2">
         <v>0</v>
@@ -6940,7 +6939,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>58</v>
       </c>
@@ -6963,7 +6962,7 @@
         <v>32</v>
       </c>
       <c r="H66" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I66" s="2">
         <v>12</v>
@@ -6988,7 +6987,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>58</v>
       </c>
@@ -7011,7 +7010,7 @@
         <v>32</v>
       </c>
       <c r="H67" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I67" s="2">
         <v>20</v>
@@ -7036,7 +7035,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="40" t="s">
         <v>73</v>
       </c>
@@ -7059,7 +7058,7 @@
         <v>32</v>
       </c>
       <c r="H68" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I68" s="41">
         <v>0</v>
@@ -7083,7 +7082,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="40" t="s">
         <v>73</v>
       </c>
@@ -7106,7 +7105,7 @@
         <v>32</v>
       </c>
       <c r="H69" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I69" s="41">
         <v>10</v>
@@ -7131,7 +7130,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="40" t="s">
         <v>73</v>
       </c>
@@ -7154,7 +7153,7 @@
         <v>32</v>
       </c>
       <c r="H70" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I70" s="41">
         <v>20</v>
@@ -7179,7 +7178,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="40" t="s">
         <v>85</v>
       </c>
@@ -7190,7 +7189,7 @@
         <v>148</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E71" s="40" t="s">
         <v>32</v>
@@ -7202,7 +7201,7 @@
         <v>32</v>
       </c>
       <c r="H71" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I71" s="41">
         <v>0</v>
@@ -7226,7 +7225,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="40" t="s">
         <v>85</v>
       </c>
@@ -7237,7 +7236,7 @@
         <v>148</v>
       </c>
       <c r="D72" s="40" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E72" s="40" t="s">
         <v>32</v>
@@ -7249,7 +7248,7 @@
         <v>32</v>
       </c>
       <c r="H72" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I72" s="41">
         <v>15</v>
@@ -7274,7 +7273,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="40" t="s">
         <v>85</v>
       </c>
@@ -7285,7 +7284,7 @@
         <v>148</v>
       </c>
       <c r="D73" s="40" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E73" s="40" t="s">
         <v>32</v>
@@ -7297,7 +7296,7 @@
         <v>32</v>
       </c>
       <c r="H73" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I73" s="41">
         <v>30</v>
@@ -7322,7 +7321,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="40" t="s">
         <v>14</v>
       </c>
@@ -7330,11 +7329,11 @@
         <v>141</v>
       </c>
       <c r="C74" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="D74" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="D74" s="40" t="s">
-        <v>167</v>
-      </c>
       <c r="E74" s="40" t="s">
         <v>32</v>
       </c>
@@ -7345,7 +7344,7 @@
         <v>32</v>
       </c>
       <c r="H74" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I74" s="41">
         <v>0</v>
@@ -7371,7 +7370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="40" t="s">
         <v>14</v>
       </c>
@@ -7379,11 +7378,11 @@
         <v>141</v>
       </c>
       <c r="C75" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="D75" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="D75" s="40" t="s">
-        <v>167</v>
-      </c>
       <c r="E75" s="40" t="s">
         <v>32</v>
       </c>
@@ -7394,7 +7393,7 @@
         <v>32</v>
       </c>
       <c r="H75" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I75" s="41">
         <v>12</v>
@@ -7420,7 +7419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="40" t="s">
         <v>14</v>
       </c>
@@ -7428,11 +7427,11 @@
         <v>141</v>
       </c>
       <c r="C76" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="D76" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="D76" s="40" t="s">
-        <v>167</v>
-      </c>
       <c r="E76" s="40" t="s">
         <v>32</v>
       </c>
@@ -7443,7 +7442,7 @@
         <v>32</v>
       </c>
       <c r="H76" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I76" s="41">
         <v>14</v>
@@ -7469,7 +7468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="40" t="s">
         <v>35</v>
       </c>
@@ -7477,10 +7476,10 @@
         <v>141</v>
       </c>
       <c r="C77" s="40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D77" s="40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E77" s="40" t="s">
         <v>32</v>
@@ -7492,7 +7491,7 @@
         <v>32</v>
       </c>
       <c r="H77" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I77" s="41">
         <v>0</v>
@@ -7517,7 +7516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="40" t="s">
         <v>35</v>
       </c>
@@ -7525,10 +7524,10 @@
         <v>141</v>
       </c>
       <c r="C78" s="40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D78" s="40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E78" s="40" t="s">
         <v>32</v>
@@ -7540,7 +7539,7 @@
         <v>32</v>
       </c>
       <c r="H78" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I78" s="41">
         <v>10</v>
@@ -7565,7 +7564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="40" t="s">
         <v>35</v>
       </c>
@@ -7573,10 +7572,10 @@
         <v>141</v>
       </c>
       <c r="C79" s="40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D79" s="40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E79" s="40" t="s">
         <v>32</v>
@@ -7588,7 +7587,7 @@
         <v>32</v>
       </c>
       <c r="H79" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I79" s="41">
         <v>14</v>
@@ -7613,7 +7612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="40" t="s">
         <v>55</v>
       </c>
@@ -7621,10 +7620,10 @@
         <v>141</v>
       </c>
       <c r="C80" s="40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D80" s="40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E80" s="40" t="s">
         <v>32</v>
@@ -7636,7 +7635,7 @@
         <v>32</v>
       </c>
       <c r="H80" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I80" s="41">
         <v>0</v>
@@ -7652,7 +7651,7 @@
         <v>5</v>
       </c>
       <c r="M80" s="41" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="N80" s="41" t="s">
         <v>20</v>
@@ -7661,7 +7660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="40" t="s">
         <v>55</v>
       </c>
@@ -7669,10 +7668,10 @@
         <v>141</v>
       </c>
       <c r="C81" s="40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D81" s="40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E81" s="40" t="s">
         <v>32</v>
@@ -7684,7 +7683,7 @@
         <v>32</v>
       </c>
       <c r="H81" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I81" s="41">
         <v>16</v>
@@ -7700,7 +7699,7 @@
         <v>3</v>
       </c>
       <c r="M81" s="41" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="N81" s="41" t="s">
         <v>22</v>
@@ -7709,7 +7708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" s="40" t="s">
         <v>55</v>
       </c>
@@ -7717,10 +7716,10 @@
         <v>141</v>
       </c>
       <c r="C82" s="40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D82" s="40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E82" s="40" t="s">
         <v>32</v>
@@ -7732,7 +7731,7 @@
         <v>32</v>
       </c>
       <c r="H82" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I82" s="41">
         <v>22</v>
@@ -7748,7 +7747,7 @@
         <v>1</v>
       </c>
       <c r="M82" s="41" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N82" s="41" t="s">
         <v>18</v>
@@ -7757,9 +7756,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="40" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B83" s="40" t="s">
         <v>124</v>
@@ -7768,7 +7767,7 @@
         <v>148</v>
       </c>
       <c r="D83" s="40" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E83" s="40" t="s">
         <v>32</v>
@@ -7780,7 +7779,7 @@
         <v>32</v>
       </c>
       <c r="H83" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I83" s="41">
         <v>99</v>
@@ -7795,18 +7794,18 @@
         <v>1</v>
       </c>
       <c r="M83" s="41" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N83" s="41" t="s">
         <v>18</v>
       </c>
       <c r="O83" s="40" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="40" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B84" s="40" t="s">
         <v>124</v>
@@ -7815,7 +7814,7 @@
         <v>148</v>
       </c>
       <c r="D84" s="40" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E84" s="40" t="s">
         <v>32</v>
@@ -7827,7 +7826,7 @@
         <v>32</v>
       </c>
       <c r="H84" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I84" s="41">
         <v>50</v>
@@ -7842,18 +7841,18 @@
         <v>3</v>
       </c>
       <c r="M84" s="41" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N84" s="41" t="s">
         <v>22</v>
       </c>
       <c r="O84" s="40" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="40" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B85" s="40" t="s">
         <v>124</v>
@@ -7862,7 +7861,7 @@
         <v>148</v>
       </c>
       <c r="D85" s="40" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E85" s="40" t="s">
         <v>32</v>
@@ -7874,7 +7873,7 @@
         <v>32</v>
       </c>
       <c r="H85" s="40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I85" s="41">
         <v>0</v>
@@ -7889,16 +7888,16 @@
         <v>5</v>
       </c>
       <c r="M85" s="41" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="N85" s="41" t="s">
         <v>20</v>
       </c>
       <c r="O85" s="40" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="40" t="s">
         <v>15</v>
       </c>
@@ -7906,19 +7905,19 @@
         <v>142</v>
       </c>
       <c r="D86" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="E86" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F86" t="s">
+        <v>32</v>
+      </c>
+      <c r="G86" t="s">
+        <v>32</v>
+      </c>
+      <c r="H86" t="s">
         <v>173</v>
-      </c>
-      <c r="E86" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F86" t="s">
-        <v>32</v>
-      </c>
-      <c r="G86" t="s">
-        <v>32</v>
-      </c>
-      <c r="H86" t="s">
-        <v>175</v>
       </c>
       <c r="I86" s="41" t="s">
         <v>24</v>
@@ -7933,7 +7932,7 @@
         <v>1</v>
       </c>
       <c r="M86" s="41" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="N86" s="41" t="s">
         <v>32</v>
@@ -7942,7 +7941,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="87" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="40" t="s">
         <v>15</v>
       </c>
@@ -7950,19 +7949,19 @@
         <v>142</v>
       </c>
       <c r="D87" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="E87" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F87" t="s">
+        <v>32</v>
+      </c>
+      <c r="G87" t="s">
+        <v>32</v>
+      </c>
+      <c r="H87" t="s">
         <v>173</v>
-      </c>
-      <c r="E87" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F87" t="s">
-        <v>32</v>
-      </c>
-      <c r="G87" t="s">
-        <v>32</v>
-      </c>
-      <c r="H87" t="s">
-        <v>175</v>
       </c>
       <c r="I87" s="41" t="s">
         <v>28</v>
@@ -7977,7 +7976,7 @@
         <v>3</v>
       </c>
       <c r="M87" s="41" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="N87" s="41" t="s">
         <v>32</v>
@@ -7986,7 +7985,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="88" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="40" t="s">
         <v>15</v>
       </c>
@@ -7994,19 +7993,19 @@
         <v>142</v>
       </c>
       <c r="D88" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="E88" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F88" t="s">
+        <v>32</v>
+      </c>
+      <c r="G88" t="s">
+        <v>32</v>
+      </c>
+      <c r="H88" t="s">
         <v>173</v>
-      </c>
-      <c r="E88" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="F88" t="s">
-        <v>32</v>
-      </c>
-      <c r="G88" t="s">
-        <v>32</v>
-      </c>
-      <c r="H88" t="s">
-        <v>175</v>
       </c>
       <c r="I88" s="41" t="s">
         <v>31</v>
@@ -8030,7 +8029,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="89" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -8038,10 +8037,10 @@
         <v>142</v>
       </c>
       <c r="C89" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D89" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E89" t="s">
         <v>32</v>
@@ -8053,7 +8052,7 @@
         <v>32</v>
       </c>
       <c r="H89" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I89" s="3" t="s">
         <v>32</v>
@@ -8077,7 +8076,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>36</v>
       </c>
@@ -8085,10 +8084,10 @@
         <v>142</v>
       </c>
       <c r="C90" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D90" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E90" t="s">
         <v>32</v>
@@ -8100,7 +8099,7 @@
         <v>32</v>
       </c>
       <c r="H90" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I90" s="3">
         <v>1</v>
@@ -8124,7 +8123,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>36</v>
       </c>
@@ -8132,10 +8131,10 @@
         <v>142</v>
       </c>
       <c r="C91" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D91" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E91" t="s">
         <v>32</v>
@@ -8147,7 +8146,7 @@
         <v>32</v>
       </c>
       <c r="H91" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I91" s="3">
         <v>2</v>
@@ -8171,7 +8170,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="92" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>36</v>
       </c>
@@ -8179,10 +8178,10 @@
         <v>142</v>
       </c>
       <c r="C92" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D92" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E92" t="s">
         <v>32</v>
@@ -8194,7 +8193,7 @@
         <v>32</v>
       </c>
       <c r="H92" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I92" s="3" t="s">
         <v>51</v>
@@ -8218,7 +8217,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="93" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>36</v>
       </c>
@@ -8226,10 +8225,10 @@
         <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D93" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E93" t="s">
         <v>32</v>
@@ -8241,7 +8240,7 @@
         <v>32</v>
       </c>
       <c r="H93" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I93" s="3" t="s">
         <v>56</v>
@@ -8265,7 +8264,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>36</v>
       </c>
@@ -8273,10 +8272,10 @@
         <v>142</v>
       </c>
       <c r="C94" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D94" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E94" t="s">
         <v>32</v>
@@ -8288,7 +8287,7 @@
         <v>32</v>
       </c>
       <c r="H94" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I94" s="3" t="s">
         <v>59</v>
@@ -8312,7 +8311,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>36</v>
       </c>
@@ -8320,10 +8319,10 @@
         <v>142</v>
       </c>
       <c r="C95" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D95" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E95" t="s">
         <v>32</v>
@@ -8335,7 +8334,7 @@
         <v>32</v>
       </c>
       <c r="H95" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I95" s="3">
         <v>5</v>
@@ -8359,7 +8358,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="96" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>7</v>
       </c>
@@ -8370,7 +8369,7 @@
         <v>144</v>
       </c>
       <c r="D96" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E96" t="s">
         <v>32</v>
@@ -8382,7 +8381,7 @@
         <v>32</v>
       </c>
       <c r="H96" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>20</v>
@@ -8406,7 +8405,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="97" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>7</v>
       </c>
@@ -8417,7 +8416,7 @@
         <v>144</v>
       </c>
       <c r="D97" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E97" t="s">
         <v>32</v>
@@ -8429,7 +8428,7 @@
         <v>32</v>
       </c>
       <c r="H97" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>22</v>
@@ -8453,7 +8452,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="98" spans="1:15" s="40" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>7</v>
       </c>
@@ -8464,7 +8463,7 @@
         <v>144</v>
       </c>
       <c r="D98" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E98" t="s">
         <v>32</v>
@@ -8476,7 +8475,7 @@
         <v>32</v>
       </c>
       <c r="H98" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>18</v>
@@ -8500,7 +8499,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>7</v>
       </c>
@@ -8511,7 +8510,7 @@
         <v>144</v>
       </c>
       <c r="D99" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E99" t="s">
         <v>32</v>
@@ -8523,7 +8522,7 @@
         <v>32</v>
       </c>
       <c r="H99" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>32</v>
@@ -8547,18 +8546,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B100" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C100" t="s">
         <v>144</v>
       </c>
       <c r="D100" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E100" t="s">
         <v>32</v>
@@ -8570,7 +8569,7 @@
         <v>32</v>
       </c>
       <c r="H100" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I100" s="3" t="s">
         <v>32</v>
@@ -8594,7 +8593,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>7</v>
       </c>
@@ -8605,7 +8604,7 @@
         <v>144</v>
       </c>
       <c r="D101" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E101" t="s">
         <v>32</v>
@@ -8617,7 +8616,7 @@
         <v>32</v>
       </c>
       <c r="H101" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I101">
         <v>1</v>
@@ -8638,10 +8637,10 @@
         <v>32</v>
       </c>
       <c r="O101" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>7</v>
       </c>
@@ -8652,7 +8651,7 @@
         <v>144</v>
       </c>
       <c r="D102" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E102" t="s">
         <v>32</v>
@@ -8664,7 +8663,7 @@
         <v>32</v>
       </c>
       <c r="H102" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I102">
         <v>3</v>
@@ -8685,10 +8684,10 @@
         <v>32</v>
       </c>
       <c r="O102" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>7</v>
       </c>
@@ -8699,7 +8698,7 @@
         <v>144</v>
       </c>
       <c r="D103" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E103" t="s">
         <v>32</v>
@@ -8711,7 +8710,7 @@
         <v>32</v>
       </c>
       <c r="H103" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I103">
         <v>5</v>
@@ -8732,10 +8731,10 @@
         <v>32</v>
       </c>
       <c r="O103" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>7</v>
       </c>
@@ -8746,45 +8745,45 @@
         <v>144</v>
       </c>
       <c r="D104" t="s">
+        <v>192</v>
+      </c>
+      <c r="E104" t="s">
+        <v>32</v>
+      </c>
+      <c r="F104" t="s">
+        <v>32</v>
+      </c>
+      <c r="G104" t="s">
+        <v>32</v>
+      </c>
+      <c r="H104" t="s">
+        <v>173</v>
+      </c>
+      <c r="I104" t="s">
+        <v>32</v>
+      </c>
+      <c r="J104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L104" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="M104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N104" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O104" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>194</v>
-      </c>
-      <c r="E104" t="s">
-        <v>32</v>
-      </c>
-      <c r="F104" t="s">
-        <v>32</v>
-      </c>
-      <c r="G104" t="s">
-        <v>32</v>
-      </c>
-      <c r="H104" t="s">
-        <v>175</v>
-      </c>
-      <c r="I104" t="s">
-        <v>32</v>
-      </c>
-      <c r="J104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L104" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="M104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="N104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O104" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>196</v>
       </c>
       <c r="B105" t="s">
         <v>136</v>
@@ -8793,7 +8792,7 @@
         <v>144</v>
       </c>
       <c r="D105" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="E105" t="s">
         <v>32</v>
@@ -8805,7 +8804,7 @@
         <v>32</v>
       </c>
       <c r="H105" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I105" s="2">
         <v>3</v>
@@ -8820,7 +8819,7 @@
         <v>5</v>
       </c>
       <c r="M105" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="N105" s="2" t="s">
         <v>20</v>
@@ -8829,9 +8828,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B106" t="s">
         <v>136</v>
@@ -8840,7 +8839,7 @@
         <v>144</v>
       </c>
       <c r="D106" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="E106" t="s">
         <v>32</v>
@@ -8852,7 +8851,7 @@
         <v>32</v>
       </c>
       <c r="H106" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I106" s="2">
         <v>2</v>
@@ -8867,7 +8866,7 @@
         <v>3</v>
       </c>
       <c r="M106" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="N106" s="2" t="s">
         <v>22</v>
@@ -8876,9 +8875,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B107" t="s">
         <v>136</v>
@@ -8887,7 +8886,7 @@
         <v>144</v>
       </c>
       <c r="D107" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="E107" t="s">
         <v>32</v>
@@ -8899,7 +8898,7 @@
         <v>32</v>
       </c>
       <c r="H107" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I107" s="2">
         <v>1</v>
@@ -8914,7 +8913,7 @@
         <v>1</v>
       </c>
       <c r="M107" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="N107" s="2" t="s">
         <v>18</v>
@@ -8923,9 +8922,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B108" t="s">
         <v>136</v>
@@ -8934,7 +8933,7 @@
         <v>144</v>
       </c>
       <c r="D108" t="s">
-        <v>197</v>
+        <v>215</v>
       </c>
       <c r="E108" t="s">
         <v>32</v>
@@ -8946,7 +8945,7 @@
         <v>32</v>
       </c>
       <c r="H108" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I108" s="2">
         <v>0</v>
@@ -8961,7 +8960,7 @@
         <v>32</v>
       </c>
       <c r="M108" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="N108" s="2" t="s">
         <v>32</v>
@@ -8970,19 +8969,19 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
+        <v>204</v>
+      </c>
+      <c r="B109" t="s">
+        <v>205</v>
+      </c>
+      <c r="C109" t="s">
+        <v>206</v>
+      </c>
+      <c r="D109" t="s">
         <v>207</v>
       </c>
-      <c r="B109" t="s">
-        <v>208</v>
-      </c>
-      <c r="C109" t="s">
-        <v>209</v>
-      </c>
-      <c r="D109" t="s">
-        <v>210</v>
-      </c>
       <c r="E109" t="s">
         <v>32</v>
       </c>
@@ -8993,7 +8992,7 @@
         <v>32</v>
       </c>
       <c r="H109" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I109" s="2">
         <v>0</v>
@@ -9008,28 +9007,28 @@
         <v>5</v>
       </c>
       <c r="M109" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="N109" s="2" t="s">
         <v>20</v>
       </c>
       <c r="O109" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>204</v>
+      </c>
+      <c r="B110" t="s">
+        <v>205</v>
+      </c>
+      <c r="C110" t="s">
+        <v>206</v>
+      </c>
+      <c r="D110" t="s">
         <v>207</v>
       </c>
-      <c r="B110" t="s">
-        <v>208</v>
-      </c>
-      <c r="C110" t="s">
-        <v>209</v>
-      </c>
-      <c r="D110" t="s">
-        <v>210</v>
-      </c>
       <c r="E110" t="s">
         <v>32</v>
       </c>
@@ -9040,7 +9039,7 @@
         <v>32</v>
       </c>
       <c r="H110" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I110" s="2">
         <v>0.01</v>
@@ -9055,28 +9054,28 @@
         <v>3</v>
       </c>
       <c r="M110" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="N110" s="2" t="s">
         <v>22</v>
       </c>
       <c r="O110" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
+        <v>204</v>
+      </c>
+      <c r="B111" t="s">
+        <v>205</v>
+      </c>
+      <c r="C111" t="s">
+        <v>206</v>
+      </c>
+      <c r="D111" t="s">
         <v>207</v>
       </c>
-      <c r="B111" t="s">
-        <v>208</v>
-      </c>
-      <c r="C111" t="s">
-        <v>209</v>
-      </c>
-      <c r="D111" t="s">
-        <v>210</v>
-      </c>
       <c r="E111" t="s">
         <v>32</v>
       </c>
@@ -9087,7 +9086,7 @@
         <v>32</v>
       </c>
       <c r="H111" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I111" s="2">
         <v>0.5</v>
@@ -9102,24 +9101,17 @@
         <v>1</v>
       </c>
       <c r="M111" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N111" s="2" t="s">
         <v>18</v>
       </c>
       <c r="O111" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O111" xr:uid="{E0FD6E8C-F414-4D9F-82CB-33D09B6D4DCD}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Pool Quantity &amp; Quality"/>
-        <filter val="Pools- Deep Pools"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:O111" xr:uid="{E0FD6E8C-F414-4D9F-82CB-33D09B6D4DCD}"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="O74" r:id="rId1" xr:uid="{3DD1971B-CBAE-41F4-A49E-E6B715DE820C}"/>

</xml_diff>